<commit_message>
09/08/2020 CHANGE UPDATES TO DATES
</commit_message>
<xml_diff>
--- a/modified_books.xlsx
+++ b/modified_books.xlsx
@@ -352,274 +352,274 @@
     <t>3357084330</t>
   </si>
   <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '32595035')])), ('isbn', '1474600042'), ('isbn13', '9781474600040'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '17')])), ('uri', 'kca://book/amzn1.gr.book.v1.pT8U80AoRYVn5k5h20vuOQ'), ('title', 'We Only Saw Happiness'), ('title_without_series', 'We Only Saw Happiness'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1476266549l/32595035._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1476266549l/32595035._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/32595035-we-only-saw-happiness'), ('num_pages', '320'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Weidenfeld &amp; Nicholson'), ('publication_day', '29'), ('publication_year', '2016'), ('publication_month', '12'), ('average_rating', '3.64'), ('ratings_count', '779'), ('description', "'We looked like the perfect young family, something out of a magazine, in shades of marshmallow pink...'&lt;br /&gt; A photograph. The father smiling beside his new car, the mother pregnant and radiant, the little girl placing cuddly toys in the cot for her new baby brother. All we see is the happiness.&lt;br /&gt; 'We don't see my mother. We don't see the lies.'&lt;br /&gt; But behind every picture there is a story. And behind that story, there are others.&lt;br /&gt; Every family has its secrets.&lt;br /&gt; When Antoine was young, he believed in love at first sight. He finds the woman of his dreams, Nathalie, and has two children. But when Antoine's life implodes, he does something unspeakable.&lt;br /&gt; Antoine's journey to come to terms with what he has done will take him across seas and continents, deep into his own heart and the hearts of others.&lt;br /&gt; Because in order to find true happiness, you have to know where to look..."), ('authors', OrderedDict([('author', OrderedDict([('id', '5416412'), ('name', 'Grégoire Delacourt'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1374772295p5/5416412.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1374772295p2/5416412.jpg')])), ('link', 'https://www.goodreads.com/author/show/5416412.Gr_goire_Delacourt'), ('average_rating', '3.55'), ('ratings_count', '13927'), ('text_reviews_count', '2134')]))])), ('published', '2016'), ('work', OrderedDict([('id', '42573935'), ('uri', 'kca://work/amzn1.gr.work.v1.IsjqYt9xlzObwwGlZBGiIw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17250')])), ('isbn', '0142437336'), ('isbn13', '9780142437339'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '6228')])), ('uri', 'kca://book/amzn1.gr.book.v1.4QGkL9_VomC7Ay9rPVfpFw'), ('title', 'The Crucible'), ('title_without_series', 'The Crucible'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1547467608l/17250._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1547467608l/17250._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17250.The_Crucible'), ('num_pages', '143'), ('format', 'Paperback'), ('edition_information', 'Penguin Classics (US/CAN)'), ('publisher', 'Penguin Books'), ('publication_day', '25'), ('publication_year', '2003'), ('publication_month', '3'), ('average_rating', '3.58'), ('ratings_count', '317018'), ('description', '"I believe that the reader will discover here the essential nature of one of the strangest and most awful chapters in human history," Arthur Miller wrote of his classic play about the witch-hunts and trials in seventeenth-century Salem, Massachusetts. Based on historical people and real events, Miller\'s drama is a searing portrait of a community engulfed by hysteria. In the rigid theocracy of Salem, rumors that women are practicing witchcraft galvanize the town\'s most basic fears and suspicions; and when a young girl accuses Elizabeth Proctor of being a witch, self-righteous church leaders and townspeople insist that Elizabeth be brought to trial. The ruthlessness of the prosecutors and the eagerness of neighbor to testify against neighbor brilliantly illuminates the destructive power of socially sanctioned violence.&lt;br /&gt;&lt;br /&gt;Written in 1953, &lt;i&gt;The Crucible&lt;/i&gt; is a mirror Miller uses to reflect the anti-communist hysteria inspired by Senator Joseph McCarthy\'s "witch-hunts" in the United States. Within the text itself, Miller contemplates the parallels, writing, "Political opposition... is given an inhumane overlay, which then justifies the abrogation of all normally applied customs of civilized behavior. A political policy is equated with moral right, and opposition to it with diabolical malevolence."&lt;br /&gt;&lt;br /&gt;WIth an introduction by Christopher Bigsby.&lt;br /&gt;(back cover)'), ('authors', OrderedDict([('author', OrderedDict([('id', '8120'), ('name', 'Arthur  Miller'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201186455p5/8120.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201186455p2/8120.jpg')])), ('link', 'https://www.goodreads.com/author/show/8120.Arthur_Miller'), ('average_rating', '3.59'), ('ratings_count', '550416'), ('text_reviews_count', '14952')]))])), ('published', '2003'), ('work', OrderedDict([('id', '1426723'), ('uri', 'kca://work/amzn1.gr.work.v1.Jaxd0bIoSWAN9rx4HzDwjQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '886785')])), ('isbn', '0714833568'), ('isbn13', '9780714833569'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '21')])), ('uri', 'kca://book/amzn1.gr.book.v1.rAxLhrIuurET1Dbx2hMPoA'), ('title', 'Modern Architecture Since 1900'), ('title_without_series', 'Modern Architecture Since 1900'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/886785.Modern_Architecture_Since_1900'), ('num_pages', '736'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Phaidon Press'), ('publication_day', '27'), ('publication_year', '1996'), ('publication_month', '6'), ('average_rating', '4.09'), ('ratings_count', '1051'), ('description', 'Since its first publication in 1982, &lt;i&gt;Modern Architecture Since 1900&lt;/i&gt; has become established as a contemporary classic. Worldwide in scope, it combines a clear historical outline with masterly analysis and interpretation. Technical, economic, social and intellectual developments are brought together in a comprehensive narrative which provides a setting for the detailed examination of buildings. Throughout the book the author\'s focus is on the individual architect, and on the qualities that give outstanding buildings their lasting value.&lt;br /&gt;&lt;br /&gt;For the third edition, the text has been radically revised and expanded, incorporating much new material and a fresh appreciation of regional identity and variety. Seven chapters are entirely new, including expanded coverage of recent world architecture.&lt;br /&gt;&lt;br /&gt;Described by James Ackerman of Harvard University as "immeasurably the finest work covering this field in existence", this book presents a penetrating analysis of the modern tradition and its origins, tracing the creative interaction between old and new that has generated such an astonishing richness of architectural forms across the world and throughout the century.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3976667'), ('name', 'William J.R. Curtis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1380554725p5/3976667.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1380554725p2/3976667.jpg')])), ('link', 'https://www.goodreads.com/author/show/3976667.William_J_R_Curtis'), ('average_rating', '4.08'), ('ratings_count', '1129'), ('text_reviews_count', '23')]))])), ('published', '1996'), ('work', OrderedDict([('id', '872044'), ('uri', 'kca://work/amzn1.gr.work.v1.ZSoJ4MCRLdTd6Th4yZ0n6g')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '11012')])), ('isbn', '0192839993'), ('isbn13', '9780192839992'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3405')])), ('uri', 'kca://book/amzn1.gr.book.v1.KblRjbRdBwFtFzWvuWDuhw'), ('title', 'Dubliners'), ('title_without_series', 'Dubliners'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1334138184l/11012._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1334138184l/11012._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/11012.Dubliners'), ('num_pages', '207'), ('format', 'Paperback'), ('edition_information', "Oxford World's Classics"), ('publisher', 'Oxford University Press'), ('publication_day', '15'), ('publication_year', '2001'), ('publication_month', '3'), ('average_rating', '3.85'), ('ratings_count', '120674'), ('description', 'This work of art reflects life in Ireland at the turn of the last century, and by rejecting euphemism, reveals to the Irish their unromantic realities. Each of the 15 stories offers glimpses into the lives of ordinary Dubliners, and collectively they paint a portrait of a nation.'), ('authors', OrderedDict([('author', OrderedDict([('id', '5144'), ('name', 'James Joyce'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517863935p5/5144.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517863935p2/5144.jpg')])), ('link', 'https://www.goodreads.com/author/show/5144.James_Joyce'), ('average_rating', '3.74'), ('ratings_count', '412938'), ('text_reviews_count', '21267')]))])), ('published', '2001'), ('work', OrderedDict([('id', '260248'), ('uri', 'kca://work/amzn1.gr.work.v1.0VPHnf0j0ZK6NC33OETGgQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '100915')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15566')])), ('uri', 'kca://book/amzn1.gr.book.v1.bTpunK9LhLneojBwpPB9iQ'), ('title', 'The Lion, the Witch and the Wardrobe (Chronicles of Narnia, #1)'), ('title_without_series', 'The Lion, the Witch and the Wardrobe'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353029077l/100915._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353029077l/100915._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/100915.The_Lion_the_Witch_and_the_Wardrobe'), ('num_pages', '206'), ('format', 'Paperback'), ('edition_information', 'Film Tie-in Edition (US/CAN)'), ('publisher', 'HarperCollins Publishers'), ('publication_day', None), ('publication_year', '2005'), ('publication_month', None), ('average_rating', '4.22'), ('ratings_count', '2077083'), ('description', "Narnia...the land beyond the wardrobe door, a secret place frozen in eternal winter, a magical country waiting to be set free.&lt;br /&gt;&lt;br /&gt;Lucy is the first to find the secret of the wardrobe in the professor's mysterious old house. At first her brothers and sister don't believe her when she tells of her visit to the land of Narnia. But soon Edmund, then Peter and Susan step through the wardrobe themselves. In Narnia they find a country buried under the evil enchantment of the White Witch. When they meet the Lion Aslan, they realize they've been called to a great adventure and bravely join the battle to free Narnia from the Witch's sinister spell."), ('authors', OrderedDict([('author', OrderedDict([('id', '1069006'), ('name', 'C.S. Lewis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1564671804p5/1069006.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1564671804p2/1069006.jpg')])), ('link', 'https://www.goodreads.com/author/show/1069006.C_S_Lewis'), ('average_rating', '4.15'), ('ratings_count', '5735847'), ('text_reviews_count', '133362')]))])), ('published', '2005'), ('work', OrderedDict([('id', '4790821'), ('uri', 'kca://work/amzn1.gr.work.v1.rqpJlzO5rS559vW35rJa1w')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '48855')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '22066')])), ('uri', 'kca://book/amzn1.gr.book.v1.NpJw6QbRgLr9alsXArRByw'), ('title', 'The Diary of a Young Girl'), ('title_without_series', 'The Diary of a Young Girl'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1560816565l/48855._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1560816565l/48855._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/48855.The_Diary_of_a_Young_Girl'), ('num_pages', '283'), ('format', 'Mass Market Paperback'), ('edition_information', 'US / CAN Edition'), ('publisher', 'Bantam'), ('publication_day', None), ('publication_year', '1993'), ('publication_month', '7'), ('average_rating', '4.15'), ('ratings_count', '2663204'), ('description', 'Discovered in the attic in which she spent the last years of her life, Anne Frank’s remarkable diary has become a world classic—a powerful reminder of the horrors of war and an eloquent testament to the human spirit. &lt;br /&gt;&lt;br /&gt;In 1942, with the Nazis occupying Holland, a thirteen-year-old Jewish girl and her family fled their home in Amsterdam and went into hiding. For the next two years, until their whereabouts were betrayed to the Gestapo, the Franks and another family lived cloistered in the “Secret Annexe” of an old office building. Cut off from the outside world, they faced hunger, boredom, the constant cruelties of living in confined quarters, and the ever-present threat of discovery and death. In her diary Anne Frank recorded vivid impressions of her experiences during this period. By turns thoughtful, moving, and surprisingly humorous, her account offers a fascinating commentary on human courage and frailty and a compelling self-portrait of a sensitive and spirited young woman whose promise was tragically cut short.&lt;br /&gt;--back cover'), ('authors', OrderedDict([('author', OrderedDict([('id', '3720'), ('name', 'Anne Frank'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1343271406p5/3720.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1343271406p2/3720.jpg')])), ('link', 'https://www.goodreads.com/author/show/3720.Anne_Frank'), ('average_rating', '4.15'), ('ratings_count', '2715878'), ('text_reviews_count', '29724')]))])), ('published', '1993'), ('work', OrderedDict([('id', '3532896'), ('uri', 'kca://work/amzn1.gr.work.v1.Hn8z2cQc--WW1zAa5fCZ8Q')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '23418')])), ('isbn', '0375424431'), ('isbn13', '9780375424434'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '568')])), ('uri', 'kca://book/amzn1.gr.book.v1.4Xb6Kyv3wTW1yf-CyMYZww'), ('title', 'The Architecture of Happiness'), ('title_without_series', 'The Architecture of Happiness'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1320402527l/23418._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1320402527l/23418._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/23418.The_Architecture_of_Happiness'), ('num_pages', '280'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Pantheon Books'), ('publication_day', '3'), ('publication_year', '2006'), ('publication_month', '10'), ('average_rating', '3.86'), ('ratings_count', '9461'), ('description', "One of the great but often unmentioned causes of both happiness and misery is the quality of our environment: the kinds of walls, chairs, buildings and streets that surround us.&lt;br /&gt;&lt;br /&gt;And yet a concern for architecture and design is too often described as frivolous, even self-indulgent. &lt;i&gt;The Architecture of Happiness&lt;/i&gt; starts from the idea that where we are heavily influences who we can be, and it argues that it is architecture's task to stand as an eloquent reminder of our full potential.&lt;br /&gt;&lt;br /&gt;Whereas many architects are wary of openly discussing the word beauty, this book has at its center the large and naÃ¯ve question: What is a beautiful building? It is a tour through the philosophy and psychology of architecture that aims to change the way we think about our homes, our streets and ourselves."), ('authors', OrderedDict([('author', OrderedDict([('id', '13199'), ('name', 'Alain de Botton'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1189753902p5/13199.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1189753902p2/13199.jpg')])), ('link', 'https://www.goodreads.com/author/show/13199.Alain_de_Botton'), ('average_rating', '3.88'), ('ratings_count', '156191'), ('text_reviews_count', '14818')]))])), ('published', '2006'), ('work', OrderedDict([('id', '14280280'), ('uri', 'kca://work/amzn1.gr.work.v1.rEzwDi9RY4yEBtT22gamiw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65118')])), ('isbn', '1405206128'), ('isbn13', '9781405206129'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1631')])), ('uri', 'kca://book/amzn1.gr.book.v1.N-akGxhuwZFzm7LbrmJFRA'), ('title', 'The Hostile Hospital (A Series of Unfortunate Events, #8)'), ('title_without_series', 'The Hostile Hospital'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1442446120l/65118._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1442446120l/65118._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65118.The_Hostile_Hospital'), ('num_pages', '272'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Egmont'), ('publication_day', '10'), ('publication_year', '2003'), ('publication_month', '5'), ('average_rating', '3.98'), ('ratings_count', '95424'), ('description', 'There is nothing to be found in the pages of these books but misery and despair. You still have time to choose something else to read. But if you must know what unpleasantries befall the charming and clever Baudelaire children read on...The Hostile Hospital - There are many pleasant things to read about, but this book contains none of them. Within its pages are such burdensome details as a suspicious shopkeeper, unnecessary surgery, heartshaped balloons, and some very starling news about a fire. Clearly you do not want to read about such things.'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2003'), ('work', OrderedDict([('id', '2361348'), ('uri', 'kca://work/amzn1.gr.work.v1.ZpzpFRdXjTgW8J55PN2lTA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65112')])), ('isbn', '0064410161'), ('isbn13', '9780064410168'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3898')])), ('uri', 'kca://book/amzn1.gr.book.v1.o5jBgMg8ttG282oaM2iIDQ'), ('title', 'The End (A Series of Unfortunate Events, #13)'), ('title_without_series', 'The End'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524761836l/65112._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524761836l/65112._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65112.The_End'), ('num_pages', '337'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '13'), ('publication_year', '2006'), ('publication_month', '10'), ('average_rating', '4.01'), ('ratings_count', '86833'), ('description', "The last volume of the fabulously popular A Series of Unfortunate Events series, in which the history of the Baudelaire orphans is brought to its end.&lt;br /&gt;&lt;br /&gt;You are presumably looking at the back of this book, or the end of the end. The end of the end is the best place to begin the end, because if you read the end from the beginning of the beginning of the end to the end of the end of the end, you will arrive at the end of the end of your rope. &lt;br /&gt;&lt;br /&gt;This book is the last in A Series of Unfortunate Events, and even if you braved the previous twelve volumes, you probably can't stand such unpleasantries as a fearsome storm, a suspicious beverage, a herd of wild sheep, an enormous bird cage, and a truly haunting secret about the Baudelaire parents. &lt;br /&gt;&lt;br /&gt;It has been my solemn occupation to complete the history of the Baudelaire orphans, and at last I am finished. You likely have some other occupation, so if I were you I would drop this book at once, so the end does not finish you. &lt;br /&gt;&lt;br /&gt;With all due respect, &lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2006'), ('work', OrderedDict([('id', '838691'), ('uri', 'kca://work/amzn1.gr.work.v1.OqpRj6gIRLqzkyybvvAbRQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65110')])), ('isbn', '0064410153'), ('isbn13', '9780064410151'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2021')])), ('uri', 'kca://book/amzn1.gr.book.v1.sKBvH0WXYsoxUb8stGauIw'), ('title', 'The Penultimate Peril (A Series of Unfortunate Events, #12)'), ('title_without_series', 'The Penultimate Peril'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524161970l/65110._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524161970l/65110._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65110.The_Penultimate_Peril'), ('num_pages', '353'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '18'), ('publication_year', '2005'), ('publication_month', '10'), ('average_rating', '4.06'), ('ratings_count', '87050'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;If this is the first book you found while searching for a book to read next, then the first thing you should know is that this next-to-last book is what you should put down first. Sadly, this book presents the next-to-last chronicle of the lives of the Baudelaire orphans, and it is next-to-first in its supply of misery, despair, and unpleasantness.&lt;/p&gt;&lt;p&gt;Probably the next-to-last thing you would like to read about are a harpoon gun, a rooftop sunbathing alon, two mysterious initials, three unidentified triplets, a notorious villain, and an unsavory curry.&lt;/p&gt;&lt;p&gt;Next-to-last things are the first thing to be avoided, and so allow me to recommend that you put this next-to-last book down first, and find something else to read next at last, such a s the next-to-last book in another chronicle, or a chronicle containing other next-to-last things, so that this next-to-last book does not become the last book you will read.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2005'), ('work', OrderedDict([('id', '838097'), ('uri', 'kca://work/amzn1.gr.work.v1.3aEI3fpcHODxBn9RwdHPqQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65111')])), ('isbn', '0064410145'), ('isbn13', '9780064410144'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1972')])), ('uri', 'kca://book/amzn1.gr.book.v1.YaMjhdf0gtU1qDfmuUVL-A'), ('title', 'The Grim Grotto (A Series of Unfortunate Events, #11)'), ('title_without_series', 'The Grim Grotto'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519247467l/65111._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519247467l/65111._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65111.The_Grim_Grotto'), ('num_pages', '323'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '21'), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '4.01'), ('ratings_count', '94205'), ('description', "Dear Reader, &lt;br /&gt;&lt;br /&gt;Unless you are a slug, a sea anemone, or mildew, you probably prefer not to be damp. You might also prefer not to read this book, in which the Baudelaire siblings encounter an unpleasant amount of dampness as they descend into the depths of despair, underwater. &lt;br /&gt;&lt;br /&gt;In fact, the horrors they encounter are too numerous to list, and you wouldn't want me even to mention the worst of it, which includes mushrooms, a desperate search for something lost, a mechanical monster, a distressing message from a lost friend, and tap dancing. &lt;br /&gt;&lt;br /&gt;As a dedicated author who has pledged to keep recording the depressing story of the Baudelaires, I must continue to delve deep into the cavernous depths of the orphans' lives. You, on the other hand, may delve into some happier book in order to keep your eyes and your spirits from being dampened. &lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2004'), ('work', OrderedDict([('id', '1168322'), ('uri', 'kca://work/amzn1.gr.work.v1.UtMiT7w_j77ysE78-oMoGQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '297792')])), ('isbn', '0064410137'), ('isbn13', '9780064410137'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2131')])), ('uri', 'kca://book/amzn1.gr.book.v1.KPR1e-RXoBoMpF1Wx5lRWQ'), ('title', 'The Slippery Slope (A Series of Unfortunate Events, #10)'), ('title_without_series', 'The Slippery Slope'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518835363l/297792._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518835363l/297792._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/297792.The_Slippery_Slope'), ('num_pages', '337'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '23'), ('publication_year', '2003'), ('publication_month', '9'), ('average_rating', '4.03'), ('ratings_count', '103343'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;Like handshakes, house pets, or raw carrots, many things are preferable when not slippery. Unfortunately, in this miserable volume, I am afraid that Violet, Klaus, and Sunny Baudelaire run into more than their fair share of slipperiness during their harrowing journey up--and down--a range of strange and distressing mountains.&lt;p&gt;In order to spare you any further repulsion, it would be best not to mention any of the unpleasant details of this story, particularly a secret message, a toboggan, a deceitful map, a swarm of snow gnats, a scheming villain, a troupe of organized youngsters, a covered casserole dish, and a surprising survivor of a terrible fire.&lt;/p&gt;&lt;p&gt;Unfortunately, I have dedicated my life to researching and recording the sad tale of the Baudelaire orphans. There is no reason for you to dedicate your-self to such things, and you might instead dedicate yourself to letting this slippery book slip from your hands into a nearby trash receptacle, or deep pit.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2003'), ('work', OrderedDict([('id', '2146706'), ('uri', 'kca://work/amzn1.gr.work.v1.Nidc-fP0LJc7sWuh6AE06Q')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '324277')])), ('isbn', '0064410129'), ('isbn13', '9780064410120'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2130')])), ('uri', 'kca://book/amzn1.gr.book.v1.XJc_8ov0VbLt7ak5mbAVTQ'), ('title', 'The Carnivorous Carnival (A Series of Unfortunate Events, #9)'), ('title_without_series', 'The Carnivorous Carnival'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518209848l/324277._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518209848l/324277._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/324277.The_Carnivorous_Carnival'), ('num_pages', '286'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '17'), ('publication_year', '2002'), ('publication_month', '10'), ('average_rating', '3.99'), ('ratings_count', '106725'), ('description', '&lt;i&gt;Dear reader&lt;/i&gt;,&lt;br /&gt;&lt;br /&gt;The word "carnivorous," which appears in the title of this book, means "meat-eating," and once you have read such a bloodthirsty word, there is no reason to read any further. This carnivorous volume contains such a distressing story that consuming any of its contents would be far more stomach-turning than even the most imbalanced meal.&lt;br /&gt;&lt;br /&gt;To avoid causing discomfort, it would be best if I didn\'t mention any of the unnerving ingredients of this story, particularly a confusing map, an ambidextrous person, an unruly crowd, a wooden plank, and Chabo the Wolf Baby.&lt;br /&gt;&lt;br /&gt;Sadly for me, my time is filled with researching and recording the displeasing and disenchanting lives of the Baudelaire orphans. But your time might be better filled with something more palatable, such as eating your vegetables, or feeding them to someone else.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;With all due respect&lt;/i&gt;,&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2002'), ('work', OrderedDict([('id', '984147'), ('uri', 'kca://work/amzn1.gr.work.v1.wUjMV1dlx_UGGmBmcgg3pA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '150037')])), ('isbn', '0060566221'), ('isbn13', '9780060566227'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2220')])), ('uri', 'kca://book/amzn1.gr.book.v1.MxcD0KwNfDghjb7JHgBC_A'), ('title', 'The Vile Village (A Series of Unfortunate Events, #7)'), ('title_without_series', 'The Vile Village'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352066958l/150037._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352066958l/150037._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/150037.The_Vile_Village'), ('num_pages', '272'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '24'), ('publication_year', '2001'), ('publication_month', '4'), ('average_rating', '3.96'), ('ratings_count', '116777'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;You have undoubtedly picked up this book by mistake, so please put it down. Nobody in their right mind would read this particular book about the lives of Violet, Klaus, and Sunny Baudelaire on purpose, because each dismal moment of their stay in the village of V.F.D. has been faithfully and dreadfully recorded in these pages. I can think of no single reason why anyone would want to open a book containing such unpleasant matters as migrating crows, an angry mob, a newspaper headline, the arrest of innocent people, the Deluxe Cell, and some very strange hats. It is my solemn and sacred occupation to research each detail of the Baudelaire children's lives and write them all down, but you may prefer to do some other solemn and sacred thing, such as reading another book instead.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2001'), ('work', OrderedDict([('id', '324576'), ('uri', 'kca://work/amzn1.gr.work.v1.isKFj2SwiZmAFC0l2uZ45g')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '172327')])), ('isbn', '0060566213'), ('isbn13', '9780060566210'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2591')])), ('uri', 'kca://book/amzn1.gr.book.v1.MmhTLciyQyHsKwkk-vP0sw'), ('title', 'The Ersatz Elevator (A Series of Unfortunate Events, #6)'), ('title_without_series', 'The Ersatz Elevator'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1514267383l/172327._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1514267383l/172327._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/172327.The_Ersatz_Elevator'), ('num_pages', '259'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'HarperCollins Publishers'), ('publication_day', '20'), ('publication_year', '2001'), ('publication_month', '2'), ('average_rating', '4.04'), ('ratings_count', '119109'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;If you have just picked up this book, then it is not too late to put it back down. Like the previous books in A SERIES OF UNFORTUNATE EVENTS, there is nothing to be found in these pages but misery, despair, and discomfort, and you still have time to choose something else to read.&lt;/p&gt;&lt;p&gt;Within the chapters of this story, Violet, Klaus and Sunny Baudelaire encounter a darkened staircase, a red herring, some friends in a dire situation, three mysterious initials, a liar with an evil scheme, a secret passageway, and parsley soda.&lt;/p&gt;&lt;p&gt;I have sworn to write down these tales of the Baudelaire orphans so the general public will know each terrible thing that has happened to them, but if you decide to read something else instead, you will save yourself from a heapful of horror and woe.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2001'), ('work', OrderedDict([('id', '1168344'), ('uri', 'kca://work/amzn1.gr.work.v1.U9-MEJgi89OXJkBtt282vA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '131123')])), ('isbn', '0064408639'), ('isbn13', '9780064408639'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3173')])), ('uri', 'kca://book/amzn1.gr.book.v1.5IgXnU5LuMMqkeb8hJgbqQ'), ('title', 'The Austere Academy (A Series of Unfortunate Events, #5)'), ('title_without_series', 'The Austere Academy'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1517277307l/131123._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1517277307l/131123._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/131123.The_Austere_Academy'), ('num_pages', '221'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '31'), ('publication_year', '2000'), ('publication_month', '8'), ('average_rating', '3.99'), ('ratings_count', '128511'), ('description', "Dear Reader, &lt;br /&gt;&lt;br /&gt;If you are looking for a story about cheerful youngsters spending a jolly time at boarding school, look elsewhere. Violet, Klaus, and Sunny Baudelaire are intelligent and resourceful children, and you might expect that they would do very well at school. Don't. For the Baudelaires, school turns out to be another miserable episode in their unlucky lives. &lt;br /&gt;&lt;br /&gt;Truth be told, within the chapters that make up this dreadful story, the children will face snapping crabs, strict punishments, dripping fungus, comprehensive exams, violin recitals, S.O.R.E., and the metric system. &lt;br /&gt;&lt;br /&gt;It is my solemn duty to stay up all night researching and writing the history of these three hapless youngsters, but you may be more comfortable getting a good night's sleep. In that case, you should probably choose some other book. &lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1165972'), ('uri', 'kca://work/amzn1.gr.work.v1.hc5aeS0-2YZWQzvNAaFDIA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65119')])), ('isbn', '0439272637'), ('isbn13', '9780439272636'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3158')])), ('uri', 'kca://book/amzn1.gr.book.v1.cwsqrGnBpl8pYvcEzpiWqg'), ('title', 'The Miserable Mill (A Series of Unfortunate Events, #4)'), ('title_without_series', 'The Miserable Mill'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146209l/65119._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146209l/65119._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65119.The_Miserable_Mill'), ('num_pages', '194'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '15'), ('publication_year', '2000'), ('publication_month', '4'), ('average_rating', '3.86'), ('ratings_count', '135833'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;I hope, for your sake, that you have not chosen to read this book because you are in the mood for a pleasant experience. If this is the case, I advise you to put this book down instantaneously, because of all the books describing the unhappy lives of the Baudelaire orphans, The Miserable Mill might be the unhappiest yet. Violet, Klaus, and Sunny Baudelaire are sent to Paltryville to work in a lumber mill, and they find disaster and misfortune lurking behind every log.&lt;br /&gt;&lt;br /&gt;The pages of this book, I'm sorry to inform you, contain such unpleasantries as a giant pincher machine, a bad casserole, a man with a cloud of smoke where his head should be, a hypnotist, a terrible accident resulting in injury, and coupons.&lt;br /&gt;&lt;br /&gt;I have promised to write down the entire history of these three poor children, but you haven't, so if you prefer stories that are more heartwarming, please feel free to make another selection.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1209957'), ('uri', 'kca://work/amzn1.gr.work.v1._IQA4lfOoi-TkPbblApQ8Q')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '438492')])), ('isbn', '0064407683'), ('isbn13', '9780064407687'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '4170')])), ('uri', 'kca://book/amzn1.gr.book.v1._aUS-_mAErJpQ5eyte0BAg'), ('title', 'The Wide Window (A Series of Unfortunate Events, #3)'), ('title_without_series', 'The Wide Window'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518654331l/438492._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518654331l/438492._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/438492.The_Wide_Window'), ('num_pages', '214'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '25'), ('publication_year', '2000'), ('publication_month', '2'), ('average_rating', '3.94'), ('ratings_count', '154937'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;If you have not read anything about the Baudelaire orphans, then before you read even one more sentence, you should know this: Violet, Klaus, and Sunny are kindhearted and quick-witted; but their lives, I am sorry to say, are filled with bad luck and misery. All of the stories about these three children are unhappy and wretched, and this one may be the worst of them all. If you haven't got the stomach for a story that includes a hurricane, a signalling device, hungry leeches, cold cucumber soup, a horrible villain, and a doll named Pretty Penny, then this book will probably fill you with despair. I will continue to record these tragic tales, for that is what I do. You, however, should decide for yourself whether you can possibly endure this miserable story.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1168377'), ('uri', 'kca://work/amzn1.gr.work.v1.X7RFHj-prALpuMXH_TqjNA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '78418')])), ('isbn', '0439206480'), ('isbn13', '9780439206488'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5238')])), ('uri', 'kca://book/amzn1.gr.book.v1.qLIM816ncARYXqU-PxgONg'), ('title', 'The Reptile Room (A Series of Unfortunate Events, #2)'), ('title_without_series', 'The Reptile Room'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146294l/78418._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146294l/78418._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/78418.The_Reptile_Room'), ('num_pages', '192'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '30'), ('publication_year', '1999'), ('publication_month', '9'), ('average_rating', '3.99'), ('ratings_count', '177534'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;If you have picked up this book with the hope of finding a simple and cheery tale, I'm afraid you have picked up the wrong book altogether. The story may seem cheery at first, when the Baudelaire children spend time in the company of some interesting reptiles and a giddy uncle, but don't be fooled. If you know anything at all about the unlucky Baudelaire children, you already know that even pleasant events lead down the same road to misery.&lt;br /&gt;&lt;br /&gt;In fact, within the pages you now hold in your hands, the three siblings endure a car accident, a terrible odor, a deadly serpent, a long knife, a large brass reading lamp, and the appearance of a person they'd hoped never to see again.&lt;br /&gt;&lt;br /&gt;I am bound to record these tragic events, but you are free to put this book back on the shelf and seek something lighter.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '1999'), ('work', OrderedDict([('id', '888312'), ('uri', 'kca://work/amzn1.gr.work.v1.RFUKbJ7fsZRi9dPU8XqccQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1622')])), ('isbn', '0743477545'), ('isbn13', '9780743477543'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5793')])), ('uri', 'kca://book/amzn1.gr.book.v1.lR1AfwDypVhrjCWKj1EDUw'), ('title', "A Midsummer Night's Dream"), ('title_without_series', "A Midsummer Night's Dream"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327874534l/1622._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327874534l/1622._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1622.A_Midsummer_Night_s_Dream'), ('num_pages', '240'), ('format', 'Paperback'), ('edition_information', 'Folger Shakespeare Library'), ('publisher', 'Simon &amp; Schuster Paperbacks'), ('publication_day', None), ('publication_year', '2016'), ('publication_month', '7'), ('average_rating', '3.95'), ('ratings_count', '436354'), ('description', "Shakespeare's intertwined love polygons begin to get complicated from the start--Demetrius and Lysander both want Hermia but she only has eyes for Lysander. Bad news is, Hermia's father wants Demetrius for a son-in-law. On the outside is Helena, whose unreturned love burns hot for Demetrius. Hermia and Lysander plan to flee from the city under cover of darkness but are pursued by an enraged Demetrius (who is himself pursued by an enraptured Helena). In the forest, unbeknownst to the mortals, Oberon and Titania (King and Queen of the faeries) are having a spat over a servant boy. The plot twists up when Oberon's head mischief-maker, Puck, runs loose with a flower which causes people to fall in love with the first thing they see upon waking. Throw in a group of labourers preparing a play for the Duke's wedding (one of whom is given a donkey's head and Titania for a lover by Puck) and the complications become fantastically funny."), ('authors', OrderedDict([('author', OrderedDict([('id', '947'), ('name', 'William Shakespeare'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1586700347p5/947.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1586700347p2/947.jpg')])), ('link', 'https://www.goodreads.com/author/show/947.William_Shakespeare'), ('average_rating', '3.87'), ('ratings_count', '6178888'), ('text_reviews_count', '113650')]))])), ('published', '2016'), ('work', OrderedDict([('id', '894834'), ('uri', 'kca://work/amzn1.gr.work.v1.YiKowoSszfZ21MlDdsqApw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2156')])), ('isbn', '0192802631'), ('isbn13', '9780192802637'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '11929')])), ('uri', 'kca://book/amzn1.gr.book.v1.k8DSe52-iqTSlumfATCuOw'), ('title', 'Persuasion'), ('title_without_series', 'Persuasion'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2156.Persuasion'), ('num_pages', '249'), ('format', 'Paperback'), ('edition_information', "Oxford World's Classics"), ('publisher', 'Oxford University Press'), ('publication_day', '18'), ('publication_year', '2004'), ('publication_month', '3'), ('average_rating', '4.14'), ('ratings_count', '511933'), ('description', "Twenty-seven-year old Anne Elliot is Austen's most adult heroine. Eight years before the story proper begins, she is happily betrothed to a naval officer, Frederick Wentworth, but she precipitously breaks off the engagement when persuaded by her friend Lady Russell that such a match is unworthy. The breakup produces in Anne a deep and long-lasting regret. When later Wentworth returns from sea a rich and successful captain, he finds Anne's family on the brink of financial ruin and his own sister a tenant in Kellynch Hall, the Elliot estate. All the tension of the novel revolves around one question: Will Anne and Wentworth be reunited in their love?&lt;br /&gt;&lt;br /&gt;Jane Austen once compared her writing to painting on a little bit of ivory, 2 inches square. Readers of &lt;i&gt;Persuasion&lt;/i&gt; will discover that neither her skill for delicate, ironic observations on social custom, love, and marriage nor her ability to apply a sharp focus lens to English manners and morals has deserted her in her final finished work."), ('authors', OrderedDict([('author', OrderedDict([('id', '1265'), ('name', 'Jane Austen'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588941810p5/1265.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588941810p2/1265.jpg')])), ('link', 'https://www.goodreads.com/author/show/1265.Jane_Austen'), ('average_rating', '4.12'), ('ratings_count', '5910834'), ('text_reviews_count', '167287')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2534720'), ('uri', 'kca://work/amzn1.gr.work.v1.R7MwsnCfyHc7718MW02Mlw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '19302')])), ('isbn', '0142402494'), ('isbn13', '9780142402498'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2671')])), ('uri', 'kca://book/amzn1.gr.book.v1.ii6LisChBeRuZTUpUJ9wtQ'), ('title', 'Pippi Longstocking'), ('title_without_series', 'Pippi Longstocking'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519300455l/19302._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519300455l/19302._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/19302.Pippi_Longstocking'), ('num_pages', '160'), ('format', 'Mass Market Paperback'), ('edition_information', 'Puffin Modern Classics, US / CAN'), ('publisher', 'Puffin Books'), ('publication_day', '21'), ('publication_year', '2005'), ('publication_month', '4'), ('average_rating', '4.13'), ('ratings_count', '163626'), ('description', 'Tommy and his sister Annika have a new neighbor, and her name is Pippi Longstocking. She has crazy red pigtails, no parents to tell her what to do, a horse that lives on her porch, and a flair for the outrageous that seems to lead to one adventure after another!&lt;br /&gt;--back cover'), ('authors', OrderedDict([('author', OrderedDict([('id', '410653'), ('name', 'Astrid Lindgren'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1194544214p5/410653.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1194544214p2/410653.jpg')])), ('link', 'https://www.goodreads.com/author/show/410653.Astrid_Lindgren'), ('average_rating', '4.18'), ('ratings_count', '343362'), ('text_reviews_count', '9733')]))])), ('published', '2005'), ('work', OrderedDict([('id', '2056462'), ('uri', 'kca://work/amzn1.gr.work.v1.E1lszyEERQLYQMtVqxoJIA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '78411')])), ('isbn', '0439206472'), ('isbn13', '9780439206471'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '13568')])), ('uri', 'kca://book/amzn1.gr.book.v1.OldE8Tvjj9nHLRUqfcPEvA'), ('title', 'The Bad Beginning (A Series of Unfortunate Events, #1)'), ('title_without_series', 'The Bad Beginning'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1436737029l/78411._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1436737029l/78411._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/78411.The_Bad_Beginning'), ('num_pages', '176'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '30'), ('publication_year', '1999'), ('publication_month', '9'), ('average_rating', '3.95'), ('ratings_count', '385950'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;I'm sorry to say that the book you are holding in your hands is extremely unpleasant. It tells an unhappy tale about three very unlucky children. Even though they are charming and clever, the Baudelaire siblings lead lives filled with misery and woe. From the very first page of this book when the children are at the beach and receive terrible news, continuing on through the entire story, disaster lurks at their heels. One might say they are magnets for misfortune.&lt;br /&gt;&lt;br /&gt;In this short book alone, the three youngsters encounter a greedy and repulsive villain, itchy clothing, a disastrous fire, a plot to steal their fortune, and cold porridge for breakfast.&lt;br /&gt;&lt;br /&gt;It is my sad duty to write down these unpleasant tales, but there is nothing stopping you from putting this book down at once and reading something happy, if you prefer that sort of thing.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1955634'), ('text_reviews_count', '71792')]))])), ('published', '1999'), ('work', OrderedDict([('id', '1069597'), ('uri', 'kca://work/amzn1.gr.work.v1.OmRsXq3qTORc2Lu2Vb3xfQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '24178')])), ('isbn', '0064410935'), ('isbn13', '9780064410939'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15441')])), ('uri', 'kca://book/amzn1.gr.book.v1.-3kSw9en_4pNo5tVmbKj8g'), ('title', "Charlotte's Web"), ('title_without_series', "Charlotte's Web"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1439632243l/24178._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1439632243l/24178._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/24178.Charlotte_s_Web'), ('num_pages', '184'), ('format', 'Paperback'), ('edition_information', 'Full Color Edition'), ('publisher', 'HarperCollinsPublishers'), ('publication_day', '1'), ('publication_year', '2001'), ('publication_month', '10'), ('average_rating', '4.17'), ('ratings_count', '1378932'), ('description', 'This beloved book by E. B. White, author of &lt;i&gt;Stuart Little&lt;/i&gt; and &lt;i&gt;The Trumpet of the Swan&lt;/i&gt;, is a classic of children\'s literature that is "just about perfect." This high-quality paperback features vibrant illustrations colorized by Rosemary Wells!&lt;br /&gt;&lt;br /&gt;Some Pig. Humble. Radiant. These are the words in Charlotte\'s Web, high up in Zuckerman\'s barn. Charlotte\'s spiderweb tells of her feelings for a little pig named Wilbur, who simply wants a friend. They also express the love of a girl named Fern, who saved Wilbur\'s life when he was born the runt of his litter.&lt;br /&gt;&lt;br /&gt;E. B. White\'s Newbery Honor Book is a tender novel of friendship, love, life, and death that will continue to be enjoyed by generations to come. This edition contains newly color illustrations by Garth Williams, the acclaimed illustrator of E. B. White\'s &lt;i&gt;Stuart Little&lt;/i&gt; and Laura Ingalls Wilder\'s Little House series, among many other books.'), ('authors', OrderedDict([('author', OrderedDict([('id', '988142'), ('name', 'E.B. White'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198519412p5/988142.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198519412p2/988142.jpg')])), ('link', 'https://www.goodreads.com/author/show/988142.E_B_White'), ('average_rating', '4.15'), ('ratings_count', '1650856'), ('text_reviews_count', '28424')]))])), ('published', '2001'), ('work', OrderedDict([('id', '987048'), ('uri', 'kca://work/amzn1.gr.work.v1.cG9p_zAXsGI5Bz6-5OtD3g')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38709')])), ('isbn', '0439244196'), ('isbn13', '9780439244190'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '18129')])), ('uri', 'kca://book/amzn1.gr.book.v1.RJ9IilhRW_Pz1BbzO4_XrQ'), ('title', 'Holes (Holes, #1)'), ('title_without_series', 'Holes'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1552422497l/38709._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1552422497l/38709._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38709.Holes'), ('num_pages', '233'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic'), ('publication_day', '2'), ('publication_year', '2000'), ('publication_month', '9'), ('average_rating', '3.97'), ('ratings_count', '947104'), ('description', 'Stanley tries to dig up the truth in this inventive and darkly humorous tale of crime and punishment -- and redemption. &lt;br /&gt;&lt;br /&gt;Stanley Yelnats is under a curse. A curse that began with his no-good-dirty-rotten- pig-stealing-great-great-grandfather and has since followed generations of Yelnats. Now Stanley has been unjustly sent to a boys\' detention center, Camp Green Lake, where the warden makes the boys "build character" by spending all day, every day, digging holes: five feet wide and five feet deep. It doesn\'t take long for Stanley to realize there\'s more than character improvement going on at Camp Green Lake. The boys are digging holes because the warden is looking for something. Stanley tries to dig up the truth in this inventive and darkly humorous tale of crime and punishment—and redemption.'), ('authors', OrderedDict([('author', OrderedDict([('id', '6569'), ('name', 'Louis Sachar'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_200x266-d279b33f8eec0f27b7272477f09806be.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_50x66-82093808bca726cb3249a493fbd3bd0f.png')])), ('link', 'https://www.goodreads.com/author/show/6569.Louis_Sachar'), ('average_rating', '3.99'), ('ratings_count', '1213019'), ('text_reviews_count', '32955')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1679789'), ('uri', 'kca://work/amzn1.gr.work.v1.NMFGIHdxhGf4RWZG-LLdsw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '117251')])), ('isbn', '0393315053'), ('isbn13', '9780393315059'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '237')])), ('uri', 'kca://book/amzn1.gr.book.v1.UXhE6ZhrWWsShrS2ITXPbA'), ('title', 'Hamlet: Screenplay, Introduction And Film Diary'), ('title_without_series', 'Hamlet: Screenplay, Introduction And Film Diary'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/117251.Hamlet'), ('num_pages', '224'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'W. W. Norton  Company'), ('publication_day', '17'), ('publication_year', '1996'), ('publication_month', '11'), ('average_rating', '4.14'), ('ratings_count', '181027'), ('description', 'Often credited with creating a popular movie audience for Shakespeare, Kenneth Branagh has wanted for many years to bring to the screen the complete, full-length version of &lt;em&gt;Hamlet&lt;/em&gt;, Shakespeare\'s greatest play.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;"The film, like the play, will have something for everyone," he says. "Its a ghost story, a thriller, an action-packed murder mystery, and a great tragedy that is profoundly moving." With an outstanding cast of international actors--including Derek Jacobi as Claudius, Julie Christie as Gertrude, Kate Winslet as Ophelia, Charlton Heston as the Player King, Robin Williams as Osric, and Gerard Depardieu as Reynaldo--Branagh\'s version, in which he will play the title role as well as direct, is sure to go down in film history.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;This beautiful volume includes Branagh\'s introduction and screenplay adaptation of Shakespeare\'s text, color and black-and-white stills, and a production diary that takes us behind the scenes for a day-to-day look at the shooting of his film.'), ('authors', OrderedDict([('author', OrderedDict([('id', '55118'), ('name', 'Kenneth Branagh'), ('role', 'introduction and screenplay'), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330849315p5/55118.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330849315p2/55118.jpg')])), ('link', 'https://www.goodreads.com/author/show/55118.Kenneth_Branagh'), ('average_rating', '4.13'), ('ratings_count', '184708'), ('text_reviews_count', '988')]))])), ('published', '1996'), ('work', OrderedDict([('id', '112914'), ('uri', 'kca://work/amzn1.gr.work.v1.fs3e5pOoUjUs95N0SU6zKA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '7624')])), ('isbn', '0140283331'), ('isbn13', '9780140283334'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '27289')])), ('uri', 'kca://book/amzn1.gr.book.v1.kSnNl4MoBUSPb-pSSfaVZQ'), ('title', 'Lord of the Flies'), ('title_without_series', 'Lord of the Flies'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327869409l/7624._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327869409l/7624._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/7624.Lord_of_the_Flies'), ('num_pages', '182'), ('format', 'Paperback'), ('edition_information', 'Penguin Great Books of the 20th Century'), ('publisher', 'Penguin Books'), ('publication_day', '1'), ('publication_year', '1999'), ('publication_month', '10'), ('average_rating', '3.68'), ('ratings_count', '2216910'), ('description', 'At the dawn of the next world war, a plane crashes on an uncharted island, stranding a group of schoolboys. At first, with no adult supervision, their freedom is something to celebrate; this far from civilization the boys can do anything they want. Anything. They attempt to forge their own society, failing, however, in the face of terror, sin and evil. And as order collapses, as strange howls echo in the night, as terror begins its reign, the hope of adventure seems as far from reality as the hope of being rescued. Labeled a parable, an allegory, a myth, a morality tale, a parody, a political treatise, even a vision of the apocalypse, Lord of the Flies is perhaps our most memorable novel about “the end of innocence, the darkness of man’s heart.”'), ('authors', OrderedDict([('author', OrderedDict([('id', '306'), ('name', 'William Golding'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198342496p5/306.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198342496p2/306.jpg')])), ('link', 'https://www.goodreads.com/author/show/306.William_Golding'), ('average_rating', '3.68'), ('ratings_count', '2235929'), ('text_reviews_count', '37918')]))])), ('published', '1999'), ('work', OrderedDict([('id', '2766512'), ('uri', 'kca://work/amzn1.gr.work.v1.mylCQ2vLQs_kZba8SrXsZg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2998')])), ('isbn', '0517189607'), ('isbn13', '9780517189603'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '12535')])), ('uri', 'kca://book/amzn1.gr.book.v1.-Yu5KHr8IQYAK0jK10dTJQ'), ('title', 'The Secret Garden'), ('title_without_series', 'The Secret Garden'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327873635l/2998._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327873635l/2998._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2998.The_Secret_Garden'), ('num_pages', '331'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', "Children's Classics"), ('publication_day', '1'), ('publication_year', '1998'), ('publication_month', '9'), ('average_rating', '4.14'), ('ratings_count', '867149'), ('description', '"One of the most delightful and enduring classics of children\'s literature, The Secret Garden by Victorian author Frances Hodgson Burnett has remained a firm favorite with children the world over ever since it made its first appearance. Initially published as a serial story in 1910 in The American Magazine, it was brought out in novel form in 1911. &lt;br /&gt; &lt;br /&gt;The plot centers round Mary Lennox, a young English girl who returns to England from India, having suffered the immense trauma by losing both her parents in a cholera epidemic. However, her memories of her parents are not pleasant, as they were a selfish, neglectful and pleasure-seeking couple. Mary is given to the care of her uncle Archibald Craven, whom she has never met. She travels to his home, Misselthwaite Manor located in the gloomy Yorkshire, a vast change from the sunny and warm climate she was used to. When she arrives, she is a rude, stubborn and given to stormy temper tantrums. However, her nature undergoes a gradual transformation when she learns of the tragedies that have befallen her strict and disciplinarian uncle whom she earlier feared and despised. Once when he\'s away from home, Mary discovers a charming walled garden which is always kept locked. The mystery deepens when she hears sounds of sobbing from somewhere within her uncle\'s vast mansion. The kindly servants ignore her queries or pretend they haven\'t heard, spiking Mary\'s curiosity. &lt;br /&gt; &lt;br /&gt;The Secret Garden appeals to both young and old alike. It has wonderful elements of mystery, spirituality, charming characters and an authentic rendering of childhood emotions and experiences. Commonsense, truth and kindness, compassion and a belief in the essential goodness of human beings lie at the heart of this unforgettable story. It is the best known of Frances Hodgson Burnett\'s works, though most of us have definitely heard of, if not read, her other novel Little Lord Fauntleroy. &lt;br /&gt; &lt;br /&gt;The book has been adapted extensively on stage, film and television and translated into all the world\'s major languages. In 1991, a Japanese anime version was launched for television in Japan. It remains a popular and beloved story of a child\'s journey into maturity, and a must-read for every child, parent, teacher and anyone who would enjoy this fascinating glimpse of childhood. One of the most delightful and enduring classics of children\'s literature, The Secret Garden by Victorian author Frances Hodgson Burnett has remained a firm favorite with children the world over ever since it made its first appearance. Initially published as a serial story in 1910 in The American Magazine, it was brought out in novel form in 1911." &lt;br /&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '2041'), ('name', 'Frances Hodgson Burnett'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1197934848p5/2041.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1197934848p2/2041.jpg')])), ('link', 'https://www.goodreads.com/author/show/2041.Frances_Hodgson_Burnett'), ('average_rating', '4.14'), ('ratings_count', '1179838'), ('text_reviews_count', '28323')]))])), ('published', '1998'), ('work', OrderedDict([('id', '3186437'), ('uri', 'kca://work/amzn1.gr.work.v1.63Qg_3M6esESm_90XodD4A')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '157993')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '23816')])), ('uri', 'kca://book/amzn1.gr.book.v1.UOzV_dE308M_I5mJxsCmsA'), ('title', 'The Little Prince'), ('title_without_series', 'The Little Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1367545443l/157993._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1367545443l/157993._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/157993.The_Little_Prince'), ('num_pages', '93'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harcourt, Inc.'), ('publication_day', '29'), ('publication_year', '2000'), ('publication_month', '6'), ('average_rating', '4.31'), ('ratings_count', '1305007'), ('description', 'Moral allegory and spiritual autobiography, The Little Prince is the most translated book in the French language. With a timeless charm it tells the story of a little boy who leaves the safety of his own tiny planet to travel the universe, learning the vagaries of adult behaviour through a series of extraordinary encounters. His personal odyssey culminates in a voyage to Earth and further adventures.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1020792'), ('name', 'Antoine de Saint-Exupéry'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330853515p5/1020792.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330853515p2/1020792.jpg')])), ('link', 'https://www.goodreads.com/author/show/1020792.Antoine_de_Saint_Exup_ry'), ('average_rating', '4.30'), ('ratings_count', '1340154'), ('text_reviews_count', '40855')]))])), ('published', '2000'), ('work', OrderedDict([('id', '2180358'), ('uri', 'kca://work/amzn1.gr.work.v1.F958pAbwgIwD68AA4MkC3A')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1162543')])), ('isbn', '031606792X'), ('isbn13', '9780316067928'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '43741')])), ('uri', 'kca://book/amzn1.gr.book.v1.IbwK04dpXq1GUVbwYB4SNQ'), ('title', 'Breaking Dawn (Twilight, #4)'), ('title_without_series', 'Breaking Dawn'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039438l/1162543._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039438l/1162543._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1162543.Breaking_Dawn'), ('num_pages', '756'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '2'), ('publication_year', '2008'), ('publication_month', '8'), ('average_rating', '3.69'), ('ratings_count', '1292116'), ('description', '&lt;b&gt;"Don\'t be afraid," I murmured. "We belong together."&lt;br /&gt;I was abruptly overwhelmed by the truth of my own words. &lt;br /&gt;This moment was so perfect, so right, there was no way to doubt it.&lt;br /&gt;His arms wrapped around me,&lt;br /&gt;holding me against him....&lt;br /&gt;It felt like every nerve ending in my body was a live wire.&lt;br /&gt;"Forever," he agreed.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;WHEN YOU LOVED THE ONE WHO WAS KILLING YOU, IT LEFT YOU NO OPTIONS. How could you run, how could you fight, when doing so would hurt that beloved one? If your life was all you had to give, how could you not give it? If it was someone you truly loved?&lt;br /&gt;&lt;br /&gt;TO BE IRREVOCABLY IN LOVE WITH A VAMPIRE is both fantasy and nightmare woven into a dangerously heightened reality for Bella Swan. Pulled in one direction by her intense passion for Edward Cullen, and in another by her profound connection to werewolf Jacob Black, a tumultuous year of temptation, loss, and strife have led her to the ultimate turning point. Her imminent choice to either join the dark but seductive world of immortals or to pursue a fully human life has become the thread from which the fates of two tribes hangs.&lt;br /&gt;&lt;br /&gt;NOW THAT BELLA HAS MADE HER DECISION, a startling chain of unprecedented events is about to unfold with potentially devastating, and unfathomable, consequences. Just when the frayed strands of Bella\'s life - first discovered in &lt;i&gt;Twilight&lt;/i&gt;, then scattered and torn in &lt;i&gt;New Moon&lt;/i&gt; and &lt;i&gt;Eclipse&lt;/i&gt; - seem ready to heal and knit together, could they be destroyed... forever?&lt;br /&gt;&lt;br /&gt;THE ASTONISHING, BREATHLESSLY anticipated conclusion to the Twilight Saga, &lt;i&gt;Breaking Dawn&lt;/i&gt; illuminates the secrets and mysteries of this spellbinding romantic epic that has entranced millions.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10570758'), ('text_reviews_count', '318064')]))])), ('published', '2008'), ('work', OrderedDict([('id', '2960529'), ('uri', 'kca://work/amzn1.gr.work.v1.xP6iGogq7HD98dx88kJDog')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '428263')])), ('isbn', '0316160202'), ('isbn13', '9780316160209'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '34173')])), ('uri', 'kca://book/amzn1.gr.book.v1.pz8Z_QjrdiX_lE1SPb4VKQ'), ('title', 'Eclipse (Twilight, #3)'), ('title_without_series', 'Eclipse'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361038355l/428263._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361038355l/428263._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/428263.Eclipse'), ('num_pages', '629'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '7'), ('publication_year', '2007'), ('publication_month', '8'), ('average_rating', '3.69'), ('ratings_count', '1390153'), ('description', '&lt;b&gt;"BELLA?"&lt;br /&gt;Edward\'s soft voice came from behind me. I turned to see him spring lightly up the porch steps, his hair windblown from running. He pulled me into his arms at once, just like he had in the parking lot, and kissed me again.&lt;br /&gt;This kiss frightened me. There was too much tension, too strong an edge to the way his lips crushed mine - like he was afraid we had only so much time left to us.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;As Seattle is ravaged by a string of mysterious killings and a malicious vampire continues her quest for revenge, Bella once again finds herself surrounded by danger. In the midst of it all, she is forced to choose between her love for Edward and her friendship with Jacob - knowing that her decision has the potential to ignite the ageless struggle between vampire and werewolf. With her graduation quickly approaching, Bella has one more decision to make: life or death. But which is which?&lt;br /&gt;&lt;br /&gt;READERS CAPTIVATED BY &lt;i&gt;Twilight&lt;/i&gt; AND &lt;i&gt;New Moon&lt;/i&gt; will eagerly devour &lt;i&gt;Eclipse&lt;/i&gt;, the much-anticipated third book in Stephenie Meyer\'s riveting vampire love saga.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10570758'), ('text_reviews_count', '318064')]))])), ('published', '2007'), ('work', OrderedDict([('id', '2675454'), ('uri', 'kca://work/amzn1.gr.work.v1.IwzpEvvlhAc8tuScGbwg8g')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '49041')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '42817')])), ('uri', 'kca://book/amzn1.gr.book.v1.g1Os7AXGqAOo89211CQ8sQ'), ('title', 'New Moon (Twilight, #2)'), ('title_without_series', 'New Moon'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039440l/49041._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039440l/49041._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/49041.New_Moon'), ('num_pages', '563'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '6'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '3.53'), ('ratings_count', '1428488'), ('description', '&lt;i&gt;There is an alternate cover edition for ISBN13 9780316160193 &lt;a href="https://www.goodreads.com/book/show/22857914" rel="nofollow"&gt;here&lt;/a&gt;.&lt;/i&gt; &lt;br /&gt;&lt;br /&gt;&lt;b&gt;I knew we were both in mortal danger. Still, in that instant, I felt &lt;i&gt;well&lt;/i&gt;. Whole. I could feel my heart racing in my chest, the blood pulsing hot and fast through my veins again. My lungs filled deep with the sweet scent that came off his skin. It was like there had never been any hole in my chest. I was perfect - not healed, but as if there had never been a wound in the first place. &lt;/b&gt;&lt;br /&gt;&lt;br /&gt;I FELT LIKE I WAS TRAPPED IN ONE OF THOSE TERRIFYING NIGHTMARES, the one where you have to run, run till your lungs burst, but you can\'t make your body move fast enough.... But this was no dream, and, unlike the nightmare, I wasn\'t running for my life; I was racing to save something infinitely more precious. My own life meant little to me today. &lt;br /&gt;&lt;br /&gt;FOR BELLA SWAN THERE IS ONE THING more important than life itself: Edward Cullen. But being in love with a vampire is even more dangerous than Bella could ever have imagined. Edward has already rescued Bella from the clutches of one evil vampire, but now, as their daring relationship threatens all that is near and dear to them, they realize their troubles may be just beginning....&lt;br /&gt;&lt;br /&gt;LEGIONS OF READERS ENTRANCED BY THE &lt;i&gt;New York Times&lt;/i&gt; bestseller &lt;i&gt;Twilight&lt;/i&gt; are hungry for the continuing story of star-crossed lovers Bell and Edward. In &lt;i&gt;New Moon&lt;/i&gt;, Stephanie Meyer delivers another irresistible combination of romance and suspense with a supernatural spin. passionate, riveting, and full of surprising twists and turns, this vampire love saga is well on its way to literary immortality.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10570758'), ('text_reviews_count', '318064')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3203964'), ('uri', 'kca://work/amzn1.gr.work.v1.1fzgJvmQrkvntdirmyYMoA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '41865')])), ('isbn', '0316015849'), ('isbn13', '9780316015844'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '96394')])), ('uri', 'kca://book/amzn1.gr.book.v1.v0ZqZFRkizei9mByA-3BpA'), ('title', 'Twilight (Twilight, #1)'), ('title_without_series', 'Twilight'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039443l/41865._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039443l/41865._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/41865.Twilight'), ('num_pages', '501'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Little, Brown and Company'), ('publication_day', '6'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '3.60'), ('ratings_count', '4850977'), ('description', "About three things I was absolutely positive.&lt;br /&gt;&lt;br /&gt;First, Edward was a vampire.&lt;br /&gt;&lt;br /&gt;Second, there was a part of him—and I didn't know how dominant that part might be—that thirsted for my blood.&lt;br /&gt;&lt;br /&gt;And third, I was unconditionally and irrevocably in love with him.&lt;br /&gt;&lt;br /&gt;Deeply seductive and extraordinarily suspenseful, Twilight is a love story with bite."), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10570758'), ('text_reviews_count', '318064')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3212258'), ('uri', 'kca://work/amzn1.gr.work.v1.f8lFp92oAIBHtSmSo4txRg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '138134')])), ('isbn', '0679601082'), ('isbn13', '9780679601081'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '197')])), ('uri', 'kca://book/amzn1.gr.book.v1.jHhIqJDxfidTucKwK0_KDA'), ('title', 'The Complete Poems'), ('title_without_series', 'The Complete Poems'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/138134.The_Complete_Poems'), ('num_pages', '416'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Modern Library'), ('publication_day', '26'), ('publication_year', '1994'), ('publication_month', '4'), ('average_rating', '4.25'), ('ratings_count', '21054'), ('description', None), ('authors', OrderedDict([('author', OrderedDict([('id', '11978'), ('name', 'John Keats'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198548090p5/11978.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198548090p2/11978.jpg')])), ('link', 'https://www.goodreads.com/author/show/11978.John_Keats'), ('average_rating', '4.18'), ('ratings_count', '52315'), ('text_reviews_count', '2253')]))])), ('published', '1994'), ('work', OrderedDict([('id', '1701632'), ('uri', 'kca://work/amzn1.gr.work.v1.-Q9Xhp8Zo5zxZHg4prI2AQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '890')])), ('isbn', '0142000671'), ('isbn13', '9780142000670'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '26400')])), ('uri', 'kca://book/amzn1.gr.book.v1.qtwvMU3sqr2Wph0NOU770w'), ('title', 'Of Mice and Men'), ('title_without_series', 'Of Mice and Men'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1511302904l/890._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1511302904l/890._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/890.Of_Mice_and_Men'), ('num_pages', '103'), ('format', 'Paperback'), ('edition_information', 'Steinbeck Centennial Edition, US / CAN Edition'), ('publisher', 'Penguin Books'), ('publication_day', '8'), ('publication_year', '2002'), ('publication_month', '1'), ('average_rating', '3.88'), ('ratings_count', '1904183'), ('description', 'The compelling story of two outsiders striving to find their place in an unforgiving world. &lt;br /&gt;&lt;br /&gt;Drifters in search of work, George and his simple-minded friend Lennie have nothing in the world except each other and a dream -- a dream that one day they will have some land of their own. Eventually they find work on a ranch in California’s Salinas Valley, but their hopes are doomed as Lennie, struggling against extreme cruelty, misunderstanding and feelings of jealousy, becomes a victim of his own strength. &lt;br /&gt;&lt;br /&gt;Tackling universal themes such as the friendship of a shared vision, and giving voice to America’s lonely and dispossessed, &lt;i&gt;Of Mice and Men&lt;/i&gt; has proved one of Steinbeck’s most popular works, achieving success as a novel, a Broadway play and three acclaimed films.'), ('authors', OrderedDict([('author', OrderedDict([('id', '585'), ('name', 'John Steinbeck'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1182118389p5/585.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1182118389p2/585.jpg')])), ('link', 'https://www.goodreads.com/author/show/585.John_Steinbeck'), ('average_rating', '3.94'), ('ratings_count', '3680388'), ('text_reviews_count', '103354')]))])), ('published', '2002'), ('work', OrderedDict([('id', '40283'), ('uri', 'kca://work/amzn1.gr.work.v1.eBaTt5IH0gu2aaYbJLCgog')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '35031085')])), ('isbn', '0143131842'), ('isbn13', '9780143131847'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5370')])), ('uri', 'kca://book/amzn1.gr.book.v1.21GvfWvotjWsRqb6TzH_Vw'), ('title', 'Frankenstein: The 1818 Text'), ('title_without_series', 'Frankenstein: The 1818 Text'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1498841231l/35031085._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1498841231l/35031085._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/35031085-frankenstein'), ('num_pages', '288'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Penguin Classics'), ('publication_day', '8'), ('publication_year', '2018'), ('publication_month', '3'), ('average_rating', '3.80'), ('ratings_count', '1135268'), ('description', "Mary Shelley's seminal novel of the scientist whose creation becomes a monster&lt;br /&gt;&lt;br /&gt;This edition is the original 1818 text, which preserves the hard-hitting and politically charged aspects of Shelley's original writing, as well as her unflinching wit and strong female voice. This edition also includes a new introduction and suggestions for further reading by author and Shelley expert Charlotte Gordon, literary excerpts and reviews selected by Gordon and a chronology and essay by preeminent Shelley scholar Charles E. Robinson."), ('authors', OrderedDict([('author', OrderedDict([('id', '11139'), ('name', 'Mary Wollstonecraft Shelley'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588859766p5/11139.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588859766p2/11139.jpg')])), ('link', 'https://www.goodreads.com/author/show/11139.Mary_Wollstonecraft_Shelley'), ('average_rating', '3.80'), ('ratings_count', '1169111'), ('text_reviews_count', '34707')]))])), ('published', '2018'), ('work', OrderedDict([('id', '4836639'), ('uri', 'kca://work/amzn1.gr.work.v1.HYrCHs2hgbojzi9917_vCg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '136251')])), ('isbn', '0545010225'), ('isbn13', '9780545010221'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '53112')])), ('uri', 'kca://book/amzn1.gr.book.v1.J45EZhldLHRv1GBWdMc7Uw'), ('title', 'Harry Potter and the Deathly Hallows (Harry Potter, #7)'), ('title_without_series', 'Harry Potter and the Deathly Hallows'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474171184l/136251._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474171184l/136251._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/136251.Harry_Potter_and_the_Deathly_Hallows'), ('num_pages', '759'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Arthur A. Levine Books / Scholastic Inc.'), ('publication_day', '21'), ('publication_year', '2007'), ('publication_month', '7'), ('average_rating', '4.62'), ('ratings_count', '2732395'), ('description', 'Harry Potter is leaving Privet Drive for the last time. But as he climbs into the sidecar of Hagrid’s motorbike and they take to the skies, he knows Lord Voldemort and the Death Eaters will not be far behind.&lt;br /&gt;&lt;br /&gt;The protective charm that has kept him safe until now is broken. But the Dark Lord is breathing fear into everything he loves. And he knows he can’t keep hiding.&lt;br /&gt;&lt;br /&gt;To stop Voldemort, Harry knows he must find the remaining Horcruxes and destroy them.&lt;br /&gt;&lt;br /&gt;He will have to face his enemy in one final battle.&lt;br /&gt;--jkrowling.com'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2007'), ('work', OrderedDict([('id', '2963218'), ('uri', 'kca://work/amzn1.gr.work.v1.Adr1zpcHTPWrbOovOdZhlA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '29126')])), ('uri', 'kca://book/amzn1.gr.book.v1.L9KPn9NQyHxsNneS-mDWAg'), ('title', 'Harry Potter and the Half-Blood Prince (Harry Potter, #6)'), ('title_without_series', 'Harry Potter and the Half-Blood Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1587697303l/1._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1587697303l/1._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1.Harry_Potter_and_the_Half_Blood_Prince'), ('num_pages', '652'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic Inc.'), ('publication_day', '16'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '4.57'), ('ratings_count', '2370671'), ('description', "The war against Voldemort is not going well; even Muggle governments are noticing. Ron scans the obituary pages of the &lt;i&gt;Daily Prophet&lt;/i&gt;, looking for familiar names. Dumbledore is absent from Hogwarts for long stretches of time, and the Order of the Phoenix has already suffered losses.&lt;br /&gt;&lt;br /&gt;And yet . . .&lt;br /&gt;&lt;br /&gt;As in all wars, life goes on. The Weasley twins expand their business. Sixth-year students learn to Apparate - and lose a few eyebrows in the process. Teenagers flirt and fight and fall in love. Classes are never straightforward, through Harry receives some extraordinary help from the mysterious Half-Blood Prince.&lt;br /&gt;&lt;br /&gt;So it's the home front that takes center stage in the multilayered sixth installment of the story of Harry Potter. Here at Hogwarts, Harry will search for the full and complete story of the boy who became Lord Voldemort - and thereby find what may be his only vulnerability."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2006'), ('work', OrderedDict([('id', '41335427'), ('uri', 'kca://work/amzn1.gr.work.v1.txipecnIYua0HbI4GhIAkA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2')])), ('isbn', '0439358078'), ('isbn13', '9780439358071'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '31059')])), ('uri', 'kca://book/amzn1.gr.book.v1.uGB1cTbG_Dm5BpjL_i7pqw'), ('title', 'Harry Potter and the Order of the Phoenix (Harry Potter, #5)'), ('title_without_series', 'Harry Potter and the Order of the Phoenix'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1546910265l/2._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1546910265l/2._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2.Harry_Potter_and_the_Order_of_the_Phoenix'), ('num_pages', '870'), ('format', 'Paperback'), ('edition_information', 'US Edition'), ('publisher', 'Scholastic Inc.'), ('publication_day', None), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '4.50'), ('ratings_count', '2436978'), ('description', 'There is a door at the end of a silent corridor. And it’s haunting Harry Pottter’s dreams. Why else would he be waking in the middle of the night, screaming in terror?&lt;br /&gt;&lt;br /&gt;Harry has a lot on his mind for this, his fifth year at Hogwarts: a Defense Against the Dark Arts teacher with a personality like poisoned honey; a big surprise on the Gryffindor Quidditch team; and the looming terror of the Ordinary Wizarding Level exams. But all these things pale next to the growing threat of He-Who-Must-Not-Be-Named - a threat that neither the magical government nor the authorities at Hogwarts can stop.&lt;br /&gt;&lt;br /&gt;As the grasp of darkness tightens, Harry must discover the true depth and strength of his friends, the importance of boundless loyalty, and the shocking price of unbearable sacrifice.&lt;br /&gt;&lt;br /&gt;His fate depends on them all.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2809203'), ('uri', 'kca://work/amzn1.gr.work.v1.QBlq2dw4tPMZSuXhlMeXww')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '33360')])), ('uri', 'kca://book/amzn1.gr.book.v1.Qtinlqa0DGyf_iLtfFVrCQ'), ('title', 'Harry Potter and the Goblet of Fire (Harry Potter, #4)'), ('title_without_series', 'Harry Potter and the Goblet of Fire'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1554006152l/6._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1554006152l/6._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6.Harry_Potter_and_the_Goblet_of_Fire'), ('num_pages', '734'), ('format', 'Paperback'), ('edition_information', 'First Scholastic Trade Paperback Edition'), ('publisher', 'Scholastic'), ('publication_day', '28'), ('publication_year', '2002'), ('publication_month', '9'), ('average_rating', '4.56'), ('ratings_count', '2518274'), ('description', "Harry Potter is midway through his training as a wizard and his coming of age. Harry wants to get away from the pernicious Dursleys and go to the International Quidditch Cup with Hermione, Ron, and the Weasleys. He wants to dream about Cho Chang, his crush (and maybe do more than dream). He wants to find out about the mysterious event that's supposed to take place at Hogwarts this year, an event involving two other rival schools of magic, and a competition that hasn't happened for hundreds of years. He wants to be a normal, fourteen-year-old wizard. But unfortunately for Harry Potter, he's not normal - even by wizarding standards.&lt;br /&gt;&lt;br /&gt;And in his case, different can be deadly."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2002'), ('work', OrderedDict([('id', '3046572'), ('uri', 'kca://work/amzn1.gr.work.v1.USb5ObBtcLXUuC3i9aoelA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '15881')])), ('isbn', '0439064864'), ('isbn13', '9780439064866'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '36950')])), ('uri', 'kca://book/amzn1.gr.book.v1.KlY-hIN06yK2_7Y8_mQVig'), ('title', 'Harry Potter and the Chamber of Secrets (Harry Potter, #2)'), ('title_without_series', 'Harry Potter and the Chamber of Secrets'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474169725l/15881._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474169725l/15881._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/15881.Harry_Potter_and_the_Chamber_of_Secrets'), ('num_pages', '341'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Arthur A. Levine Books / Scholastic Inc.'), ('publication_day', '2'), ('publication_year', '1999'), ('publication_month', '6'), ('average_rating', '4.43'), ('ratings_count', '2641930'), ('description', 'Ever since Harry Potter had come home for the summer, the Dursleys had been so mean and hideous that all Harry wanted was to get back to the Hogwarts School for Witchcraft and Wizardry. But just as he’s packing his bags, Harry receives a warning from a strange impish creature who says that if Harry returns to Hogwarts, disaster will strike.&lt;br /&gt;&lt;br /&gt;And strike it does. For in Harry’s second year at Hogwarts, fresh torments and horrors arise, including an outrageously stuck-up new professor and a spirit who haunts the girls’ bathroom. But then the real trouble begins – someone is turning Hogwarts students to stone. Could it be Draco Malfoy, a more poisonous rival than ever? Could it possible be Hagrid, whose mysterious past is finally told? Or could it be the one everyone at Hogwarts most suspects… Harry Potter himself!'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '1999'), ('work', OrderedDict([('id', '6231171'), ('uri', 'kca://work/amzn1.gr.work.v1.PjwTgn-_w5b0mY40RgNxdw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '5')])), ('isbn', '043965548X'), ('isbn13', '9780439655484'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '38657')])), ('uri', 'kca://book/amzn1.gr.book.v1.om7j-Dd6wInrhO7TVy51Ow'), ('title', 'Harry Potter and the Prisoner of Azkaban (Harry Potter, #3)'), ('title_without_series', 'Harry Potter and the Prisoner of Azkaban'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1499277281l/5._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1499277281l/5._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/5.Harry_Potter_and_the_Prisoner_of_Azkaban'), ('num_pages', '435'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Scholastic Inc.'), ('publication_day', '1'), ('publication_year', '2004'), ('publication_month', '5'), ('average_rating', '4.57'), ('ratings_count', '2714006'), ('description', "Harry Potter's third year at Hogwarts is full of new dangers. A convicted murderer, Sirius Black, has broken out of Azkaban prison, and it seems he's after Harry. Now Hogwarts is being patrolled by the dementors, the Azkaban guards who are hunting Sirius. But Harry can't imagine that Sirius or, for that matter, the evil Lord Voldemort could be more frightening than the dementors themselves, who have the terrible power to fill anyone they come across with aching loneliness and despair. Meanwhile, life continues as usual at Hogwarts. A top-of-the-line broom takes Harry's success at Quidditch, the sport of the Wizarding world, to new heights. A cute fourth-year student catches his eye. And he becomes close with the new Defense of the Dark Arts teacher, who was a childhood friend of his father. Yet despite the relative safety of life at Hogwarts and the best efforts of the dementors, the threat of Sirius Black grows ever closer. But if Harry has learned anything from his education in wizardry, it is that things are often not what they seem. Tragic revelations, heartwarming surprises, and high-stakes magical adventures await the boy wizard in this funny and poignant third installment of the beloved series.&lt;br /&gt;--scholastic.com"), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2402163'), ('uri', 'kca://work/amzn1.gr.work.v1.ZkLfli5sQE5ax3qSa7235Q')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '3')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '78752')])), ('uri', 'kca://book/amzn1.gr.book.v1.tJT_00n8UPpvWa-zWHEAXg'), ('title', "Harry Potter and the Sorcerer's Stone (Harry Potter, #1)"), ('title_without_series', "Harry Potter and the Sorcerer's Stone"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474154022l/3._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474154022l/3._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/3.Harry_Potter_and_the_Sorcerer_s_Stone'), ('num_pages', '309'), ('format', 'Hardcover'), ('edition_information', 'Library Edition'), ('publisher', 'Scholastic Inc'), ('publication_day', '1'), ('publication_year', '2003'), ('publication_month', '11'), ('average_rating', '4.47'), ('ratings_count', '6831567'), ('description', "Alternate cover edition of ISBN 9780439554930&lt;br /&gt;&lt;br /&gt;Harry Potter's life is miserable. His parents are dead and he's stuck with his heartless relatives, who force him to live in a tiny closet under the stairs. But his fortune changes when he receives a letter that tells him the truth about himself: he's a wizard. A mysterious visitor rescues him from his relatives and takes him to his new home, Hogwarts School of Witchcraft and Wizardry.&lt;br /&gt;&lt;br /&gt;After a lifetime of bottling up his magical powers, Harry finally feels like a normal kid. But even within the Wizarding community, he is special. He is the boy who lived: the only person to have ever survived a killing curse inflicted by the evil Lord Voldemort, who launched a brutal takeover of the Wizarding world, only to vanish after failing to kill Harry.&lt;br /&gt;&lt;br /&gt;Though Harry's first year at Hogwarts is the best of his life, not everything is perfect. There is a dangerous secret object hidden within the castle walls, and Harry believes it's his responsibility to prevent it from falling into evil hands. But doing so will bring him into contact with forces more terrifying than he ever could have imagined.&lt;br /&gt;&lt;br /&gt;Full of sympathetic characters, wildly imaginative situations, and countless exciting details, the first installment in the series assembles an unforgettable magical world and sets the stage for many high-stakes adventures to come."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '24986400'), ('text_reviews_count', '573700')]))])), ('published', '2003'), ('work', OrderedDict([('id', '4640799'), ('uri', 'kca://work/amzn1.gr.work.v1.TbpxJa2CwiSSz_9W2FruoA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40940121')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1384')])), ('uri', 'kca://book/amzn1.gr.book.v1.itZyR1Fk_Ix0XJXvaEPHLg'), ('title', 'Bridge to Terabithia'), ('title_without_series', 'Bridge to Terabithia'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532478367l/40940121._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532478367l/40940121._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40940121-bridge-to-terabithia'), ('num_pages', '190'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'HarperCollins'), ('publication_day', '6'), ('publication_year', '2009'), ('publication_month', '10'), ('average_rating', '4.01'), ('ratings_count', '433647'), ('description', "Jess Aarons' greatest ambition is to be the fastest runner in his grade. He's been practicing all summer and can't wait to see his classmates' faces when he beats them all. But on the first day of school, a new girl boldly crosses over to the boys' side and outruns everyone.&lt;br /&gt;&lt;br /&gt;That's not a very promising beginning for a friendship, but Jess and Leslie Burke become inseparable. Together they create Terabithia, a magical kingdom in the woods where the two of them reign as king and queen, and their imaginations set the only limits."), ('authors', OrderedDict([('author', OrderedDict([('id', '1949'), ('name', 'Katherine Paterson'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/1949.Katherine_Paterson'), ('average_rating', '3.97'), ('ratings_count', '512809'), ('text_reviews_count', '19140')]))])), ('published', '2009'), ('work', OrderedDict([('id', '2237401'), ('uri', 'kca://work/amzn1.gr.work.v1.zzEPgoJCNWRJZ6AuRm8EeQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17158513')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2262')])), ('uri', 'kca://book/amzn1.gr.book.v1.TcadId_zixkpux9JQfySwA'), ('title', 'Captive Prince: Volume Two (Captive Prince, #2)'), ('title_without_series', 'Captive Prince: Volume Two'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356027904l/17158513._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356027904l/17158513._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17158513-captive-prince'), ('num_pages', '216'), ('format', 'ebook'), ('edition_information', None), ('publisher', None), ('publication_day', None), ('publication_year', '2012'), ('publication_month', None), ('average_rating', '4.43'), ('ratings_count', '38912'), ('description', 'With their countries on the brink of war, Damen and his new master, Prince Laurent, must exchange the intrigues of the palace for the sweeping might of the battlefield as they travel to the border to avert a lethal plot.&lt;br /&gt;&lt;br /&gt;Forced to hide his identity, Damen finds himself increasingly drawn to the dangerous, charismatic Laurent. But as the fledgling trust between the two men deepens, the truth of secrets from both their pasts is poised to deal them the crowning death blow . . .'), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '191848'), ('text_reviews_count', '25580')]))])), ('published', '2012'), ('work', OrderedDict([('id', '23581952'), ('uri', 'kca://work/amzn1.gr.work.v1.aY-h5auqNU0sOr_bcd1WSw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17158532')])), ('isbn', '174348495X'), ('isbn13', '9781743484951'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3164')])), ('uri', 'kca://book/amzn1.gr.book.v1.tzJZCfUkGUT1Wy3DGs6PqA'), ('title', 'Kings Rising (Captive Prince, #3)'), ('title_without_series', 'Kings Rising'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1454160767l/17158532._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1454160767l/17158532._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17158532-kings-rising'), ('num_pages', '385'), ('format', 'ebook'), ('edition_information', None), ('publisher', 'Penguin Group Australia'), ('publication_day', '2'), ('publication_year', '2016'), ('publication_month', '2'), ('average_rating', '4.46'), ('ratings_count', '33408'), ('description', "&lt;i&gt;Damianos of Akielos has returned&lt;/i&gt;.&lt;br /&gt; &lt;br /&gt;His identity now revealed, Damen must face his master Prince Laurent as Damianos of Akielos, the man Laurent has sworn to kill.&lt;br /&gt; &lt;br /&gt;On the brink of a momentous battle, the future of both their countries hangs in the balance. In the south, Kastor’s forces are massing. In the north, the Regent’s armies are mobilising for war. Damen’s only hope of reclaiming his throne is to fight together with Laurent against their usurpers.&lt;br /&gt; &lt;br /&gt;Forced into an uneasy alliance the two princes journey deep into Akielos, where they face their most dangerous opposition yet. But even if the fragile trust they have built survives the revelation of Damen’s identity—can it stand against the Regent's final, deadly play for the throne?"), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '191848'), ('text_reviews_count', '25580')]))])), ('published', '2016'), ('work', OrderedDict([('id', '23581990'), ('uri', 'kca://work/amzn1.gr.work.v1.-_QRlY1zWL90hb8zqfcwlg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1618')])), ('isbn', '1400032717'), ('isbn13', '9781400032716'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '36400')])), ('uri', 'kca://book/amzn1.gr.book.v1.-HbDY4-Aoh2zmGKIXjEwKg'), ('title', 'The Curious Incident of the Dog in the Night-Time'), ('title_without_series', 'The Curious Incident of the Dog in the Night-Time'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1479863624l/1618._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1479863624l/1618._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1618.The_Curious_Incident_of_the_Dog_in_the_Night_Time'), ('num_pages', '226'), ('format', 'Paperback'), ('edition_information', 'Vintage Contemporaries'), ('publisher', 'Vintage'), ('publication_day', '18'), ('publication_year', '2004'), ('publication_month', '5'), ('average_rating', '3.88'), ('ratings_count', '1166455'), ('description', "Christopher John Francis Boone knows all the countries of the world and their capitals and every prime number up to 7,057. He relates well to animals but has no understanding of human emotions. He cannot stand to be touched. And he detests the color yellow.&lt;br /&gt;&lt;br /&gt;Although gifted with a superbly logical brain, for fifteen-year-old Christopher everyday interactions and admonishments have little meaning. He lives on patterns, rules, and a diagram kept in his pocket. Then one day, a neighbor's dog, Wellington, is killed and his carefully constructive universe is threatened. Christopher sets out to solve the murder in the style of his favourite (logical) detective, Sherlock Holmes. What follows makes for a novel that is funny, poignant and fascinating in its portrayal of a person whose curse and blessing are a mind that perceives the world entirely literally."), ('authors', OrderedDict([('author', OrderedDict([('id', '1050'), ('name', 'Mark Haddon'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1337988298p5/1050.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1337988298p2/1050.jpg')])), ('link', 'https://www.goodreads.com/author/show/1050.Mark_Haddon'), ('average_rating', '3.86'), ('ratings_count', '1229619'), ('text_reviews_count', '51460')]))])), ('published', '2004'), ('work', OrderedDict([('id', '4259809'), ('uri', 'kca://work/amzn1.gr.work.v1.8XQyL2-mXgV1VRh3euWYmw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '7260188')])), ('isbn', '0439023513'), ('isbn13', '9780439023511'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '91606')])), ('uri', 'kca://book/amzn1.gr.book.v1.hFVPFpO-8DyF11Gy1k4d7A'), ('title', 'Mockingjay (The Hunger Games, #3)'), ('title_without_series', 'Mockingjay'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722918l/7260188._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722918l/7260188._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/7260188-mockingjay'), ('num_pages', '390'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '24'), ('publication_year', '2010'), ('publication_month', '8'), ('average_rating', '4.04'), ('ratings_count', '2286580'), ('description', "The final book in the ground-breaking HUNGER GAMES trilogy, this new foiled edition of MOCKINGJAY is available for a limited period of time. Against all odds, Katniss Everdeen has survived the Hunger Games twice. But now that she's made it out of the bloody arena alive, she's still not safe. The Capitol is angry. The Capitol wants revenge. Who do they think should pay for the unrest? Katniss. And what's worse, President Snow has made it clear that no one else is safe either. Not Katniss's family, not her friends, not the people of District 12."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11504417'), ('text_reviews_count', '404612')]))])), ('published', '2010'), ('work', OrderedDict([('id', '8812783'), ('uri', 'kca://work/amzn1.gr.work.v1.4IASwwiLmBwCmDcIe56XuQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6148028')])), ('isbn', '0439023491'), ('isbn13', '9780439023498'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '85541')])), ('uri', 'kca://book/amzn1.gr.book.v1.c5JlFHJrTIJY5yfmJN8b0w'), ('title', 'Catching Fire (The Hunger Games, #2)'), ('title_without_series', 'Catching Fire'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722941l/6148028._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722941l/6148028._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6148028-catching-fire'), ('num_pages', '391'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '1'), ('publication_year', '2009'), ('publication_month', '9'), ('average_rating', '4.29'), ('ratings_count', '2440550'), ('description', "&lt;b&gt;SPARKS ARE IGNITING.&lt;br /&gt;FLAMES ARE SPREADING.&lt;br /&gt;AND THE CAPITAL WANTS REVENGE.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;Against all odds, Katniss Everdeen has survived the Hunger Games. She and fellow District 12 tribute Peeta Mellark are miraculously still alive. Katniss should be relieved, happy even. Yet nothing is the way Katniss wishes it to be. Gale holds her at an icy distance. Peeta has turned his back on her completely. And there are whispers of a rebellion against the Capitol - a rebellion that Katniss and Peeta may have helped create.&lt;br /&gt;&lt;br /&gt;Much to her shock, Katniss has fueled an unrest that she's afraid she cannot stop. And what scares her even more is that she's not entirely convinced she should try. As time draws near for Katniss and Peeta to visit the districts on the Capitol's cruel Victory Tour, the stakes are higher than ever. If they can't prove, without a shadow of a doubt, that they are lost in their love for each other, the consequences will be horrifying. Katniss is about to be tested as never before."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11504417'), ('text_reviews_count', '404612')]))])), ('published', '2009'), ('work', OrderedDict([('id', '6171458'), ('uri', 'kca://work/amzn1.gr.work.v1.2o2efDDMSYr-E3ruRr1VcA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2767052')])), ('isbn', '0439023483'), ('isbn13', '9780439023481'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '153595')])), ('uri', 'kca://book/amzn1.gr.book.v1.YaoKZD8xVx72w5T1ZgR1YQ'), ('title', 'The Hunger Games (The Hunger Games, #1)'), ('title_without_series', 'The Hunger Games'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722975l/2767052._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722975l/2767052._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2767052-the-hunger-games'), ('num_pages', '374'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '14'), ('publication_year', '2008'), ('publication_month', '9'), ('average_rating', '4.33'), ('ratings_count', '6237785'), ('description', "&lt;b&gt;WINNING MEANS FAME AND FORTUNE.&lt;br /&gt;LOSING MEANS CERTAIN DEATH.&lt;br /&gt;THE HUNGER GAMES HAVE BEGUN. . . .&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;In the ruins of a place once known as North America lies the nation of Panem, a shining Capitol surrounded by twelve outlying districts. The Capitol is harsh and cruel and keeps the districts in line by forcing them all to send one boy and once girl between the ages of twelve and eighteen to participate in the annual Hunger Games, a fight to the death on live TV.&lt;br /&gt;&lt;br /&gt;Sixteen-year-old Katniss Everdeen regards it as a death sentence when she steps forward to take her sister's place in the Games. But Katniss has been close to dead before—and survival, for her, is second nature. Without really meaning to, she becomes a contender. But if she is to win, she will have to start making choices that weight survival against humanity and life against love."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_200x266-3061b784cc8e7f021c6430c9aba94587.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/f_50x66-6a03a5c12233c941481992b82eea8d23.png')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11504417'), ('text_reviews_count', '404612')]))])), ('published', '2008'), ('work', OrderedDict([('id', '2792775'), ('uri', 'kca://work/amzn1.gr.work.v1.qDM8aVuWTQKRymQBUS02og')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '5659')])), ('isbn', '0143039091'), ('isbn13', '9780143039099'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3679')])), ('uri', 'kca://book/amzn1.gr.book.v1.Y6Tj1XDUHYcT9fle4yewtg'), ('title', 'The Wind in the Willows'), ('title_without_series', 'The Wind in the Willows'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423183570l/5659._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423183570l/5659._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/5659.The_Wind_in_the_Willows'), ('num_pages', '197'), ('format', 'Paperback'), ('edition_information', 'Penguin Classics'), ('publisher', 'Penguin Books'), ('publication_day', '27'), ('publication_year', '2005'), ('publication_month', '10'), ('average_rating', '3.99'), ('ratings_count', '173878'), ('description', '"There is nothing half so much worth doing as simply messing around in boats."&lt;br /&gt;&lt;br /&gt;When Mole flees his little underground home he discovers new friends and adventures with Raj, Toad and Badger.&lt;br /&gt;&lt;br /&gt;This much-loved story has been carefully retold for young children to enjoy. With beautiful illustrations throughout, it provides the perfect introduction to a classic tale.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3843'), ('name', 'Kenneth Grahame'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201018750p5/3843.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201018750p2/3843.jpg')])), ('link', 'https://www.goodreads.com/author/show/3843.Kenneth_Grahame'), ('average_rating', '3.99'), ('ratings_count', '185042'), ('text_reviews_count', '6779')]))])), ('published', '2005'), ('work', OrderedDict([('id', '1061285'), ('uri', 'kca://work/amzn1.gr.work.v1.yTxsyacrG8lEOhoyMEh2aw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1852')])), ('isbn', '0439227143'), ('isbn13', '9780439227148'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7853')])), ('uri', 'kca://book/amzn1.gr.book.v1.N3Hj-jJMvOmCMWeUygmRPw'), ('title', 'The Call of the Wild'), ('title_without_series', 'The Call of the Wild'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1452291694l/1852._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1452291694l/1852._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1852.The_Call_of_the_Wild'), ('num_pages', '172'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Scholastic'), ('publication_day', '1'), ('publication_year', '2001'), ('publication_month', '1'), ('average_rating', '3.87'), ('ratings_count', '331153'), ('description', "First published in 1903, &lt;i&gt;The Call of the Wild&lt;/i&gt; is regarded as Jack London's masterpiece. Based on London's experiences as a gold prospector in the Canadian wilderness and his ideas about nature and the struggle for existence, &lt;i&gt;The Call of the Wild&lt;/i&gt; is a tale about unbreakable spirit and the fight for survival in the frozen Alaskan Klondike."), ('authors', OrderedDict([('author', OrderedDict([('id', '1240'), ('name', 'Jack London'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1508674808p5/1240.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1508674808p2/1240.jpg')])), ('link', 'https://www.goodreads.com/author/show/1240.Jack_London'), ('average_rating', '3.96'), ('ratings_count', '734439'), ('text_reviews_count', '26289')]))])), ('published', '2001'), ('work', OrderedDict([('id', '3252320'), ('uri', 'kca://work/amzn1.gr.work.v1.nZyZdlJnNCISNRPQkGznZw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '295')])), ('isbn', '0753453800'), ('isbn13', '9780753453803'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7151')])), ('uri', 'kca://book/amzn1.gr.book.v1.NMDBN_fq2yR6xaC4HcPWOw'), ('title', 'Treasure Island'), ('title_without_series', 'Treasure Island'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485248909l/295._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485248909l/295._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/295.Treasure_Island'), ('num_pages', '311'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Kingfisher'), ('publication_day', '15'), ('publication_year', '2001'), ('publication_month', '9'), ('average_rating', '3.83'), ('ratings_count', '391347'), ('description', '"For sheer storytelling delight and pure adventure, &lt;i&gt;Treasure Island&lt;/i&gt; has never been surpassed. From the moment young Jim Hawkins first encounters the sinister Blind Pew at the Admiral Benbow Inn until the climactic battle for treasure on a tropic isle, the novel creates scenes and characters that have fired the imaginations of generations of readers. Written by a superb prose stylist, a master of both action and atmosphere, the story centers upon the conflict between good and evil - but in this case a particularly engaging form of evil. It is the villainy of that most ambiguous rogue Long John Silver that sets the tempo of this tale of treachery, greed, and daring. Designed to forever kindle a dream of high romance and distant horizons, &lt;i&gt;Treasure Island&lt;/i&gt; is, in the words of G. K. Chesterton, \'the realization of an ideal, that which is promised in its provocative and beckoning map; a vision not only of white skeletons but also green palm trees and sapphire seas.\' G. S. Fraser terms it \'an utterly original book\' and goes on to write: \'There will always be a place for stories like &lt;i&gt;Treasure Island&lt;/i&gt; that can keep boys and old men happy.\''), ('authors', OrderedDict([('author', OrderedDict([('id', '854076'), ('name', 'Robert Louis Stevenson'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192746024p5/854076.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192746024p2/854076.jpg')])), ('link', 'https://www.goodreads.com/author/show/854076.Robert_Louis_Stevenson'), ('average_rating', '3.85'), ('ratings_count', '1078987'), ('text_reviews_count', '35749')]))])), ('published', '2001'), ('work', OrderedDict([('id', '3077988'), ('uri', 'kca://work/amzn1.gr.work.v1.jmdkybKCkfrZq5SG8p4pNg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '236093')])), ('isbn', '0140621679'), ('isbn13', '9780140621679'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7632')])), ('uri', 'kca://book/amzn1.gr.book.v1.UivhNgteUMaLX0zsj4Y5Hw'), ('title', 'The Wonderful Wizard of Oz (Oz, #1)'), ('title_without_series', 'The Wonderful Wizard of Oz'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1398003737l/236093._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1398003737l/236093._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/236093.The_Wonderful_Wizard_of_Oz'), ('num_pages', '154'), ('format', 'Paperback'), ('edition_information', 'Penguin Popular Classics'), ('publisher', 'Penguin'), ('publication_day', None), ('publication_year', '1995'), ('publication_month', None), ('average_rating', '3.99'), ('ratings_count', '356870'), ('description', 'When Dorothy and her little dog Toto are caught in a tornado, they and their Kansas farmhouse are suddenly transported to Oz, where Munchkins live, monkeys fly and Wicked Witches rule. Desperate to return home, and with the Wicked Witch of the West on their trail, Dorothy and Toto - together with new friends the Tin Woodsman, Scarecrow and cowardly Lion - embark on a fantastic quest along the Yellow Brick Road in search of the Emerald City. There they hope to meet the legendary, all-powerful Wizard of Oz, who alone may hold the power to grant their every wish.&lt;br /&gt;&lt;br /&gt;Just as captivating as it was a hundred years ago, this is a story that all ages will love.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3242'), ('name', 'L. Frank Baum'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1383720421p5/3242.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1383720421p2/3242.jpg')])), ('link', 'https://www.goodreads.com/author/show/3242.L_Frank_Baum'), ('average_rating', '3.97'), ('ratings_count', '551785'), ('text_reviews_count', '22671')]))])), ('published', '1995'), ('work', OrderedDict([('id', '1993810'), ('uri', 'kca://work/amzn1.gr.work.v1.Brq5W1RwLwTS7yX4kPgQNQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '93')])), ('isbn', '0753454947'), ('isbn13', '9780753454947'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2386')])), ('uri', 'kca://book/amzn1.gr.book.v1.62w6yF6ljGRIHf98OEYAfQ'), ('title', 'Heidi (Heidi, #1-2)'), ('title_without_series', 'Heidi'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/93.Heidi'), ('num_pages', '352'), ('format', 'Paperback'), ('edition_information', 'Kingfisher Classics'), ('publisher', 'Kingfisher'), ('publication_day', '15'), ('publication_year', '2002'), ('publication_month', '11'), ('average_rating', '3.99'), ('ratings_count', '170004'), ('description', 'Little orphan Heidi goes to live high in the Alps with her gruff grandfather and brings happiness to all who know her on the mountain. When Heidi goes to Frankfurt to work in a wealthy household, she dreams of returning to the mountains and meadows, her friend Peter, and her beloved grandfather.'), ('authors', OrderedDict([('author', OrderedDict([('id', '49'), ('name', 'Johanna Spyri'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201029829p5/49.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201029829p2/49.jpg')])), ('link', 'https://www.goodreads.com/author/show/49.Johanna_Spyri'), ('average_rating', '4.00'), ('ratings_count', '186766'), ('text_reviews_count', '4407')]))])), ('published', '2002'), ('work', OrderedDict([('id', '1738595'), ('uri', 'kca://work/amzn1.gr.work.v1.vupk7zK34JDihBVCwsZlrw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '8127')])), ('isbn', '0451528824'), ('isbn13', '9780451528827'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '14917')])), ('uri', 'kca://book/amzn1.gr.book.v1.srpZjZlpcE9dl03dhQOy8w'), ('title', 'Anne of Green Gables (Anne of Green Gables, #1)'), ('title_without_series', 'Anne of Green Gables'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/8127.Anne_of_Green_Gables'), ('num_pages', '320'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Signet Book'), ('publication_day', '6'), ('publication_year', '2003'), ('publication_month', '5'), ('average_rating', '4.26'), ('ratings_count', '705055'), ('description', "As soon as Anne Shirley arrives at the snug white farmhouse called Green Gables, she is sure she wants to stay forever . . . but will the Cuthberts send her back to to the orphanage? Anne knows she's not what they expected—a skinny girl with fiery red hair and a temper to match. If only she can convince them to let her stay, she'll try very hard not to keep rushing headlong into scrapes and blurting out the first thing that comes to her mind. Anne is not like anyone else, the Cuthberts agree; she is special—a girl with an enormous imagination. This orphan girl dreams of the day when she can call herself Anne of Green Gables."), ('authors', OrderedDict([('author', OrderedDict([('id', '5350'), ('name', 'L.M. Montgomery'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1188896723p5/5350.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1188896723p2/5350.jpg')])), ('link', 'https://www.goodreads.com/author/show/5350.L_M_Montgomery'), ('average_rating', '4.22'), ('ratings_count', '1585830'), ('text_reviews_count', '55333')]))])), ('published', '2003'), ('work', OrderedDict([('id', '3464264'), ('uri', 'kca://work/amzn1.gr.work.v1.s7yrHLy8bDalH9w11O-zTQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1934')])), ('isbn', '0451529308'), ('isbn13', '9780451529305'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '20807')])), ('uri', 'kca://book/amzn1.gr.book.v1.AMKxo9pbFFRBV4qA6jnIYQ'), ('title', 'Little Women'), ('title_without_series', 'Little Women'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1562690475l/1934._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1562690475l/1934._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1934.Little_Women'), ('num_pages', '449'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Signet Classics'), ('publication_day', '6'), ('publication_year', '2004'), ('publication_month', '4'), ('average_rating', '4.08'), ('ratings_count', '1642213'), ('description', 'Generations of readers young and old, male and female, have fallen in love with the March sisters of Louisa May Alcott’s most popular and enduring novel, &lt;i&gt;Little Women&lt;/i&gt;. Here are talented tomboy and author-to-be Jo, tragically frail Beth, beautiful Meg, and romantic, spoiled Amy, united in their devotion to each other and their struggles to survive in New England during the Civil War.&lt;br /&gt;&lt;p&gt;It is no secret that Alcott based &lt;i&gt;Little Women&lt;/i&gt; on her own early life. While her father, the freethinking reformer and abolitionist Bronson Alcott, hobnobbed with such eminent male authors as Emerson, Thoreau, and Hawthorne, Louisa supported herself and her sisters with "woman’s work,” including sewing, doing laundry, and acting as a domestic servant. But she soon discovered she could make more money writing. &lt;i&gt;Little Women&lt;/i&gt; brought her lasting fame and fortune, and far from being the "girl’s book” her publisher requested, it explores such timeless themes as love and death, war and peace, the conflict between personal ambition and family responsibilities, and the clash of cultures between Europe and America.&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '1315'), ('name', 'Louisa May Alcott'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1200326665p5/1315.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1200326665p2/1315.jpg')])), ('link', 'https://www.goodreads.com/author/show/1315.Louisa_May_Alcott'), ('average_rating', '4.06'), ('ratings_count', '1899448'), ('text_reviews_count', '43180')]))])), ('published', '2004'), ('work', OrderedDict([('id', '3244642'), ('uri', 'kca://work/amzn1.gr.work.v1.d2eQgjlqgwEpanKeHkUAgw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '43822024')])), ('isbn', '1481497065'), ('isbn13', '9781481497060'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5668')])), ('uri', 'kca://book/amzn1.gr.book.v1.7OM3tkgHAmqpnWaIkl3PMA'), ('title', 'The Toll (Arc of a Scythe, #3)'), ('title_without_series', 'The Toll'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558117336l/43822024._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558117336l/43822024._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/43822024-the-toll'), ('num_pages', '625'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon &amp; Schuster Books for Young Readers'), ('publication_day', '5'), ('publication_year', '2019'), ('publication_month', '11'), ('average_rating', '4.27'), ('ratings_count', '35706'), ('description', 'It’s been three years since Rowan and Citra disappeared; since Scythe Goddard came into power; since the Thunderhead closed itself off to everyone but Grayson Tolliver.&lt;br /&gt;&lt;br /&gt;In this pulse-pounding conclusion to &lt;i&gt;New York Times &lt;/i&gt;bestselling author Neal Shusterman’s Arc of a Scythe trilogy, constitutions are tested and old friends are brought back from the dead.'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '676859'), ('text_reviews_count', '88669')]))])), ('published', '2019'), ('work', OrderedDict([('id', '59222476'), ('uri', 'kca://work/amzn1.gr.work.v1.pJ1XvuR9ZysrKirtcMVmFA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1696832')])), ('isbn', '1405450509'), ('isbn13', '9781405450508'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15')])), ('uri', 'kca://book/amzn1.gr.book.v1.64kJoRdr3znWUxZmSCO-Pg'), ('title', 'Beers of the World'), ('title_without_series', 'Beers of the World'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1696832.Beers_of_the_World'), ('num_pages', None), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Parragon Publishing'), ('publication_day', '1'), ('publication_year', '2005'), ('publication_month', '11'), ('average_rating', '3.63'), ('ratings_count', '102'), ('description', None), ('authors', OrderedDict([('author', OrderedDict([('id', '781570'), ('name', 'David Kenning'), ('role', 'Creator'), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/781570.David_Kenning'), ('average_rating', '3.55'), ('ratings_count', '121'), ('text_reviews_count', '20')]))])), ('published', '2005'), ('work', OrderedDict([('id', '1693795'), ('uri', 'kca://work/amzn1.gr.work.v1.CKgueeRMrVBTWuSsun1TyQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '45714170')])), ('isbn', '1406375500'), ('isbn13', '9781406375503'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '230')])), ('uri', 'kca://book/amzn1.gr.book.v1.SJ0DJBotk0KBV2R7Hodmvg'), ('title', 'Burn'), ('title_without_series', 'Burn'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1571075314l/45714170._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1571075314l/45714170._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/45714170-burn'), ('num_pages', '384'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Walker Books'), ('publication_day', '2'), ('publication_year', '2020'), ('publication_month', '6'), ('average_rating', '3.93'), ('ratings_count', '1723'), ('description', "In 1956 Sarah Dewhurst's father shocks her by hiring a dragon to work the farm. The dragon is a smaller blue rather than the traditional larger reds, though even the reds are now scarce. When the blue dragon, Kazimir, unexpectedly saves Sarah and her friend Jason Inagawa from the attentions of the racist police deputy, Kelby, everything changes. Sarah is part of a prophecy and she must escape the clutches of Malcolm, an assassin from a Believer Cell, the dragon-worshiping cult. When Sarah, Malcolm, and Kazimir eventually converge, they are thrown into another universe, where dragons seem never to have existed. Can they save this world and the one they left?"), ('authors', OrderedDict([('author', OrderedDict([('id', '370361'), ('name', 'Patrick Ness'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p5/370361.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p2/370361.jpg')])), ('link', 'https://www.goodreads.com/author/show/370361.Patrick_Ness'), ('average_rating', '4.12'), ('ratings_count', '631057'), ('text_reviews_count', '87055')]))])), ('published', '2020'), ('work', OrderedDict([('id', '70488386'), ('uri', 'kca://work/amzn1.gr.work.v1.aWmQvrbF9XEnGSR-EcfpqA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '31194576')])), ('isbn', '1406377279'), ('isbn13', '9781406377279'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1951')])), ('uri', 'kca://book/amzn1.gr.book.v1.4KQFkkhwyf4ECNZYLNkUBw'), ('title', 'Release'), ('title_without_series', 'Release'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485454954l/31194576._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485454954l/31194576._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/31194576-release'), ('num_pages', '287'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Walker Books'), ('publication_day', '4'), ('publication_year', '2017'), ('publication_month', '5'), ('average_rating', '3.70'), ('ratings_count', '14051'), ('description', 'It’s Saturday, it’s summer and, although he doesn’t know it yet, everything in Adam Thorn’s life is going to fall apart. Relationships will change, he’ll change, but maybe, just maybe, he’ll find freedom in the release.&lt;br /&gt;&lt;br /&gt;Time is running out though, because way across town a ghost as risen from the lake. Searching, yearning, she leaves a trail of destruction in her wake…'), ('authors', OrderedDict([('author', OrderedDict([('id', '370361'), ('name', 'Patrick Ness'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p5/370361.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p2/370361.jpg')])), ('link', 'https://www.goodreads.com/author/show/370361.Patrick_Ness'), ('average_rating', '4.12'), ('ratings_count', '631057'), ('text_reviews_count', '87055')]))])), ('published', '2017'), ('work', OrderedDict([('id', '51840657'), ('uri', 'kca://work/amzn1.gr.work.v1.xigxG5wUTMZ4EMpqIofCbg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '33555224')])), ('isbn', '1442472456'), ('isbn13', '9781442472457'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9245')])), ('uri', 'kca://book/amzn1.gr.book.v1.vY1B_oebTKCZxjW7sZRB-Q'), ('title', 'Thunderhead (Arc of a Scythe, #2)'), ('title_without_series', 'Thunderhead'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1505658534l/33555224._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1505658534l/33555224._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/33555224-thunderhead'), ('num_pages', '504'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon &amp; Schuster Books for Young Readers'), ('publication_day', '9'), ('publication_year', '2018'), ('publication_month', '1'), ('average_rating', '4.49'), ('ratings_count', '66065'), ('description', 'Rowan has gone rogue, and has taken it upon himself to put the Scythedom through a trial by fire. Literally. In the year since Winter Conclave, he has gone off-grid, and has been striking out against corrupt scythes—not only in MidMerica, but across the entire continent. He is a dark folk hero now—“Scythe Lucifer”—a vigilante taking down corrupt scythes in flames.&lt;br /&gt;&lt;br /&gt;Citra, now a junior scythe under Scythe Curie, sees the corruption and wants to help change it from the inside out, but is thwarted at every turn, and threatened by the “new order” scythes. Realizing she cannot do this alone—or even with the help of Scythe Curie and Faraday, she does the unthinkable, and risks being “deadish” so she can communicate with the Thunderhead—the only being on earth wise enough to solve the dire problems of a perfect world. But will it help solve those problems, or simply watch as perfection goes into decline?'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '676859'), ('text_reviews_count', '88669')]))])), ('published', '2018'), ('work', OrderedDict([('id', '54332060'), ('uri', 'kca://work/amzn1.gr.work.v1.csIUSRTP1nG0ilANHKdtvw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '28954189')])), ('isbn', '1442472421'), ('isbn13', '9781442472426'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '17009')])), ('uri', 'kca://book/amzn1.gr.book.v1.lW-2WpgCkQiPUhVi7Apjvw'), ('title', 'Scythe (Arc of a Scythe, #1)'), ('title_without_series', 'Scythe'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1456172676l/28954189._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1456172676l/28954189._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/28954189-scythe'), ('num_pages', '435'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon  Schuster Books for Young Readers'), ('publication_day', '22'), ('publication_year', '2016'), ('publication_month', '11'), ('average_rating', '4.34'), ('ratings_count', '124732'), ('description', '&lt;i&gt;Thou shalt kill.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;A world with no hunger, no disease, no war, no misery. Humanity has conquered all those things, and has even conquered death. Now scythes are the only ones who can end life—and they are commanded to do so, in order to keep the size of the population under control.&lt;br /&gt;&lt;br /&gt;Citra and Rowan are chosen to apprentice to a scythe—a role that neither wants. These teens must master the “art” of taking life, knowing that the consequence of failure could mean losing their own.'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '676859'), ('text_reviews_count', '88669')]))])), ('published', '2016'), ('work', OrderedDict([('id', '49179216'), ('uri', 'kca://work/amzn1.gr.work.v1.5n8t82DJpsluB4PsN0tTRA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '16143347')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '39255')])), ('uri', 'kca://book/amzn1.gr.book.v1.K-UvT466iI9PDxkBVNr4wQ'), ('title', 'We Were Liars'), ('title_without_series', 'We Were Liars'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1402749479l/16143347._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1402749479l/16143347._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/16143347-we-were-liars'), ('num_pages', '242'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Delacorte Press'), ('publication_day', '13'), ('publication_year', '2014'), ('publication_month', '5'), ('average_rating', '3.84'), ('ratings_count', '441079'), ('description', 'A beautiful and distinguished family.&lt;br /&gt;A private island.&lt;br /&gt;A brilliant, damaged girl; a passionate, political boy.&lt;br /&gt;A group of four friends—the Liars—whose friendship turns destructive.&lt;br /&gt;A revolution. An accident. A secret.&lt;br /&gt;Lies upon lies.&lt;br /&gt;True love.&lt;br /&gt;The truth.&lt;br /&gt; &lt;br /&gt;&lt;i&gt;We Were Liars&lt;/i&gt; is a modern, sophisticated suspense novel from &lt;i&gt;New York Times&lt;/i&gt; bestselling author, National Book Award finalist, and Printz Award honoree E. Lockhart. &lt;br /&gt;&lt;br /&gt;Read it.&lt;br /&gt;&lt;br /&gt;And if anyone asks you how it ends, just LIE.'), ('authors', OrderedDict([('author', OrderedDict([('id', '173491'), ('name', 'E. Lockhart'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1399077200p5/173491.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1399077200p2/173491.jpg')])), ('link', 'https://www.goodreads.com/author/show/173491.E_Lockhart'), ('average_rating', '3.78'), ('ratings_count', '579377'), ('text_reviews_count', '64038')]))])), ('published', '2014'), ('work', OrderedDict([('id', '21975829'), ('uri', 'kca://work/amzn1.gr.work.v1.SGGFlQ0RQuN1B3XE8ibruQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '29391367')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', '9780994310972'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '75')])), ('uri', 'kca://book/amzn1.gr.book.v1.Jj4YqqkesFUaPlrQUhF88A'), ('title', 'Chapter One: You have the power to change stuff'), ('title_without_series', 'Chapter One: You have the power to change stuff'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1457174638l/29391367._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1457174638l/29391367._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/29391367-chapter-one'), ('num_pages', '254'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'The Messenger Group'), ('publication_day', None), ('publication_year', '2016'), ('publication_month', '2'), ('average_rating', '4.20'), ('ratings_count', '585'), ('description', 'CHAPTER ONE is a story of epic proportions by Thankyou co-founder Daniel Flynn. It’s a bumpy and entertaining ride of gut-wrenching decisions, wild mistakes and daring moves into business, marketing, social enterprise and beyond. Follow the journey of three Australian kids from Melbourne with zero business experience and the shared belief that we all have the power to change stuff.&lt;br /&gt;&lt;br /&gt;Chapter One is more than a book. It’s an invitation, addressed to you. To inspire you to challenge what you know and remind you that crazy ideas can become a reality. It’s also an opportunity to be a part of something big. Something that could change the course of history.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3060790'), ('name', 'Daniel Flynn'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/3060790.Daniel_Flynn'), ('average_rating', '4.19'), ('ratings_count', '589'), ('text_reviews_count', '84')]))])), ('published', '2016'), ('work', OrderedDict([('id', '49645010'), ('uri', 'kca://work/amzn1.gr.work.v1.t_y7EkxOYbIkatJPWXAWXg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40097951')])), ('isbn', '1250301696'), ('isbn13', '9781250301697'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '35185')])), ('uri', 'kca://book/amzn1.gr.book.v1.Vjz3eASF7bmIo5WYoKMsnA'), ('title', 'The Silent Patient'), ('title_without_series', 'The Silent Patient'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582759969l/40097951._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582759969l/40097951._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40097951-the-silent-patient'), ('num_pages', '325'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Celadon Books'), ('publication_day', '5'), ('publication_year', '2019'), ('publication_month', '2'), ('average_rating', '4.09'), ('ratings_count', '419520'), ('description', 'Alicia Berenson’s life is seemingly perfect. A famous painter married to an in-demand fashion photographer, she lives in a grand house with big windows overlooking a park in one of London’s most desirable areas. One evening her husband Gabriel returns home late from a fashion shoot, and Alicia shoots him five times in the face, and then never speaks another word.&lt;br /&gt;&lt;br /&gt;Alicia’s refusal to talk, or give any kind of explanation, turns a domestic tragedy into something far grander, a mystery that captures the public imagination and casts Alicia into notoriety. The price of her art skyrockets, and she, the silent patient, is hidden away from the tabloids and spotlight at the Grove, a secure forensic unit in North London.&lt;br /&gt;&lt;br /&gt;Theo Faber is a criminal psychotherapist who has waited a long time for the opportunity to work with Alicia. His determination to get her to talk and unravel the mystery of why she shot her husband takes him down a twisting path into his own motivations—a search for the truth that threatens to consume him...'), ('authors', OrderedDict([('author', OrderedDict([('id', '17621440'), ('name', 'Alex Michaelides'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1526317750p5/17621440.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1526317750p2/17621440.jpg')])), ('link', 'https://www.goodreads.com/author/show/17621440.Alex_Michaelides'), ('average_rating', '4.09'), ('ratings_count', '420431'), ('text_reviews_count', '43800')]))])), ('published', '2019'), ('work', OrderedDict([('id', '59752778'), ('uri', 'kca://work/amzn1.gr.work.v1.MUfHMLGEE_tCE7JMBSsL1A')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '22628')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '45593')])), ('uri', 'kca://book/amzn1.gr.book.v1.3TyU0wMKQZ7LYyvGh01Eqg'), ('title', 'The Perks of Being a Wallflower'), ('title_without_series', 'The Perks of Being a Wallflower'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1520093244l/22628._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1520093244l/22628._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/22628.The_Perks_of_Being_a_Wallflower'), ('num_pages', '213'), ('format', 'Paperback'), ('edition_information', '1st MTV/Pocket Books trade paperback edition (US/CAN)'), ('publisher', 'MTV Books/Pocket Books'), ('publication_day', None), ('publication_year', '1999'), ('publication_month', '2'), ('average_rating', '4.20'), ('ratings_count', '1222456'), ('description', "standing on the fringes of life...&lt;br /&gt;offers a unique perspective. But there comes a time to see&lt;br /&gt;what it looks like from the dance floor.&lt;br /&gt;&lt;br /&gt;This haunting novel about the dilemma of passivity vs. passion marks the stunning debut of a provocative new voice in contemporary fiction: The Perks of Being A WALLFLOWER&lt;br /&gt;&lt;br /&gt;This is the story of what it's like to grow up in high school. More intimate than a diary, Charlie's letters are singular and unique, hilarious and devastating. We may not know where he lives. We may not know to whom he is writing. All we know is the world he shares. Caught between trying to live his life and trying to run from it puts him on a strange course through uncharted territory. The world of first dates and mixed tapes, family dramas and new friends. The world of sex, drugs, and The Rocky Horror Picture Show, when all one requires is that the perfect song on that perfect drive to feel infinite.&lt;br /&gt;&lt;br /&gt;Through Charlie, Stephen Chbosky has created a deeply affecting coming-of-age story, a powerful novel that will spirit you back to those wild and poignant roller coaster days known as growing up.&lt;br /&gt;&lt;br /&gt;(back cover)"), ('authors', OrderedDict([('author', OrderedDict([('id', '12898'), ('name', 'Stephen Chbosky'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_200x266-d279b33f8eec0f27b7272477f09806be.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_50x66-82093808bca726cb3249a493fbd3bd0f.png')])), ('link', 'https://www.goodreads.com/author/show/12898.Stephen_Chbosky'), ('average_rating', '4.19'), ('ratings_count', '1243011'), ('text_reviews_count', '61313')]))])), ('published', '1999'), ('work', OrderedDict([('id', '2236198'), ('uri', 'kca://work/amzn1.gr.work.v1.ssZvkcqaAEbn5_xfTc0TGw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '11870085')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '139206')])), ('uri', 'kca://book/amzn1.gr.book.v1.6rIwidkUTORGkQo3jY4dcg'), ('title', 'The Fault in Our Stars'), ('title_without_series', 'The Fault in Our Stars'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1360206420l/11870085._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1360206420l/11870085._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/11870085-the-fault-in-our-stars'), ('num_pages', '313'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Dutton Books'), ('publication_day', '10'), ('publication_year', '2012'), ('publication_month', '1'), ('average_rating', '4.21'), ('ratings_count', '3450407'), ('description', "Despite the tumor-shrinking medical miracle that has bought her a few years, Hazel has never been anything but terminal, her final chapter inscribed upon diagnosis. But when a gorgeous plot twist named Augustus Waters suddenly appears at Cancer Kid Support Group, Hazel's story is about to be completely rewritten.&lt;br /&gt;&lt;br /&gt;Insightful, bold, irreverent, and raw, The Fault in Our Stars is award-winning author John Green's most ambitious and heartbreaking work yet, brilliantly exploring the funny, thrilling, and tragic business of being alive and in love."), ('authors', OrderedDict([('author', OrderedDict([('id', '1406384'), ('name', 'John Green'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353452301p5/1406384.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353452301p2/1406384.jpg')])), ('link', 'https://www.goodreads.com/author/show/1406384.John_Green'), ('average_rating', '4.04'), ('ratings_count', '6643278'), ('text_reviews_count', '348352')]))])), ('published', '2012'), ('work', OrderedDict([('id', '16827462'), ('uri', 'kca://work/amzn1.gr.work.v1.ZWeA15QphzWjRB87CLg-TA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6900')])), ('isbn', '0751529818'), ('isbn13', '9780751529814'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '21564')])), ('uri', 'kca://book/amzn1.gr.book.v1.HYlfDM7QTPV1OEJGJmRHtw'), ('title', 'Tuesdays with Morrie'), ('title_without_series', 'Tuesdays with Morrie'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423763749l/6900._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423763749l/6900._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6900.Tuesdays_with_Morrie'), ('num_pages', '210'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Warner'), ('publication_day', None), ('publication_year', '2000'), ('publication_month', None), ('average_rating', '4.11'), ('ratings_count', '762480'), ('description', "Maybe it was a grandparent, or a teacher or a colleague. Someone older, patient and wise, who understood you when you were young and searching, and gave you sound advice to help you make your way through it. For Mitch Albom, that person was Morrie Schwartz, his college professor from nearly twenty years ago.&lt;br /&gt;&lt;br /&gt;Maybe, like Mitch, you lost track of this mentor as you made your way, and the insights faded. Wouldn't you like to see that person again, ask the bigger questions that still haunt you? &lt;br /&gt;&lt;br /&gt;Mitch Albom had that second chance. He rediscovered Morrie in the last months of the older man's life. Knowing he was dying of ALS - or motor neurone disease - Mitch visited Morrie in his study every Tuesday, just as they used to back in college. Their rekindled relationship turned into one final 'class': lessons in how to live."), ('authors', OrderedDict([('author', OrderedDict([('id', '2331'), ('name', 'Mitch Albom'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1368640552p5/2331.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1368640552p2/2331.jpg')])), ('link', 'https://www.goodreads.com/author/show/2331.Mitch_Albom'), ('average_rating', '4.04'), ('ratings_count', '1757643'), ('text_reviews_count', '83886')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1995335'), ('uri', 'kca://work/amzn1.gr.work.v1.zIj_sWs9NizBbBF7FwK_mQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '19063')])), ('isbn', '0375831002'), ('isbn13', '9780375831003'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '89186')])), ('uri', 'kca://book/amzn1.gr.book.v1.A1zfLKejdNPkLkjfE8LN8Q'), ('title', 'The Book Thief'), ('title_without_series', 'The Book Thief'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1522157426l/19063._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1522157426l/19063._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/19063.The_Book_Thief'), ('num_pages', '552'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Alfred A. Knopf'), ('publication_day', '14'), ('publication_year', '2006'), ('publication_month', '3'), ('average_rating', '4.37'), ('ratings_count', '1784559'), ('description', '&lt;i&gt;Librarian\'s note: An alternate cover edition can be found &lt;a href="https://www.goodreads.com/book/show/41048862.here" title="here" rel="nofollow"&gt;here&lt;/a&gt;&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;It is 1939. Nazi Germany. The country is holding its breath. Death has never been busier, and will be busier still.&lt;br /&gt;&lt;br /&gt;By her brother\'s graveside, Liesel\'s life is changed when she picks up a single object, partially hidden in the snow. It is The Gravedigger\'s Handbook, left behind there by accident, and it is her first act of book thievery. So begins a love affair with books and words, as Liesel, with the help of her accordian-playing foster father, learns to read. Soon she is stealing books from Nazi book-burnings, the mayor\'s wife\'s library, wherever there are books to be found.&lt;br /&gt;&lt;br /&gt;But these are dangerous times. When Liesel\'s foster family hides a Jew in their basement, Liesel\'s world is both opened up, and closed down.&lt;br /&gt;&lt;br /&gt;In superbly crafted writing that burns with intensity, award-winning author Markus Zusak has given us one of the most enduring stories of our time.&lt;br /&gt;&lt;br /&gt;(Note: this title was not published as YA fiction)'), ('authors', OrderedDict([('author', OrderedDict([('id', '11466'), ('name', 'Markus Zusak'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1537240528p5/11466.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1537240528p2/11466.jpg')])), ('link', 'https://www.goodreads.com/author/show/11466.Markus_Zusak'), ('average_rating', '4.34'), ('ratings_count', '1960800'), ('text_reviews_count', '132125')]))])), ('published', '2006'), ('work', OrderedDict([('id', '878368'), ('uri', 'kca://work/amzn1.gr.work.v1.BGVqmVn5CPHsjnZIfHpUUw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6334')])), ('isbn', '1400078776'), ('isbn13', '9781400078776'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '23972')])), ('uri', 'kca://book/amzn1.gr.book.v1.t3ESMobC-9O2YByR0RqA6g'), ('title', 'Never Let Me Go'), ('title_without_series', 'Never Let Me Go'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353048590l/6334._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353048590l/6334._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6334.Never_Let_Me_Go'), ('num_pages', '288'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Vintage Books'), ('publication_day', '31'), ('publication_year', '2010'), ('publication_month', '8'), ('average_rating', '3.82'), ('ratings_count', '457251'), ('description', 'From the Booker Prize-winning author of &lt;i&gt;The Remains of the Day&lt;/i&gt; and &lt;i&gt;When We Were Orphans&lt;/i&gt;, comes an unforgettable edge-of-your-seat mystery that is at once heartbreakingly tender and morally courageous about what it means to be human.&lt;br /&gt;&lt;br /&gt;Hailsham seems like a pleasant English boarding school, far from the influences of the city. Its students are well tended and supported, trained in art and literature, and become just the sort of people the world wants them to be. But, curiously, they are taught nothing of the outside world and are allowed little contact with it.&lt;br /&gt;&lt;br /&gt;Within the grounds of Hailsham, Kathy grows from schoolgirl to young woman, but it’s only when she and her friends Ruth and Tommy leave the safe grounds of the school (as they always knew they would) that they realize the full truth of what Hailsham is.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Never Let Me Go&lt;/i&gt; breaks through the boundaries of the literary novel. It is a gripping mystery, a beautiful love story, and also a scathing critique of human arrogance and a moral examination of how we treat the vulnerable and different in our society. In exploring the themes of memory and the impact of the past, Ishiguro takes on the idea of a possible future to create his most moving and powerful book to date.'), ('authors', OrderedDict([('author', OrderedDict([('id', '4280'), ('name', 'Kazuo Ishiguro'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1424906625p5/4280.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1424906625p2/4280.jpg')])), ('link', 'https://www.goodreads.com/author/show/4280.Kazuo_Ishiguro'), ('average_rating', '3.84'), ('ratings_count', '819560'), ('text_reviews_count', '63684')]))])), ('published', '2010'), ('work', OrderedDict([('id', '1499998'), ('uri', 'kca://work/amzn1.gr.work.v1.Z4gC--jsCarRwWlyoQp-VQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '39335566')])), ('isbn', '0385543875'), ('isbn13', '9780385543873'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1527')])), ('uri', 'kca://book/amzn1.gr.book.v1.XSmg5W7_uZm9h4X_93gS5g'), ('title', 'The Water Cure'), ('title_without_series', 'The Water Cure'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1521604165l/39335566._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1521604165l/39335566._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/39335566-the-water-cure'), ('num_pages', '288'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Doubleday'), ('publication_day', '8'), ('publication_year', '2019'), ('publication_month', '1'), ('average_rating', '3.26'), ('ratings_count', '16751'), ('description', '&lt;b&gt;&lt;i&gt;The Handmaid’s Tale&lt;/i&gt; meets &lt;i&gt;The Virgin Suicides&lt;/i&gt; in this dystopic feminist revenge fantasy about three sisters on an isolated island, raised to fear men&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;King has tenderly staked out a territory for his wife and three daughters, Grace, Lia, and Sky. He has laid the barbed wire; he has anchored the buoys in the water; he has marked out a clear message: Do not enter. Or viewed from another angle: Not safe to leave. Here women are protected from the chaos and violence of men on the mainland. The cult-like rituals and therapies they endure fortify them from the spreading toxicity of a degrading world.&lt;br /&gt;&lt;br /&gt;But when their father, the only man they’ve ever seen, disappears, they retreat further inward until the day three strange men wash ashore. Over the span of one blistering hot week, a psychological cat-and-mouse game plays out. Sexual tensions and sibling rivalries flare as the sisters confront the amorphous threat the strangers represent. Can they survive the men?&lt;br /&gt;&lt;br /&gt;A haunting, riveting debut about the capacity for violence and the potency of female desire, &lt;i&gt;The Water Cure&lt;/i&gt; both devastates and astonishes as it reflects our own world back at us.'), ('authors', OrderedDict([('author', OrderedDict([('id', '6152025'), ('name', 'Sophie Mackintosh'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1536937022p5/6152025.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1536937022p2/6152025.jpg')])), ('link', 'https://www.goodreads.com/author/show/6152025.Sophie_Mackintosh'), ('average_rating', '3.31'), ('ratings_count', '18078'), ('text_reviews_count', '2593')]))])), ('published', '2019'), ('work', OrderedDict([('id', '56832986'), ('uri', 'kca://work/amzn1.gr.work.v1.Oftp5vHVmbQeEnskpnPsMg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '9305362')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '4185')])), ('uri', 'kca://book/amzn1.gr.book.v1.XRBgHq982k9dupkNGLEqLg'), ('title', 'Captive Prince (Captive Prince, #1)'), ('title_without_series', 'Captive Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356028113l/9305362._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356028113l/9305362._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/9305362-captive-prince'), ('num_pages', '240'), ('format', 'ebook'), ('edition_information', None), ('publisher', None), ('publication_day', '22'), ('publication_year', '2012'), ('publication_month', '5'), ('average_rating', '3.88'), ('ratings_count', '52024'), ('description', '&lt;b&gt;From global phenomenon C. S. Pacat comes the first in her critically acclaimed trilogy—with a bonus story.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;Damen is a warrior hero to his people, and the rightful heir to the throne of Akielos. But when his half brother seizes power, Damen is captured, stripped of his identity, and sent to serve the prince of an enemy nation as a pleasure slave.&lt;br /&gt;&lt;br /&gt;Beautiful, manipulative, and deadly, his new master, Prince Laurent, epitomizes the worst of the court at Vere. But in the lethal political web of the Veretian court, nothing is as it seems, and when Damen finds himself caught up in a play for the throne, he must work together with Laurent to survive and save his country.&lt;br /&gt;&lt;br /&gt;For Damen, there is just one rule: never, ever reveal his true identity. Because the one man Damen needs is the one man who has more reason to hate him than anyone else…&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Includes an exclusive extra story!&lt;/b&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '191848'), ('text_reviews_count', '25580')]))])), ('published', '2012'), ('work', OrderedDict([('id', '14188292'), ('uri', 'kca://work/amzn1.gr.work.v1.0CuNLmY6oZw9oaliTYsfGg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '29283884')])), ('isbn', '0062382802'), ('isbn13', '9780062382801'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '12983')])), ('uri', 'kca://book/amzn1.gr.book.v1.Lo3JQRH4kkQxjMVU6JD9Yg'), ('title', "The Gentleman's Guide to Vice and Virtue (Montague Siblings, #1)"), ('title_without_series', "The Gentleman's Guide to Vice and Virtue"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1492601464l/29283884._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1492601464l/29283884._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/29283884-the-gentleman-s-guide-to-vice-and-virtue'), ('num_pages', '513'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Katherine Tegen Books'), ('publication_day', '27'), ('publication_year', '2017'), ('publication_month', '6'), ('average_rating', '4.12'), ('ratings_count', '84096'), ('description', 'Henry “Monty” Montague was born and bred to be a gentleman, but he was never one to be tamed. The finest boarding schools in England and the constant disapproval of his father haven’t been able to curb any of his roguish passions—not for gambling halls, late nights spent with a bottle of spirits, or waking up in the arms of women or men.&lt;br /&gt;&lt;br /&gt;But as Monty embarks on his Grand Tour of Europe, his quest for a life filled with pleasure and vice is in danger of coming to an end. Not only does his father expect him to take over the family’s estate upon his return, but Monty is also nursing an impossible crush on his best friend and traveling companion, Percy.&lt;br /&gt;&lt;br /&gt;Still it isn’t in Monty’s nature to give up. Even with his younger sister, Felicity, in tow, he vows to make this yearlong escapade one last hedonistic hurrah and flirt with Percy from Paris to Rome. But when one of Monty’s reckless decisions turns their trip abroad into a harrowing manhunt that spans across Europe, it calls into question everything he knows, including his relationship with the boy he adores.'), ('authors', OrderedDict([('author', OrderedDict([('id', '7327341'), ('name', 'Mackenzi Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1512266703p5/7327341.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1512266703p2/7327341.jpg')])), ('link', 'https://www.goodreads.com/author/show/7327341.Mackenzi_Lee'), ('average_rating', '4.10'), ('ratings_count', '129724'), ('text_reviews_count', '25257')]))])), ('published', '2017'), ('work', OrderedDict([('id', '49527118'), ('uri', 'kca://work/amzn1.gr.work.v1.KF8U_R5FRuUIlCVQG4A7pQ')]))])</t>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '32595035')])), ('isbn', '1474600042'), ('isbn13', '9781474600040'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '18')])), ('uri', 'kca://book/amzn1.gr.book.v1.pT8U80AoRYVn5k5h20vuOQ'), ('title', 'We Only Saw Happiness'), ('title_without_series', 'We Only Saw Happiness'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1476266549l/32595035._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1476266549l/32595035._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/32595035-we-only-saw-happiness'), ('num_pages', '320'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Weidenfeld &amp; Nicholson'), ('publication_day', '29'), ('publication_year', '2016'), ('publication_month', '12'), ('average_rating', '3.64'), ('ratings_count', '790'), ('description', "'We looked like the perfect young family, something out of a magazine, in shades of marshmallow pink...'&lt;br /&gt; A photograph. The father smiling beside his new car, the mother pregnant and radiant, the little girl placing cuddly toys in the cot for her new baby brother. All we see is the happiness.&lt;br /&gt; 'We don't see my mother. We don't see the lies.'&lt;br /&gt; But behind every picture there is a story. And behind that story, there are others.&lt;br /&gt; Every family has its secrets.&lt;br /&gt; When Antoine was young, he believed in love at first sight. He finds the woman of his dreams, Nathalie, and has two children. But when Antoine's life implodes, he does something unspeakable.&lt;br /&gt; Antoine's journey to come to terms with what he has done will take him across seas and continents, deep into his own heart and the hearts of others.&lt;br /&gt; Because in order to find true happiness, you have to know where to look..."), ('authors', OrderedDict([('author', OrderedDict([('id', '5416412'), ('name', 'Grégoire Delacourt'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1374772295p5/5416412.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1374772295p2/5416412.jpg')])), ('link', 'https://www.goodreads.com/author/show/5416412.Gr_goire_Delacourt'), ('average_rating', '3.55'), ('ratings_count', '14059'), ('text_reviews_count', '2153')]))])), ('published', '2016'), ('work', OrderedDict([('id', '42573935'), ('uri', 'kca://work/amzn1.gr.work.v1.IsjqYt9xlzObwwGlZBGiIw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17250')])), ('isbn', '0142437336'), ('isbn13', '9780142437339'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '6261')])), ('uri', 'kca://book/amzn1.gr.book.v1.4QGkL9_VomC7Ay9rPVfpFw'), ('title', 'The Crucible'), ('title_without_series', 'The Crucible'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1547467608l/17250._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1547467608l/17250._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17250.The_Crucible'), ('num_pages', '143'), ('format', 'Paperback'), ('edition_information', 'Penguin Classics (US/CAN)'), ('publisher', 'Penguin Books'), ('publication_day', '25'), ('publication_year', '2003'), ('publication_month', '3'), ('average_rating', '3.59'), ('ratings_count', '318126'), ('description', '"I believe that the reader will discover here the essential nature of one of the strangest and most awful chapters in human history," Arthur Miller wrote of his classic play about the witch-hunts and trials in seventeenth-century Salem, Massachusetts. Based on historical people and real events, Miller\'s drama is a searing portrait of a community engulfed by hysteria. In the rigid theocracy of Salem, rumors that women are practicing witchcraft galvanize the town\'s most basic fears and suspicions; and when a young girl accuses Elizabeth Proctor of being a witch, self-righteous church leaders and townspeople insist that Elizabeth be brought to trial. The ruthlessness of the prosecutors and the eagerness of neighbor to testify against neighbor brilliantly illuminates the destructive power of socially sanctioned violence.&lt;br /&gt;&lt;br /&gt;Written in 1953, &lt;i&gt;The Crucible&lt;/i&gt; is a mirror Miller uses to reflect the anti-communist hysteria inspired by Senator Joseph McCarthy\'s "witch-hunts" in the United States. Within the text itself, Miller contemplates the parallels, writing, "Political opposition... is given an inhumane overlay, which then justifies the abrogation of all normally applied customs of civilized behavior. A political policy is equated with moral right, and opposition to it with diabolical malevolence."&lt;br /&gt;&lt;br /&gt;WIth an introduction by Christopher Bigsby.&lt;br /&gt;(back cover)'), ('authors', OrderedDict([('author', OrderedDict([('id', '8120'), ('name', 'Arthur  Miller'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201186455p5/8120.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201186455p2/8120.jpg')])), ('link', 'https://www.goodreads.com/author/show/8120.Arthur_Miller'), ('average_rating', '3.59'), ('ratings_count', '552744'), ('text_reviews_count', '15023')]))])), ('published', '2003'), ('work', OrderedDict([('id', '1426723'), ('uri', 'kca://work/amzn1.gr.work.v1.Jaxd0bIoSWAN9rx4HzDwjQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '886785')])), ('isbn', '0714833568'), ('isbn13', '9780714833569'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '21')])), ('uri', 'kca://book/amzn1.gr.book.v1.rAxLhrIuurET1Dbx2hMPoA'), ('title', 'Modern Architecture Since 1900'), ('title_without_series', 'Modern Architecture Since 1900'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/886785.Modern_Architecture_Since_1900'), ('num_pages', '736'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Phaidon Press'), ('publication_day', '27'), ('publication_year', '1996'), ('publication_month', '6'), ('average_rating', '4.08'), ('ratings_count', '1054'), ('description', 'Since its first publication in 1982, &lt;i&gt;Modern Architecture Since 1900&lt;/i&gt; has become established as a contemporary classic. Worldwide in scope, it combines a clear historical outline with masterly analysis and interpretation. Technical, economic, social and intellectual developments are brought together in a comprehensive narrative which provides a setting for the detailed examination of buildings. Throughout the book the author\'s focus is on the individual architect, and on the qualities that give outstanding buildings their lasting value.&lt;br /&gt;&lt;br /&gt;For the third edition, the text has been radically revised and expanded, incorporating much new material and a fresh appreciation of regional identity and variety. Seven chapters are entirely new, including expanded coverage of recent world architecture.&lt;br /&gt;&lt;br /&gt;Described by James Ackerman of Harvard University as "immeasurably the finest work covering this field in existence", this book presents a penetrating analysis of the modern tradition and its origins, tracing the creative interaction between old and new that has generated such an astonishing richness of architectural forms across the world and throughout the century.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3976667'), ('name', 'William J.R. Curtis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1380554725p5/3976667.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1380554725p2/3976667.jpg')])), ('link', 'https://www.goodreads.com/author/show/3976667.William_J_R_Curtis'), ('average_rating', '4.07'), ('ratings_count', '1133'), ('text_reviews_count', '23')]))])), ('published', '1996'), ('work', OrderedDict([('id', '872044'), ('uri', 'kca://work/amzn1.gr.work.v1.ZSoJ4MCRLdTd6Th4yZ0n6g')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '11012')])), ('isbn', '0192839993'), ('isbn13', '9780192839992'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3423')])), ('uri', 'kca://book/amzn1.gr.book.v1.KblRjbRdBwFtFzWvuWDuhw'), ('title', 'Dubliners'), ('title_without_series', 'Dubliners'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1334138184l/11012._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1334138184l/11012._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/11012.Dubliners'), ('num_pages', '207'), ('format', 'Paperback'), ('edition_information', "Oxford World's Classics"), ('publisher', 'Oxford University Press'), ('publication_day', '15'), ('publication_year', '2001'), ('publication_month', '3'), ('average_rating', '3.85'), ('ratings_count', '121180'), ('description', 'This work of art reflects life in Ireland at the turn of the last century, and by rejecting euphemism, reveals to the Irish their unromantic realities. Each of the 15 stories offers glimpses into the lives of ordinary Dubliners, and collectively they paint a portrait of a nation.'), ('authors', OrderedDict([('author', OrderedDict([('id', '5144'), ('name', 'James Joyce'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517863935p5/5144.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517863935p2/5144.jpg')])), ('link', 'https://www.goodreads.com/author/show/5144.James_Joyce'), ('average_rating', '3.74'), ('ratings_count', '414846'), ('text_reviews_count', '21387')]))])), ('published', '2001'), ('work', OrderedDict([('id', '260248'), ('uri', 'kca://work/amzn1.gr.work.v1.0VPHnf0j0ZK6NC33OETGgQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '100915')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15660')])), ('uri', 'kca://book/amzn1.gr.book.v1.bTpunK9LhLneojBwpPB9iQ'), ('title', 'The Lion, the Witch and the Wardrobe (Chronicles of Narnia, #1)'), ('title_without_series', 'The Lion, the Witch and the Wardrobe'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353029077l/100915._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353029077l/100915._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/100915.The_Lion_the_Witch_and_the_Wardrobe'), ('num_pages', '206'), ('format', 'Paperback'), ('edition_information', 'Film Tie-in Edition (US/CAN)'), ('publisher', 'HarperCollins Publishers'), ('publication_day', None), ('publication_year', '2005'), ('publication_month', None), ('average_rating', '4.22'), ('ratings_count', '2087362'), ('description', "Narnia...the land beyond the wardrobe door, a secret place frozen in eternal winter, a magical country waiting to be set free.&lt;br /&gt;&lt;br /&gt;Lucy is the first to find the secret of the wardrobe in the professor's mysterious old house. At first her brothers and sister don't believe her when she tells of her visit to the land of Narnia. But soon Edmund, then Peter and Susan step through the wardrobe themselves. In Narnia they find a country buried under the evil enchantment of the White Witch. When they meet the Lion Aslan, they realize they've been called to a great adventure and bravely join the battle to free Narnia from the Witch's sinister spell."), ('authors', OrderedDict([('author', OrderedDict([('id', '1069006'), ('name', 'C.S. Lewis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1564671804p5/1069006.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1564671804p2/1069006.jpg')])), ('link', 'https://www.goodreads.com/author/show/1069006.C_S_Lewis'), ('average_rating', '4.15'), ('ratings_count', '5769987'), ('text_reviews_count', '134456')]))])), ('published', '2005'), ('work', OrderedDict([('id', '4790821'), ('uri', 'kca://work/amzn1.gr.work.v1.rqpJlzO5rS559vW35rJa1w')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '48855')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '22205')])), ('uri', 'kca://book/amzn1.gr.book.v1.NpJw6QbRgLr9alsXArRByw'), ('title', 'The Diary of a Young Girl'), ('title_without_series', 'The Diary of a Young Girl'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1560816565l/48855._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1560816565l/48855._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/48855.The_Diary_of_a_Young_Girl'), ('num_pages', '283'), ('format', 'Mass Market Paperback'), ('edition_information', 'US / CAN Edition'), ('publisher', 'Bantam'), ('publication_day', None), ('publication_year', '1993'), ('publication_month', '7'), ('average_rating', '4.15'), ('ratings_count', '2678567'), ('description', 'Discovered in the attic in which she spent the last years of her life, Anne Frank’s remarkable diary has become a world classic—a powerful reminder of the horrors of war and an eloquent testament to the human spirit. &lt;br /&gt;&lt;br /&gt;In 1942, with the Nazis occupying Holland, a thirteen-year-old Jewish girl and her family fled their home in Amsterdam and went into hiding. For the next two years, until their whereabouts were betrayed to the Gestapo, the Franks and another family lived cloistered in the “Secret Annexe” of an old office building. Cut off from the outside world, they faced hunger, boredom, the constant cruelties of living in confined quarters, and the ever-present threat of discovery and death. In her diary Anne Frank recorded vivid impressions of her experiences during this period. By turns thoughtful, moving, and surprisingly humorous, her account offers a fascinating commentary on human courage and frailty and a compelling self-portrait of a sensitive and spirited young woman whose promise was tragically cut short.&lt;br /&gt;--back cover'), ('authors', OrderedDict([('author', OrderedDict([('id', '3720'), ('name', 'Anne Frank'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1343271406p5/3720.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1343271406p2/3720.jpg')])), ('link', 'https://www.goodreads.com/author/show/3720.Anne_Frank'), ('average_rating', '4.15'), ('ratings_count', '2731392'), ('text_reviews_count', '29970')]))])), ('published', '1993'), ('work', OrderedDict([('id', '3532896'), ('uri', 'kca://work/amzn1.gr.work.v1.Hn8z2cQc--WW1zAa5fCZ8Q')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '23418')])), ('isbn', '0375424431'), ('isbn13', '9780375424434'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '573')])), ('uri', 'kca://book/amzn1.gr.book.v1.4Xb6Kyv3wTW1yf-CyMYZww'), ('title', 'The Architecture of Happiness'), ('title_without_series', 'The Architecture of Happiness'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1320402527l/23418._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1320402527l/23418._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/23418.The_Architecture_of_Happiness'), ('num_pages', '280'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Pantheon Books'), ('publication_day', '3'), ('publication_year', '2006'), ('publication_month', '10'), ('average_rating', '3.86'), ('ratings_count', '9514'), ('description', "One of the great but often unmentioned causes of both happiness and misery is the quality of our environment: the kinds of walls, chairs, buildings and streets that surround us.&lt;br /&gt;&lt;br /&gt;And yet a concern for architecture and design is too often described as frivolous, even self-indulgent. &lt;i&gt;The Architecture of Happiness&lt;/i&gt; starts from the idea that where we are heavily influences who we can be, and it argues that it is architecture's task to stand as an eloquent reminder of our full potential.&lt;br /&gt;&lt;br /&gt;Whereas many architects are wary of openly discussing the word beauty, this book has at its center the large and naÃ¯ve question: What is a beautiful building? It is a tour through the philosophy and psychology of architecture that aims to change the way we think about our homes, our streets and ourselves."), ('authors', OrderedDict([('author', OrderedDict([('id', '13199'), ('name', 'Alain de Botton'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1189753902p5/13199.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1189753902p2/13199.jpg')])), ('link', 'https://www.goodreads.com/author/show/13199.Alain_de_Botton'), ('average_rating', '3.88'), ('ratings_count', '157465'), ('text_reviews_count', '14955')]))])), ('published', '2006'), ('work', OrderedDict([('id', '14280280'), ('uri', 'kca://work/amzn1.gr.work.v1.rEzwDi9RY4yEBtT22gamiw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65118')])), ('isbn', '1405206128'), ('isbn13', '9781405206129'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1642')])), ('uri', 'kca://book/amzn1.gr.book.v1.N-akGxhuwZFzm7LbrmJFRA'), ('title', 'The Hostile Hospital (A Series of Unfortunate Events, #8)'), ('title_without_series', 'The Hostile Hospital'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1442446120l/65118._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1442446120l/65118._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65118.The_Hostile_Hospital'), ('num_pages', '272'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Egmont'), ('publication_day', '10'), ('publication_year', '2003'), ('publication_month', '5'), ('average_rating', '3.98'), ('ratings_count', '95748'), ('description', 'There is nothing to be found in the pages of these books but misery and despair. You still have time to choose something else to read. But if you must know what unpleasantries befall the charming and clever Baudelaire children read on...The Hostile Hospital - There are many pleasant things to read about, but this book contains none of them. Within its pages are such burdensome details as a suspicious shopkeeper, unnecessary surgery, heartshaped balloons, and some very starling news about a fire. Clearly you do not want to read about such things.'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2003'), ('work', OrderedDict([('id', '2361348'), ('uri', 'kca://work/amzn1.gr.work.v1.ZpzpFRdXjTgW8J55PN2lTA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65112')])), ('isbn', '0064410161'), ('isbn13', '9780064410168'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3918')])), ('uri', 'kca://book/amzn1.gr.book.v1.o5jBgMg8ttG282oaM2iIDQ'), ('title', 'The End (A Series of Unfortunate Events, #13)'), ('title_without_series', 'The End'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524761836l/65112._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524761836l/65112._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65112.The_End'), ('num_pages', '337'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '13'), ('publication_year', '2006'), ('publication_month', '10'), ('average_rating', '4.01'), ('ratings_count', '87130'), ('description', "The last volume of the fabulously popular A Series of Unfortunate Events series, in which the history of the Baudelaire orphans is brought to its end.&lt;br /&gt;&lt;br /&gt;You are presumably looking at the back of this book, or the end of the end. The end of the end is the best place to begin the end, because if you read the end from the beginning of the beginning of the end to the end of the end of the end, you will arrive at the end of the end of your rope. &lt;br /&gt;&lt;br /&gt;This book is the last in A Series of Unfortunate Events, and even if you braved the previous twelve volumes, you probably can't stand such unpleasantries as a fearsome storm, a suspicious beverage, a herd of wild sheep, an enormous bird cage, and a truly haunting secret about the Baudelaire parents. &lt;br /&gt;&lt;br /&gt;It has been my solemn occupation to complete the history of the Baudelaire orphans, and at last I am finished. You likely have some other occupation, so if I were you I would drop this book at once, so the end does not finish you. &lt;br /&gt;&lt;br /&gt;With all due respect, &lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2006'), ('work', OrderedDict([('id', '838691'), ('uri', 'kca://work/amzn1.gr.work.v1.OqpRj6gIRLqzkyybvvAbRQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65110')])), ('isbn', '0064410153'), ('isbn13', '9780064410151'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2037')])), ('uri', 'kca://book/amzn1.gr.book.v1.sKBvH0WXYsoxUb8stGauIw'), ('title', 'The Penultimate Peril (A Series of Unfortunate Events, #12)'), ('title_without_series', 'The Penultimate Peril'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524161970l/65110._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1524161970l/65110._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65110.The_Penultimate_Peril'), ('num_pages', '353'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '18'), ('publication_year', '2005'), ('publication_month', '10'), ('average_rating', '4.06'), ('ratings_count', '87336'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;If this is the first book you found while searching for a book to read next, then the first thing you should know is that this next-to-last book is what you should put down first. Sadly, this book presents the next-to-last chronicle of the lives of the Baudelaire orphans, and it is next-to-first in its supply of misery, despair, and unpleasantness.&lt;/p&gt;&lt;p&gt;Probably the next-to-last thing you would like to read about are a harpoon gun, a rooftop sunbathing alon, two mysterious initials, three unidentified triplets, a notorious villain, and an unsavory curry.&lt;/p&gt;&lt;p&gt;Next-to-last things are the first thing to be avoided, and so allow me to recommend that you put this next-to-last book down first, and find something else to read next at last, such a s the next-to-last book in another chronicle, or a chronicle containing other next-to-last things, so that this next-to-last book does not become the last book you will read.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2005'), ('work', OrderedDict([('id', '838097'), ('uri', 'kca://work/amzn1.gr.work.v1.3aEI3fpcHODxBn9RwdHPqQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65111')])), ('isbn', '0064410145'), ('isbn13', '9780064410144'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1982')])), ('uri', 'kca://book/amzn1.gr.book.v1.YaMjhdf0gtU1qDfmuUVL-A'), ('title', 'The Grim Grotto (A Series of Unfortunate Events, #11)'), ('title_without_series', 'The Grim Grotto'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519247467l/65111._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519247467l/65111._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65111.The_Grim_Grotto'), ('num_pages', '323'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '21'), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '4.01'), ('ratings_count', '94497'), ('description', "Dear Reader, &lt;br /&gt;&lt;br /&gt;Unless you are a slug, a sea anemone, or mildew, you probably prefer not to be damp. You might also prefer not to read this book, in which the Baudelaire siblings encounter an unpleasant amount of dampness as they descend into the depths of despair, underwater. &lt;br /&gt;&lt;br /&gt;In fact, the horrors they encounter are too numerous to list, and you wouldn't want me even to mention the worst of it, which includes mushrooms, a desperate search for something lost, a mechanical monster, a distressing message from a lost friend, and tap dancing. &lt;br /&gt;&lt;br /&gt;As a dedicated author who has pledged to keep recording the depressing story of the Baudelaires, I must continue to delve deep into the cavernous depths of the orphans' lives. You, on the other hand, may delve into some happier book in order to keep your eyes and your spirits from being dampened. &lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2004'), ('work', OrderedDict([('id', '1168322'), ('uri', 'kca://work/amzn1.gr.work.v1.UtMiT7w_j77ysE78-oMoGQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '297792')])), ('isbn', '0064410137'), ('isbn13', '9780064410137'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2140')])), ('uri', 'kca://book/amzn1.gr.book.v1.KPR1e-RXoBoMpF1Wx5lRWQ'), ('title', 'The Slippery Slope (A Series of Unfortunate Events, #10)'), ('title_without_series', 'The Slippery Slope'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518835363l/297792._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518835363l/297792._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/297792.The_Slippery_Slope'), ('num_pages', '337'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '23'), ('publication_year', '2003'), ('publication_month', '9'), ('average_rating', '4.03'), ('ratings_count', '103632'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;Like handshakes, house pets, or raw carrots, many things are preferable when not slippery. Unfortunately, in this miserable volume, I am afraid that Violet, Klaus, and Sunny Baudelaire run into more than their fair share of slipperiness during their harrowing journey up--and down--a range of strange and distressing mountains.&lt;p&gt;In order to spare you any further repulsion, it would be best not to mention any of the unpleasant details of this story, particularly a secret message, a toboggan, a deceitful map, a swarm of snow gnats, a scheming villain, a troupe of organized youngsters, a covered casserole dish, and a surprising survivor of a terrible fire.&lt;/p&gt;&lt;p&gt;Unfortunately, I have dedicated my life to researching and recording the sad tale of the Baudelaire orphans. There is no reason for you to dedicate your-self to such things, and you might instead dedicate yourself to letting this slippery book slip from your hands into a nearby trash receptacle, or deep pit.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2003'), ('work', OrderedDict([('id', '2146706'), ('uri', 'kca://work/amzn1.gr.work.v1.Nidc-fP0LJc7sWuh6AE06Q')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '324277')])), ('isbn', '0064410129'), ('isbn13', '9780064410120'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2137')])), ('uri', 'kca://book/amzn1.gr.book.v1.XJc_8ov0VbLt7ak5mbAVTQ'), ('title', 'The Carnivorous Carnival (A Series of Unfortunate Events, #9)'), ('title_without_series', 'The Carnivorous Carnival'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518209848l/324277._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518209848l/324277._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/324277.The_Carnivorous_Carnival'), ('num_pages', '286'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '17'), ('publication_year', '2002'), ('publication_month', '10'), ('average_rating', '3.99'), ('ratings_count', '107023'), ('description', '&lt;i&gt;Dear reader&lt;/i&gt;,&lt;br /&gt;&lt;br /&gt;The word "carnivorous," which appears in the title of this book, means "meat-eating," and once you have read such a bloodthirsty word, there is no reason to read any further. This carnivorous volume contains such a distressing story that consuming any of its contents would be far more stomach-turning than even the most imbalanced meal.&lt;br /&gt;&lt;br /&gt;To avoid causing discomfort, it would be best if I didn\'t mention any of the unnerving ingredients of this story, particularly a confusing map, an ambidextrous person, an unruly crowd, a wooden plank, and Chabo the Wolf Baby.&lt;br /&gt;&lt;br /&gt;Sadly for me, my time is filled with researching and recording the displeasing and disenchanting lives of the Baudelaire orphans. But your time might be better filled with something more palatable, such as eating your vegetables, or feeding them to someone else.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;With all due respect&lt;/i&gt;,&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2002'), ('work', OrderedDict([('id', '984147'), ('uri', 'kca://work/amzn1.gr.work.v1.wUjMV1dlx_UGGmBmcgg3pA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '150037')])), ('isbn', '0060566221'), ('isbn13', '9780060566227'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2232')])), ('uri', 'kca://book/amzn1.gr.book.v1.MxcD0KwNfDghjb7JHgBC_A'), ('title', 'The Vile Village (A Series of Unfortunate Events, #7)'), ('title_without_series', 'The Vile Village'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352066958l/150037._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352066958l/150037._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/150037.The_Vile_Village'), ('num_pages', '272'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '24'), ('publication_year', '2001'), ('publication_month', '4'), ('average_rating', '3.96'), ('ratings_count', '117112'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;You have undoubtedly picked up this book by mistake, so please put it down. Nobody in their right mind would read this particular book about the lives of Violet, Klaus, and Sunny Baudelaire on purpose, because each dismal moment of their stay in the village of V.F.D. has been faithfully and dreadfully recorded in these pages. I can think of no single reason why anyone would want to open a book containing such unpleasant matters as migrating crows, an angry mob, a newspaper headline, the arrest of innocent people, the Deluxe Cell, and some very strange hats. It is my solemn and sacred occupation to research each detail of the Baudelaire children's lives and write them all down, but you may prefer to do some other solemn and sacred thing, such as reading another book instead.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2001'), ('work', OrderedDict([('id', '324576'), ('uri', 'kca://work/amzn1.gr.work.v1.isKFj2SwiZmAFC0l2uZ45g')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '172327')])), ('isbn', '0060566213'), ('isbn13', '9780060566210'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2603')])), ('uri', 'kca://book/amzn1.gr.book.v1.MmhTLciyQyHsKwkk-vP0sw'), ('title', 'The Ersatz Elevator (A Series of Unfortunate Events, #6)'), ('title_without_series', 'The Ersatz Elevator'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1514267383l/172327._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1514267383l/172327._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/172327.The_Ersatz_Elevator'), ('num_pages', '259'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'HarperCollins Publishers'), ('publication_day', '20'), ('publication_year', '2001'), ('publication_month', '2'), ('average_rating', '4.04'), ('ratings_count', '119503'), ('description', '&lt;p&gt;\n  &lt;i&gt;Dear Reader,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;If you have just picked up this book, then it is not too late to put it back down. Like the previous books in A SERIES OF UNFORTUNATE EVENTS, there is nothing to be found in these pages but misery, despair, and discomfort, and you still have time to choose something else to read.&lt;/p&gt;&lt;p&gt;Within the chapters of this story, Violet, Klaus and Sunny Baudelaire encounter a darkened staircase, a red herring, some friends in a dire situation, three mysterious initials, a liar with an evil scheme, a secret passageway, and parsley soda.&lt;/p&gt;&lt;p&gt;I have sworn to write down these tales of the Baudelaire orphans so the general public will know each terrible thing that has happened to them, but if you decide to read something else instead, you will save yourself from a heapful of horror and woe.&lt;/p&gt;&lt;p&gt;\n  &lt;i&gt;With all due respect,&lt;/i&gt;\n&lt;/p&gt;&lt;p&gt;Lemony Snicket&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2001'), ('work', OrderedDict([('id', '1168344'), ('uri', 'kca://work/amzn1.gr.work.v1.U9-MEJgi89OXJkBtt282vA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '131123')])), ('isbn', '0064408639'), ('isbn13', '9780064408639'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3184')])), ('uri', 'kca://book/amzn1.gr.book.v1.5IgXnU5LuMMqkeb8hJgbqQ'), ('title', 'The Austere Academy (A Series of Unfortunate Events, #5)'), ('title_without_series', 'The Austere Academy'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1517277307l/131123._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1517277307l/131123._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/131123.The_Austere_Academy'), ('num_pages', '221'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '31'), ('publication_year', '2000'), ('publication_month', '8'), ('average_rating', '3.99'), ('ratings_count', '129167'), ('description', "Dear Reader, &lt;br /&gt;&lt;br /&gt;If you are looking for a story about cheerful youngsters spending a jolly time at boarding school, look elsewhere. Violet, Klaus, and Sunny Baudelaire are intelligent and resourceful children, and you might expect that they would do very well at school. Don't. For the Baudelaires, school turns out to be another miserable episode in their unlucky lives. &lt;br /&gt;&lt;br /&gt;Truth be told, within the chapters that make up this dreadful story, the children will face snapping crabs, strict punishments, dripping fungus, comprehensive exams, violin recitals, S.O.R.E., and the metric system. &lt;br /&gt;&lt;br /&gt;It is my solemn duty to stay up all night researching and writing the history of these three hapless youngsters, but you may be more comfortable getting a good night's sleep. In that case, you should probably choose some other book. &lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1165972'), ('uri', 'kca://work/amzn1.gr.work.v1.hc5aeS0-2YZWQzvNAaFDIA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '65119')])), ('isbn', '0439272637'), ('isbn13', '9780439272636'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3174')])), ('uri', 'kca://book/amzn1.gr.book.v1.cwsqrGnBpl8pYvcEzpiWqg'), ('title', 'The Miserable Mill (A Series of Unfortunate Events, #4)'), ('title_without_series', 'The Miserable Mill'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146209l/65119._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146209l/65119._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/65119.The_Miserable_Mill'), ('num_pages', '194'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '15'), ('publication_year', '2000'), ('publication_month', '4'), ('average_rating', '3.86'), ('ratings_count', '136540'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;I hope, for your sake, that you have not chosen to read this book because you are in the mood for a pleasant experience. If this is the case, I advise you to put this book down instantaneously, because of all the books describing the unhappy lives of the Baudelaire orphans, The Miserable Mill might be the unhappiest yet. Violet, Klaus, and Sunny Baudelaire are sent to Paltryville to work in a lumber mill, and they find disaster and misfortune lurking behind every log.&lt;br /&gt;&lt;br /&gt;The pages of this book, I'm sorry to inform you, contain such unpleasantries as a giant pincher machine, a bad casserole, a man with a cloud of smoke where his head should be, a hypnotist, a terrible accident resulting in injury, and coupons.&lt;br /&gt;&lt;br /&gt;I have promised to write down the entire history of these three poor children, but you haven't, so if you prefer stories that are more heartwarming, please feel free to make another selection.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1209957'), ('uri', 'kca://work/amzn1.gr.work.v1._IQA4lfOoi-TkPbblApQ8Q')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '438492')])), ('isbn', '0064407683'), ('isbn13', '9780064407687'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '4189')])), ('uri', 'kca://book/amzn1.gr.book.v1._aUS-_mAErJpQ5eyte0BAg'), ('title', 'The Wide Window (A Series of Unfortunate Events, #3)'), ('title_without_series', 'The Wide Window'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518654331l/438492._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1518654331l/438492._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/438492.The_Wide_Window'), ('num_pages', '214'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'HarperCollins Publishers'), ('publication_day', '25'), ('publication_year', '2000'), ('publication_month', '2'), ('average_rating', '3.94'), ('ratings_count', '155708'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;If you have not read anything about the Baudelaire orphans, then before you read even one more sentence, you should know this: Violet, Klaus, and Sunny are kindhearted and quick-witted; but their lives, I am sorry to say, are filled with bad luck and misery. All of the stories about these three children are unhappy and wretched, and this one may be the worst of them all. If you haven't got the stomach for a story that includes a hurricane, a signalling device, hungry leeches, cold cucumber soup, a horrible villain, and a doll named Pretty Penny, then this book will probably fill you with despair. I will continue to record these tragic tales, for that is what I do. You, however, should decide for yourself whether you can possibly endure this miserable story.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1168377'), ('uri', 'kca://work/amzn1.gr.work.v1.X7RFHj-prALpuMXH_TqjNA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '78418')])), ('isbn', '0439206480'), ('isbn13', '9780439206488'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5266')])), ('uri', 'kca://book/amzn1.gr.book.v1.qLIM816ncARYXqU-PxgONg'), ('title', 'The Reptile Room (A Series of Unfortunate Events, #2)'), ('title_without_series', 'The Reptile Room'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146294l/78418._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1352146294l/78418._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/78418.The_Reptile_Room'), ('num_pages', '192'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '30'), ('publication_year', '1999'), ('publication_month', '9'), ('average_rating', '3.99'), ('ratings_count', '178558'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;If you have picked up this book with the hope of finding a simple and cheery tale, I'm afraid you have picked up the wrong book altogether. The story may seem cheery at first, when the Baudelaire children spend time in the company of some interesting reptiles and a giddy uncle, but don't be fooled. If you know anything at all about the unlucky Baudelaire children, you already know that even pleasant events lead down the same road to misery.&lt;br /&gt;&lt;br /&gt;In fact, within the pages you now hold in your hands, the three siblings endure a car accident, a terrible odor, a deadly serpent, a long knife, a large brass reading lamp, and the appearance of a person they'd hoped never to see again.&lt;br /&gt;&lt;br /&gt;I am bound to record these tragic events, but you are free to put this book back on the shelf and seek something lighter.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;br /&gt;Lemony Snicket"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '1999'), ('work', OrderedDict([('id', '888312'), ('uri', 'kca://work/amzn1.gr.work.v1.RFUKbJ7fsZRi9dPU8XqccQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1622')])), ('isbn', '0743477545'), ('isbn13', '9780743477543'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5831')])), ('uri', 'kca://book/amzn1.gr.book.v1.lR1AfwDypVhrjCWKj1EDUw'), ('title', "A Midsummer Night's Dream"), ('title_without_series', "A Midsummer Night's Dream"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327874534l/1622._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327874534l/1622._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1622.A_Midsummer_Night_s_Dream'), ('num_pages', '240'), ('format', 'Paperback'), ('edition_information', 'Folger Shakespeare Library'), ('publisher', 'Simon &amp; Schuster Paperbacks'), ('publication_day', None), ('publication_year', '2016'), ('publication_month', '7'), ('average_rating', '3.95'), ('ratings_count', '437767'), ('description', "Shakespeare's intertwined love polygons begin to get complicated from the start--Demetrius and Lysander both want Hermia but she only has eyes for Lysander. Bad news is, Hermia's father wants Demetrius for a son-in-law. On the outside is Helena, whose unreturned love burns hot for Demetrius. Hermia and Lysander plan to flee from the city under cover of darkness but are pursued by an enraged Demetrius (who is himself pursued by an enraptured Helena). In the forest, unbeknownst to the mortals, Oberon and Titania (King and Queen of the faeries) are having a spat over a servant boy. The plot twists up when Oberon's head mischief-maker, Puck, runs loose with a flower which causes people to fall in love with the first thing they see upon waking. Throw in a group of labourers preparing a play for the Duke's wedding (one of whom is given a donkey's head and Titania for a lover by Puck) and the complications become fantastically funny."), ('authors', OrderedDict([('author', OrderedDict([('id', '947'), ('name', 'William Shakespeare'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1586700347p5/947.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1586700347p2/947.jpg')])), ('link', 'https://www.goodreads.com/author/show/947.William_Shakespeare'), ('average_rating', '3.87'), ('ratings_count', '6204111'), ('text_reviews_count', '114442')]))])), ('published', '2016'), ('work', OrderedDict([('id', '894834'), ('uri', 'kca://work/amzn1.gr.work.v1.YiKowoSszfZ21MlDdsqApw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2156')])), ('isbn', '0192802631'), ('isbn13', '9780192802637'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '12032')])), ('uri', 'kca://book/amzn1.gr.book.v1.k8DSe52-iqTSlumfATCuOw'), ('title', 'Persuasion'), ('title_without_series', 'Persuasion'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2156.Persuasion'), ('num_pages', '249'), ('format', 'Paperback'), ('edition_information', "Oxford World's Classics"), ('publisher', 'Oxford University Press'), ('publication_day', '18'), ('publication_year', '2004'), ('publication_month', '3'), ('average_rating', '4.14'), ('ratings_count', '514564'), ('description', "Twenty-seven-year old Anne Elliot is Austen's most adult heroine. Eight years before the story proper begins, she is happily betrothed to a naval officer, Frederick Wentworth, but she precipitously breaks off the engagement when persuaded by her friend Lady Russell that such a match is unworthy. The breakup produces in Anne a deep and long-lasting regret. When later Wentworth returns from sea a rich and successful captain, he finds Anne's family on the brink of financial ruin and his own sister a tenant in Kellynch Hall, the Elliot estate. All the tension of the novel revolves around one question: Will Anne and Wentworth be reunited in their love?&lt;br /&gt;&lt;br /&gt;Jane Austen once compared her writing to painting on a little bit of ivory, 2 inches square. Readers of &lt;i&gt;Persuasion&lt;/i&gt; will discover that neither her skill for delicate, ironic observations on social custom, love, and marriage nor her ability to apply a sharp focus lens to English manners and morals has deserted her in her final finished work."), ('authors', OrderedDict([('author', OrderedDict([('id', '1265'), ('name', 'Jane Austen'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588941810p5/1265.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588941810p2/1265.jpg')])), ('link', 'https://www.goodreads.com/author/show/1265.Jane_Austen'), ('average_rating', '4.12'), ('ratings_count', '5944535'), ('text_reviews_count', '168760')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2534720'), ('uri', 'kca://work/amzn1.gr.work.v1.R7MwsnCfyHc7718MW02Mlw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '19302')])), ('isbn', '0142402494'), ('isbn13', '9780142402498'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2690')])), ('uri', 'kca://book/amzn1.gr.book.v1.ii6LisChBeRuZTUpUJ9wtQ'), ('title', 'Pippi Longstocking'), ('title_without_series', 'Pippi Longstocking'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519300455l/19302._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1519300455l/19302._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/19302.Pippi_Longstocking'), ('num_pages', '160'), ('format', 'Mass Market Paperback'), ('edition_information', 'Puffin Modern Classics, US / CAN'), ('publisher', 'Puffin Books'), ('publication_day', '21'), ('publication_year', '2005'), ('publication_month', '4'), ('average_rating', '4.13'), ('ratings_count', '164421'), ('description', 'Tommy and his sister Annika have a new neighbor, and her name is Pippi Longstocking. She has crazy red pigtails, no parents to tell her what to do, a horse that lives on her porch, and a flair for the outrageous that seems to lead to one adventure after another!&lt;br /&gt;--back cover'), ('authors', OrderedDict([('author', OrderedDict([('id', '410653'), ('name', 'Astrid Lindgren'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1194544214p5/410653.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1194544214p2/410653.jpg')])), ('link', 'https://www.goodreads.com/author/show/410653.Astrid_Lindgren'), ('average_rating', '4.18'), ('ratings_count', '345079'), ('text_reviews_count', '9813')]))])), ('published', '2005'), ('work', OrderedDict([('id', '2056462'), ('uri', 'kca://work/amzn1.gr.work.v1.E1lszyEERQLYQMtVqxoJIA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '78411')])), ('isbn', '0439206472'), ('isbn13', '9780439206471'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '13618')])), ('uri', 'kca://book/amzn1.gr.book.v1.OldE8Tvjj9nHLRUqfcPEvA'), ('title', 'The Bad Beginning (A Series of Unfortunate Events, #1)'), ('title_without_series', 'The Bad Beginning'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1436737029l/78411._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1436737029l/78411._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/78411.The_Bad_Beginning'), ('num_pages', '176'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic, Inc.'), ('publication_day', '30'), ('publication_year', '1999'), ('publication_month', '9'), ('average_rating', '3.95'), ('ratings_count', '388414'), ('description', "Dear Reader,&lt;br /&gt;&lt;br /&gt;I'm sorry to say that the book you are holding in your hands is extremely unpleasant. It tells an unhappy tale about three very unlucky children. Even though they are charming and clever, the Baudelaire siblings lead lives filled with misery and woe. From the very first page of this book when the children are at the beach and receive terrible news, continuing on through the entire story, disaster lurks at their heels. One might say they are magnets for misfortune.&lt;br /&gt;&lt;br /&gt;In this short book alone, the three youngsters encounter a greedy and repulsive villain, itchy clothing, a disastrous fire, a plot to steal their fortune, and cold porridge for breakfast.&lt;br /&gt;&lt;br /&gt;It is my sad duty to write down these unpleasant tales, but there is nothing stopping you from putting this book down at once and reading something happy, if you prefer that sort of thing.&lt;br /&gt;&lt;br /&gt;With all due respect,&lt;br /&gt;&lt;i&gt;Lemony Snicket&lt;/i&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '36746'), ('name', 'Lemony Snicket'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p5/36746.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1199734355p2/36746.jpg')])), ('link', 'https://www.goodreads.com/author/show/36746.Lemony_Snicket'), ('average_rating', '3.97'), ('ratings_count', '1964340'), ('text_reviews_count', '72116')]))])), ('published', '1999'), ('work', OrderedDict([('id', '1069597'), ('uri', 'kca://work/amzn1.gr.work.v1.OmRsXq3qTORc2Lu2Vb3xfQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '24178')])), ('isbn', '0064410935'), ('isbn13', '9780064410939'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15511')])), ('uri', 'kca://book/amzn1.gr.book.v1.-3kSw9en_4pNo5tVmbKj8g'), ('title', "Charlotte's Web"), ('title_without_series', "Charlotte's Web"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1439632243l/24178._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1439632243l/24178._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/24178.Charlotte_s_Web'), ('num_pages', '184'), ('format', 'Paperback'), ('edition_information', 'Full Color Edition'), ('publisher', 'HarperCollinsPublishers'), ('publication_day', '1'), ('publication_year', '2001'), ('publication_month', '10'), ('average_rating', '4.17'), ('ratings_count', '1385704'), ('description', 'This beloved book by E. B. White, author of &lt;i&gt;Stuart Little&lt;/i&gt; and &lt;i&gt;The Trumpet of the Swan&lt;/i&gt;, is a classic of children\'s literature that is "just about perfect." This high-quality paperback features vibrant illustrations colorized by Rosemary Wells!&lt;br /&gt;&lt;br /&gt;Some Pig. Humble. Radiant. These are the words in Charlotte\'s Web, high up in Zuckerman\'s barn. Charlotte\'s spiderweb tells of her feelings for a little pig named Wilbur, who simply wants a friend. They also express the love of a girl named Fern, who saved Wilbur\'s life when he was born the runt of his litter.&lt;br /&gt;&lt;br /&gt;E. B. White\'s Newbery Honor Book is a tender novel of friendship, love, life, and death that will continue to be enjoyed by generations to come. This edition contains newly color illustrations by Garth Williams, the acclaimed illustrator of E. B. White\'s &lt;i&gt;Stuart Little&lt;/i&gt; and Laura Ingalls Wilder\'s Little House series, among many other books.'), ('authors', OrderedDict([('author', OrderedDict([('id', '988142'), ('name', 'E.B. White'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198519412p5/988142.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198519412p2/988142.jpg')])), ('link', 'https://www.goodreads.com/author/show/988142.E_B_White'), ('average_rating', '4.15'), ('ratings_count', '1659426'), ('text_reviews_count', '28580')]))])), ('published', '2001'), ('work', OrderedDict([('id', '987048'), ('uri', 'kca://work/amzn1.gr.work.v1.cG9p_zAXsGI5Bz6-5OtD3g')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38709')])), ('isbn', '0439244196'), ('isbn13', '9780439244190'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '18202')])), ('uri', 'kca://book/amzn1.gr.book.v1.RJ9IilhRW_Pz1BbzO4_XrQ'), ('title', 'Holes (Holes, #1)'), ('title_without_series', 'Holes'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1552422497l/38709._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1552422497l/38709._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38709.Holes'), ('num_pages', '233'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic'), ('publication_day', '2'), ('publication_year', '2000'), ('publication_month', '9'), ('average_rating', '3.97'), ('ratings_count', '951377'), ('description', 'Stanley tries to dig up the truth in this inventive and darkly humorous tale of crime and punishment -- and redemption. &lt;br /&gt;&lt;br /&gt;Stanley Yelnats is under a curse. A curse that began with his no-good-dirty-rotten- pig-stealing-great-great-grandfather and has since followed generations of Yelnats. Now Stanley has been unjustly sent to a boys\' detention center, Camp Green Lake, where the warden makes the boys "build character" by spending all day, every day, digging holes: five feet wide and five feet deep. It doesn\'t take long for Stanley to realize there\'s more than character improvement going on at Camp Green Lake. The boys are digging holes because the warden is looking for something. Stanley tries to dig up the truth in this inventive and darkly humorous tale of crime and punishment—and redemption.'), ('authors', OrderedDict([('author', OrderedDict([('id', '6569'), ('name', 'Louis Sachar'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1595359600p5/6569.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1595359600p2/6569.jpg')])), ('link', 'https://www.goodreads.com/author/show/6569.Louis_Sachar'), ('average_rating', '3.99'), ('ratings_count', '1218339'), ('text_reviews_count', '33102')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1679789'), ('uri', 'kca://work/amzn1.gr.work.v1.NMFGIHdxhGf4RWZG-LLdsw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '117251')])), ('isbn', '0393315053'), ('isbn13', '9780393315059'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '237')])), ('uri', 'kca://book/amzn1.gr.book.v1.UXhE6ZhrWWsShrS2ITXPbA'), ('title', 'Hamlet: Screenplay, Introduction And Film Diary'), ('title_without_series', 'Hamlet: Screenplay, Introduction And Film Diary'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/117251.Hamlet'), ('num_pages', '224'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'W. W. Norton  Company'), ('publication_day', '17'), ('publication_year', '1996'), ('publication_month', '11'), ('average_rating', '4.14'), ('ratings_count', '181175'), ('description', 'Often credited with creating a popular movie audience for Shakespeare, Kenneth Branagh has wanted for many years to bring to the screen the complete, full-length version of &lt;em&gt;Hamlet&lt;/em&gt;, Shakespeare\'s greatest play.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;"The film, like the play, will have something for everyone," he says. "Its a ghost story, a thriller, an action-packed murder mystery, and a great tragedy that is profoundly moving." With an outstanding cast of international actors--including Derek Jacobi as Claudius, Julie Christie as Gertrude, Kate Winslet as Ophelia, Charlton Heston as the Player King, Robin Williams as Osric, and Gerard Depardieu as Reynaldo--Branagh\'s version, in which he will play the title role as well as direct, is sure to go down in film history.&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;This beautiful volume includes Branagh\'s introduction and screenplay adaptation of Shakespeare\'s text, color and black-and-white stills, and a production diary that takes us behind the scenes for a day-to-day look at the shooting of his film.'), ('authors', OrderedDict([('author', OrderedDict([('id', '55118'), ('name', 'Kenneth Branagh'), ('role', 'introduction and screenplay'), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330849315p5/55118.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330849315p2/55118.jpg')])), ('link', 'https://www.goodreads.com/author/show/55118.Kenneth_Branagh'), ('average_rating', '4.13'), ('ratings_count', '184894'), ('text_reviews_count', '1001')]))])), ('published', '1996'), ('work', OrderedDict([('id', '112914'), ('uri', 'kca://work/amzn1.gr.work.v1.fs3e5pOoUjUs95N0SU6zKA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '7624')])), ('isbn', '0140283331'), ('isbn13', '9780140283334'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '27427')])), ('uri', 'kca://book/amzn1.gr.book.v1.kSnNl4MoBUSPb-pSSfaVZQ'), ('title', 'Lord of the Flies'), ('title_without_series', 'Lord of the Flies'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327869409l/7624._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327869409l/7624._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/7624.Lord_of_the_Flies'), ('num_pages', '182'), ('format', 'Paperback'), ('edition_information', 'Penguin Great Books of the 20th Century'), ('publisher', 'Penguin Books'), ('publication_day', '1'), ('publication_year', '1999'), ('publication_month', '10'), ('average_rating', '3.68'), ('ratings_count', '2226425'), ('description', 'At the dawn of the next world war, a plane crashes on an uncharted island, stranding a group of schoolboys. At first, with no adult supervision, their freedom is something to celebrate; this far from civilization the boys can do anything they want. Anything. They attempt to forge their own society, failing, however, in the face of terror, sin and evil. And as order collapses, as strange howls echo in the night, as terror begins its reign, the hope of adventure seems as far from reality as the hope of being rescued. Labeled a parable, an allegory, a myth, a morality tale, a parody, a political treatise, even a vision of the apocalypse, Lord of the Flies is perhaps our most memorable novel about “the end of innocence, the darkness of man’s heart.”'), ('authors', OrderedDict([('author', OrderedDict([('id', '306'), ('name', 'William Golding'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198342496p5/306.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198342496p2/306.jpg')])), ('link', 'https://www.goodreads.com/author/show/306.William_Golding'), ('average_rating', '3.68'), ('ratings_count', '2246032'), ('text_reviews_count', '38138')]))])), ('published', '1999'), ('work', OrderedDict([('id', '2766512'), ('uri', 'kca://work/amzn1.gr.work.v1.mylCQ2vLQs_kZba8SrXsZg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2998')])), ('isbn', '0517189607'), ('isbn13', '9780517189603'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '12632')])), ('uri', 'kca://book/amzn1.gr.book.v1.-Yu5KHr8IQYAK0jK10dTJQ'), ('title', 'The Secret Garden'), ('title_without_series', 'The Secret Garden'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327873635l/2998._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327873635l/2998._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2998.The_Secret_Garden'), ('num_pages', '331'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', "Children's Classics"), ('publication_day', '1'), ('publication_year', '1998'), ('publication_month', '9'), ('average_rating', '4.14'), ('ratings_count', '872092'), ('description', '"One of the most delightful and enduring classics of children\'s literature, The Secret Garden by Victorian author Frances Hodgson Burnett has remained a firm favorite with children the world over ever since it made its first appearance. Initially published as a serial story in 1910 in The American Magazine, it was brought out in novel form in 1911. &lt;br /&gt; &lt;br /&gt;The plot centers round Mary Lennox, a young English girl who returns to England from India, having suffered the immense trauma by losing both her parents in a cholera epidemic. However, her memories of her parents are not pleasant, as they were a selfish, neglectful and pleasure-seeking couple. Mary is given to the care of her uncle Archibald Craven, whom she has never met. She travels to his home, Misselthwaite Manor located in the gloomy Yorkshire, a vast change from the sunny and warm climate she was used to. When she arrives, she is a rude, stubborn and given to stormy temper tantrums. However, her nature undergoes a gradual transformation when she learns of the tragedies that have befallen her strict and disciplinarian uncle whom she earlier feared and despised. Once when he\'s away from home, Mary discovers a charming walled garden which is always kept locked. The mystery deepens when she hears sounds of sobbing from somewhere within her uncle\'s vast mansion. The kindly servants ignore her queries or pretend they haven\'t heard, spiking Mary\'s curiosity. &lt;br /&gt; &lt;br /&gt;The Secret Garden appeals to both young and old alike. It has wonderful elements of mystery, spirituality, charming characters and an authentic rendering of childhood emotions and experiences. Commonsense, truth and kindness, compassion and a belief in the essential goodness of human beings lie at the heart of this unforgettable story. It is the best known of Frances Hodgson Burnett\'s works, though most of us have definitely heard of, if not read, her other novel Little Lord Fauntleroy. &lt;br /&gt; &lt;br /&gt;The book has been adapted extensively on stage, film and television and translated into all the world\'s major languages. In 1991, a Japanese anime version was launched for television in Japan. It remains a popular and beloved story of a child\'s journey into maturity, and a must-read for every child, parent, teacher and anyone who would enjoy this fascinating glimpse of childhood. One of the most delightful and enduring classics of children\'s literature, The Secret Garden by Victorian author Frances Hodgson Burnett has remained a firm favorite with children the world over ever since it made its first appearance. Initially published as a serial story in 1910 in The American Magazine, it was brought out in novel form in 1911." &lt;br /&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '2041'), ('name', 'Frances Hodgson Burnett'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1197934848p5/2041.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1197934848p2/2041.jpg')])), ('link', 'https://www.goodreads.com/author/show/2041.Frances_Hodgson_Burnett'), ('average_rating', '4.14'), ('ratings_count', '1186131'), ('text_reviews_count', '28568')]))])), ('published', '1998'), ('work', OrderedDict([('id', '3186437'), ('uri', 'kca://work/amzn1.gr.work.v1.63Qg_3M6esESm_90XodD4A')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '157993')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '24029')])), ('uri', 'kca://book/amzn1.gr.book.v1.UOzV_dE308M_I5mJxsCmsA'), ('title', 'The Little Prince'), ('title_without_series', 'The Little Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1367545443l/157993._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1367545443l/157993._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/157993.The_Little_Prince'), ('num_pages', '93'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harcourt, Inc.'), ('publication_day', '29'), ('publication_year', '2000'), ('publication_month', '6'), ('average_rating', '4.31'), ('ratings_count', '1317166'), ('description', None), ('authors', OrderedDict([('author', OrderedDict([('id', '1020792'), ('name', 'Antoine de Saint-Exupéry'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330853515p5/1020792.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1330853515p2/1020792.jpg')])), ('link', 'https://www.goodreads.com/author/show/1020792.Antoine_de_Saint_Exup_ry'), ('average_rating', '4.30'), ('ratings_count', '1352747'), ('text_reviews_count', '41269')]))])), ('published', '2000'), ('work', OrderedDict([('id', '2180358'), ('uri', 'kca://work/amzn1.gr.work.v1.F958pAbwgIwD68AA4MkC3A')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1162543')])), ('isbn', '031606792X'), ('isbn13', '9780316067928'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '43874')])), ('uri', 'kca://book/amzn1.gr.book.v1.IbwK04dpXq1GUVbwYB4SNQ'), ('title', 'Breaking Dawn (Twilight, #4)'), ('title_without_series', 'Breaking Dawn'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039438l/1162543._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039438l/1162543._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1162543.Breaking_Dawn'), ('num_pages', '756'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '2'), ('publication_year', '2008'), ('publication_month', '8'), ('average_rating', '3.70'), ('ratings_count', '1298452'), ('description', '&lt;b&gt;"Don\'t be afraid," I murmured. "We belong together."&lt;br /&gt;I was abruptly overwhelmed by the truth of my own words. &lt;br /&gt;This moment was so perfect, so right, there was no way to doubt it.&lt;br /&gt;His arms wrapped around me,&lt;br /&gt;holding me against him....&lt;br /&gt;It felt like every nerve ending in my body was a live wire.&lt;br /&gt;"Forever," he agreed.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;WHEN YOU LOVED THE ONE WHO WAS KILLING YOU, IT LEFT YOU NO OPTIONS. How could you run, how could you fight, when doing so would hurt that beloved one? If your life was all you had to give, how could you not give it? If it was someone you truly loved?&lt;br /&gt;&lt;br /&gt;TO BE IRREVOCABLY IN LOVE WITH A VAMPIRE is both fantasy and nightmare woven into a dangerously heightened reality for Bella Swan. Pulled in one direction by her intense passion for Edward Cullen, and in another by her profound connection to werewolf Jacob Black, a tumultuous year of temptation, loss, and strife have led her to the ultimate turning point. Her imminent choice to either join the dark but seductive world of immortals or to pursue a fully human life has become the thread from which the fates of two tribes hangs.&lt;br /&gt;&lt;br /&gt;NOW THAT BELLA HAS MADE HER DECISION, a startling chain of unprecedented events is about to unfold with potentially devastating, and unfathomable, consequences. Just when the frayed strands of Bella\'s life - first discovered in &lt;i&gt;Twilight&lt;/i&gt;, then scattered and torn in &lt;i&gt;New Moon&lt;/i&gt; and &lt;i&gt;Eclipse&lt;/i&gt; - seem ready to heal and knit together, could they be destroyed... forever?&lt;br /&gt;&lt;br /&gt;THE ASTONISHING, BREATHLESSLY anticipated conclusion to the Twilight Saga, &lt;i&gt;Breaking Dawn&lt;/i&gt; illuminates the secrets and mysteries of this spellbinding romantic epic that has entranced millions.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p5/941441.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p2/941441.jpg')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10625459'), ('text_reviews_count', '320367')]))])), ('published', '2008'), ('work', OrderedDict([('id', '2960529'), ('uri', 'kca://work/amzn1.gr.work.v1.xP6iGogq7HD98dx88kJDog')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '428263')])), ('isbn', '0316160202'), ('isbn13', '9780316160209'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '34329')])), ('uri', 'kca://book/amzn1.gr.book.v1.pz8Z_QjrdiX_lE1SPb4VKQ'), ('title', 'Eclipse (Twilight, #3)'), ('title_without_series', 'Eclipse'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361038355l/428263._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361038355l/428263._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/428263.Eclipse'), ('num_pages', '629'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '7'), ('publication_year', '2007'), ('publication_month', '8'), ('average_rating', '3.69'), ('ratings_count', '1397107'), ('description', '&lt;b&gt;"BELLA?"&lt;br /&gt;Edward\'s soft voice came from behind me. I turned to see him spring lightly up the porch steps, his hair windblown from running. He pulled me into his arms at once, just like he had in the parking lot, and kissed me again.&lt;br /&gt;This kiss frightened me. There was too much tension, too strong an edge to the way his lips crushed mine - like he was afraid we had only so much time left to us.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;As Seattle is ravaged by a string of mysterious killings and a malicious vampire continues her quest for revenge, Bella once again finds herself surrounded by danger. In the midst of it all, she is forced to choose between her love for Edward and her friendship with Jacob - knowing that her decision has the potential to ignite the ageless struggle between vampire and werewolf. With her graduation quickly approaching, Bella has one more decision to make: life or death. But which is which?&lt;br /&gt;&lt;br /&gt;READERS CAPTIVATED BY &lt;i&gt;Twilight&lt;/i&gt; AND &lt;i&gt;New Moon&lt;/i&gt; will eagerly devour &lt;i&gt;Eclipse&lt;/i&gt;, the much-anticipated third book in Stephenie Meyer\'s riveting vampire love saga.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p5/941441.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p2/941441.jpg')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10625459'), ('text_reviews_count', '320367')]))])), ('published', '2007'), ('work', OrderedDict([('id', '2675454'), ('uri', 'kca://work/amzn1.gr.work.v1.IwzpEvvlhAc8tuScGbwg8g')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '49041')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '42974')])), ('uri', 'kca://book/amzn1.gr.book.v1.g1Os7AXGqAOo89211CQ8sQ'), ('title', 'New Moon (Twilight, #2)'), ('title_without_series', 'New Moon'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039440l/49041._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039440l/49041._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/49041.New_Moon'), ('num_pages', '563'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Little, Brown and Company'), ('publication_day', '6'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '3.54'), ('ratings_count', '1436116'), ('description', '&lt;i&gt;There is an alternate cover edition for ISBN13 9780316160193 &lt;a href="https://www.goodreads.com/book/show/22857914" rel="nofollow"&gt;here&lt;/a&gt;.&lt;/i&gt; &lt;br /&gt;&lt;br /&gt;&lt;b&gt;I knew we were both in mortal danger. Still, in that instant, I felt &lt;i&gt;well&lt;/i&gt;. Whole. I could feel my heart racing in my chest, the blood pulsing hot and fast through my veins again. My lungs filled deep with the sweet scent that came off his skin. It was like there had never been any hole in my chest. I was perfect - not healed, but as if there had never been a wound in the first place. &lt;/b&gt;&lt;br /&gt;&lt;br /&gt;I FELT LIKE I WAS TRAPPED IN ONE OF THOSE TERRIFYING NIGHTMARES, the one where you have to run, run till your lungs burst, but you can\'t make your body move fast enough.... But this was no dream, and, unlike the nightmare, I wasn\'t running for my life; I was racing to save something infinitely more precious. My own life meant little to me today. &lt;br /&gt;&lt;br /&gt;FOR BELLA SWAN THERE IS ONE THING more important than life itself: Edward Cullen. But being in love with a vampire is even more dangerous than Bella could ever have imagined. Edward has already rescued Bella from the clutches of one evil vampire, but now, as their daring relationship threatens all that is near and dear to them, they realize their troubles may be just beginning....&lt;br /&gt;&lt;br /&gt;LEGIONS OF READERS ENTRANCED BY THE &lt;i&gt;New York Times&lt;/i&gt; bestseller &lt;i&gt;Twilight&lt;/i&gt; are hungry for the continuing story of star-crossed lovers Bell and Edward. In &lt;i&gt;New Moon&lt;/i&gt;, Stephanie Meyer delivers another irresistible combination of romance and suspense with a supernatural spin. passionate, riveting, and full of surprising twists and turns, this vampire love saga is well on its way to literary immortality.'), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p5/941441.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p2/941441.jpg')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10625459'), ('text_reviews_count', '320367')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3203964'), ('uri', 'kca://work/amzn1.gr.work.v1.1fzgJvmQrkvntdirmyYMoA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '41865')])), ('isbn', '0316015849'), ('isbn13', '9780316015844'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '96739')])), ('uri', 'kca://book/amzn1.gr.book.v1.v0ZqZFRkizei9mByA-3BpA'), ('title', 'Twilight (Twilight, #1)'), ('title_without_series', 'Twilight'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039443l/41865._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1361039443l/41865._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/41865.Twilight'), ('num_pages', '501'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Little, Brown and Company'), ('publication_day', '6'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '3.60'), ('ratings_count', '4874581'), ('description', "About three things I was absolutely positive.&lt;br /&gt;&lt;br /&gt;First, Edward was a vampire.&lt;br /&gt;&lt;br /&gt;Second, there was a part of him—and I didn't know how dominant that part might be—that thirsted for my blood.&lt;br /&gt;&lt;br /&gt;And third, I was unconditionally and irrevocably in love with him.&lt;br /&gt;&lt;br /&gt;Deeply seductive and extraordinarily suspenseful, Twilight is a love story with bite."), ('authors', OrderedDict([('author', OrderedDict([('id', '941441'), ('name', 'Stephenie Meyer'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p5/941441.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596739281p2/941441.jpg')])), ('link', 'https://www.goodreads.com/author/show/941441.Stephenie_Meyer'), ('average_rating', '3.65'), ('ratings_count', '10625459'), ('text_reviews_count', '320367')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3212258'), ('uri', 'kca://work/amzn1.gr.work.v1.f8lFp92oAIBHtSmSo4txRg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '138134')])), ('isbn', '0679601082'), ('isbn13', '9780679601081'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '198')])), ('uri', 'kca://book/amzn1.gr.book.v1.jHhIqJDxfidTucKwK0_KDA'), ('title', 'The Complete Poems'), ('title_without_series', 'The Complete Poems'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/138134.The_Complete_Poems'), ('num_pages', '416'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Modern Library'), ('publication_day', '26'), ('publication_year', '1994'), ('publication_month', '4'), ('average_rating', '4.25'), ('ratings_count', '21114'), ('description', None), ('authors', OrderedDict([('author', OrderedDict([('id', '11978'), ('name', 'John Keats'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198548090p5/11978.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1198548090p2/11978.jpg')])), ('link', 'https://www.goodreads.com/author/show/11978.John_Keats'), ('average_rating', '4.18'), ('ratings_count', '52575'), ('text_reviews_count', '2271')]))])), ('published', '1994'), ('work', OrderedDict([('id', '1701632'), ('uri', 'kca://work/amzn1.gr.work.v1.-Q9Xhp8Zo5zxZHg4prI2AQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '890')])), ('isbn', '0142000671'), ('isbn13', '9780142000670'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '26504')])), ('uri', 'kca://book/amzn1.gr.book.v1.qtwvMU3sqr2Wph0NOU770w'), ('title', 'Of Mice and Men'), ('title_without_series', 'Of Mice and Men'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1511302904l/890._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1511302904l/890._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/890.Of_Mice_and_Men'), ('num_pages', '103'), ('format', 'Paperback'), ('edition_information', 'Steinbeck Centennial Edition, US / CAN Edition'), ('publisher', 'Penguin Books'), ('publication_day', '8'), ('publication_year', '2002'), ('publication_month', '1'), ('average_rating', '3.88'), ('ratings_count', '1912522'), ('description', 'The compelling story of two outsiders striving to find their place in an unforgiving world. &lt;br /&gt;&lt;br /&gt;Drifters in search of work, George and his simple-minded friend Lennie have nothing in the world except each other and a dream -- a dream that one day they will have some land of their own. Eventually they find work on a ranch in California’s Salinas Valley, but their hopes are doomed as Lennie, struggling against extreme cruelty, misunderstanding and feelings of jealousy, becomes a victim of his own strength. &lt;br /&gt;&lt;br /&gt;Tackling universal themes such as the friendship of a shared vision, and giving voice to America’s lonely and dispossessed, &lt;i&gt;Of Mice and Men&lt;/i&gt; has proved one of Steinbeck’s most popular works, achieving success as a novel, a Broadway play and three acclaimed films.'), ('authors', OrderedDict([('author', OrderedDict([('id', '585'), ('name', 'John Steinbeck'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1182118389p5/585.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1182118389p2/585.jpg')])), ('link', 'https://www.goodreads.com/author/show/585.John_Steinbeck'), ('average_rating', '3.94'), ('ratings_count', '3696814'), ('text_reviews_count', '103956')]))])), ('published', '2002'), ('work', OrderedDict([('id', '40283'), ('uri', 'kca://work/amzn1.gr.work.v1.eBaTt5IH0gu2aaYbJLCgog')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '35031085')])), ('isbn', '0143131842'), ('isbn13', '9780143131847'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5474')])), ('uri', 'kca://book/amzn1.gr.book.v1.21GvfWvotjWsRqb6TzH_Vw'), ('title', 'Frankenstein: The 1818 Text'), ('title_without_series', 'Frankenstein: The 1818 Text'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1498841231l/35031085._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1498841231l/35031085._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/35031085-frankenstein'), ('num_pages', '288'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Penguin Classics'), ('publication_day', '8'), ('publication_year', '2018'), ('publication_month', '3'), ('average_rating', '3.80'), ('ratings_count', '1141181'), ('description', "Mary Shelley's seminal novel of the scientist whose creation becomes a monster&lt;br /&gt;&lt;br /&gt;This edition is the original 1818 text, which preserves the hard-hitting and politically charged aspects of Shelley's original writing, as well as her unflinching wit and strong female voice. This edition also includes a new introduction and suggestions for further reading by author and Shelley expert Charlotte Gordon, literary excerpts and reviews selected by Gordon and a chronology and essay by preeminent Shelley scholar Charles E. Robinson."), ('authors', OrderedDict([('author', OrderedDict([('id', '11139'), ('name', 'Mary Wollstonecraft Shelley'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588859766p5/11139.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588859766p2/11139.jpg')])), ('link', 'https://www.goodreads.com/author/show/11139.Mary_Wollstonecraft_Shelley'), ('average_rating', '3.81'), ('ratings_count', '1175409'), ('text_reviews_count', '34960')]))])), ('published', '2018'), ('work', OrderedDict([('id', '4836639'), ('uri', 'kca://work/amzn1.gr.work.v1.HYrCHs2hgbojzi9917_vCg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '136251')])), ('isbn', '0545010225'), ('isbn13', '9780545010221'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '53327')])), ('uri', 'kca://book/amzn1.gr.book.v1.J45EZhldLHRv1GBWdMc7Uw'), ('title', 'Harry Potter and the Deathly Hallows (Harry Potter, #7)'), ('title_without_series', 'Harry Potter and the Deathly Hallows'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474171184l/136251._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474171184l/136251._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/136251.Harry_Potter_and_the_Deathly_Hallows'), ('num_pages', '759'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Arthur A. Levine Books / Scholastic Inc.'), ('publication_day', '21'), ('publication_year', '2007'), ('publication_month', '7'), ('average_rating', '4.62'), ('ratings_count', '2746312'), ('description', 'Harry Potter is leaving Privet Drive for the last time. But as he climbs into the sidecar of Hagrid’s motorbike and they take to the skies, he knows Lord Voldemort and the Death Eaters will not be far behind.&lt;br /&gt;&lt;br /&gt;The protective charm that has kept him safe until now is broken. But the Dark Lord is breathing fear into everything he loves. And he knows he can’t keep hiding.&lt;br /&gt;&lt;br /&gt;To stop Voldemort, Harry knows he must find the remaining Horcruxes and destroy them.&lt;br /&gt;&lt;br /&gt;He will have to face his enemy in one final battle.&lt;br /&gt;--jkrowling.com'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2007'), ('work', OrderedDict([('id', '2963218'), ('uri', 'kca://work/amzn1.gr.work.v1.Adr1zpcHTPWrbOovOdZhlA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '29331')])), ('uri', 'kca://book/amzn1.gr.book.v1.L9KPn9NQyHxsNneS-mDWAg'), ('title', 'Harry Potter and the Half-Blood Prince (Harry Potter, #6)'), ('title_without_series', 'Harry Potter and the Half-Blood Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1587697303l/1._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1587697303l/1._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1.Harry_Potter_and_the_Half_Blood_Prince'), ('num_pages', '652'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Scholastic Inc.'), ('publication_day', '16'), ('publication_year', '2006'), ('publication_month', '9'), ('average_rating', '4.57'), ('ratings_count', '2384734'), ('description', "The war against Voldemort is not going well; even Muggle governments are noticing. Ron scans the obituary pages of the &lt;i&gt;Daily Prophet&lt;/i&gt;, looking for familiar names. Dumbledore is absent from Hogwarts for long stretches of time, and the Order of the Phoenix has already suffered losses.&lt;br /&gt;&lt;br /&gt;And yet . . .&lt;br /&gt;&lt;br /&gt;As in all wars, life goes on. The Weasley twins expand their business. Sixth-year students learn to Apparate - and lose a few eyebrows in the process. Teenagers flirt and fight and fall in love. Classes are never straightforward, through Harry receives some extraordinary help from the mysterious Half-Blood Prince.&lt;br /&gt;&lt;br /&gt;So it's the home front that takes center stage in the multilayered sixth installment of the story of Harry Potter. Here at Hogwarts, Harry will search for the full and complete story of the boy who became Lord Voldemort - and thereby find what may be his only vulnerability."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2006'), ('work', OrderedDict([('id', '41335427'), ('uri', 'kca://work/amzn1.gr.work.v1.txipecnIYua0HbI4GhIAkA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2')])), ('isbn', '0439358078'), ('isbn13', '9780439358071'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '31293')])), ('uri', 'kca://book/amzn1.gr.book.v1.uGB1cTbG_Dm5BpjL_i7pqw'), ('title', 'Harry Potter and the Order of the Phoenix (Harry Potter, #5)'), ('title_without_series', 'Harry Potter and the Order of the Phoenix'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1546910265l/2._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1546910265l/2._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2.Harry_Potter_and_the_Order_of_the_Phoenix'), ('num_pages', '870'), ('format', 'Paperback'), ('edition_information', 'US Edition'), ('publisher', 'Scholastic Inc.'), ('publication_day', None), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '4.50'), ('ratings_count', '2451895'), ('description', 'There is a door at the end of a silent corridor. And it’s haunting Harry Pottter’s dreams. Why else would he be waking in the middle of the night, screaming in terror?&lt;br /&gt;&lt;br /&gt;Harry has a lot on his mind for this, his fifth year at Hogwarts: a Defense Against the Dark Arts teacher with a personality like poisoned honey; a big surprise on the Gryffindor Quidditch team; and the looming terror of the Ordinary Wizarding Level exams. But all these things pale next to the growing threat of He-Who-Must-Not-Be-Named - a threat that neither the magical government nor the authorities at Hogwarts can stop.&lt;br /&gt;&lt;br /&gt;As the grasp of darkness tightens, Harry must discover the true depth and strength of his friends, the importance of boundless loyalty, and the shocking price of unbearable sacrifice.&lt;br /&gt;&lt;br /&gt;His fate depends on them all.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2809203'), ('uri', 'kca://work/amzn1.gr.work.v1.QBlq2dw4tPMZSuXhlMeXww')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '33563')])), ('uri', 'kca://book/amzn1.gr.book.v1.Qtinlqa0DGyf_iLtfFVrCQ'), ('title', 'Harry Potter and the Goblet of Fire (Harry Potter, #4)'), ('title_without_series', 'Harry Potter and the Goblet of Fire'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1554006152l/6._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1554006152l/6._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6.Harry_Potter_and_the_Goblet_of_Fire'), ('num_pages', '734'), ('format', 'Paperback'), ('edition_information', 'First Scholastic Trade Paperback Edition'), ('publisher', 'Scholastic'), ('publication_day', '28'), ('publication_year', '2002'), ('publication_month', '9'), ('average_rating', '4.56'), ('ratings_count', '2535141'), ('description', "Harry Potter is midway through his training as a wizard and his coming of age. Harry wants to get away from the pernicious Dursleys and go to the International Quidditch Cup with Hermione, Ron, and the Weasleys. He wants to dream about Cho Chang, his crush (and maybe do more than dream). He wants to find out about the mysterious event that's supposed to take place at Hogwarts this year, an event involving two other rival schools of magic, and a competition that hasn't happened for hundreds of years. He wants to be a normal, fourteen-year-old wizard. But unfortunately for Harry Potter, he's not normal - even by wizarding standards.&lt;br /&gt;&lt;br /&gt;And in his case, different can be deadly."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2002'), ('work', OrderedDict([('id', '3046572'), ('uri', 'kca://work/amzn1.gr.work.v1.USb5ObBtcLXUuC3i9aoelA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '15881')])), ('isbn', '0439064864'), ('isbn13', '9780439064866'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '37183')])), ('uri', 'kca://book/amzn1.gr.book.v1.KlY-hIN06yK2_7Y8_mQVig'), ('title', 'Harry Potter and the Chamber of Secrets (Harry Potter, #2)'), ('title_without_series', 'Harry Potter and the Chamber of Secrets'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474169725l/15881._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474169725l/15881._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/15881.Harry_Potter_and_the_Chamber_of_Secrets'), ('num_pages', '341'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Arthur A. Levine Books / Scholastic Inc.'), ('publication_day', '2'), ('publication_year', '1999'), ('publication_month', '6'), ('average_rating', '4.43'), ('ratings_count', '2657197'), ('description', 'Ever since Harry Potter had come home for the summer, the Dursleys had been so mean and hideous that all Harry wanted was to get back to the Hogwarts School for Witchcraft and Wizardry. But just as he’s packing his bags, Harry receives a warning from a strange impish creature who says that if Harry returns to Hogwarts, disaster will strike.&lt;br /&gt;&lt;br /&gt;And strike it does. For in Harry’s second year at Hogwarts, fresh torments and horrors arise, including an outrageously stuck-up new professor and a spirit who haunts the girls’ bathroom. But then the real trouble begins – someone is turning Hogwarts students to stone. Could it be Draco Malfoy, a more poisonous rival than ever? Could it possible be Hagrid, whose mysterious past is finally told? Or could it be the one everyone at Hogwarts most suspects… Harry Potter himself!'), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '1999'), ('work', OrderedDict([('id', '6231171'), ('uri', 'kca://work/amzn1.gr.work.v1.PjwTgn-_w5b0mY40RgNxdw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '5')])), ('isbn', '043965548X'), ('isbn13', '9780439655484'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '38917')])), ('uri', 'kca://book/amzn1.gr.book.v1.om7j-Dd6wInrhO7TVy51Ow'), ('title', 'Harry Potter and the Prisoner of Azkaban (Harry Potter, #3)'), ('title_without_series', 'Harry Potter and the Prisoner of Azkaban'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1499277281l/5._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1499277281l/5._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/5.Harry_Potter_and_the_Prisoner_of_Azkaban'), ('num_pages', '435'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Scholastic Inc.'), ('publication_day', '1'), ('publication_year', '2004'), ('publication_month', '5'), ('average_rating', '4.57'), ('ratings_count', '2733778'), ('description', "Harry Potter's third year at Hogwarts is full of new dangers. A convicted murderer, Sirius Black, has broken out of Azkaban prison, and it seems he's after Harry. Now Hogwarts is being patrolled by the dementors, the Azkaban guards who are hunting Sirius. But Harry can't imagine that Sirius or, for that matter, the evil Lord Voldemort could be more frightening than the dementors themselves, who have the terrible power to fill anyone they come across with aching loneliness and despair. Meanwhile, life continues as usual at Hogwarts. A top-of-the-line broom takes Harry's success at Quidditch, the sport of the Wizarding world, to new heights. A cute fourth-year student catches his eye. And he becomes close with the new Defense of the Dark Arts teacher, who was a childhood friend of his father. Yet despite the relative safety of life at Hogwarts and the best efforts of the dementors, the threat of Sirius Black grows ever closer. But if Harry has learned anything from his education in wizardry, it is that things are often not what they seem. Tragic revelations, heartwarming surprises, and high-stakes magical adventures await the boy wizard in this funny and poignant third installment of the beloved series.&lt;br /&gt;--scholastic.com"), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2004'), ('work', OrderedDict([('id', '2402163'), ('uri', 'kca://work/amzn1.gr.work.v1.ZkLfli5sQE5ax3qSa7235Q')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '3')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '79146')])), ('uri', 'kca://book/amzn1.gr.book.v1.tJT_00n8UPpvWa-zWHEAXg'), ('title', "Harry Potter and the Sorcerer's Stone (Harry Potter, #1)"), ('title_without_series', "Harry Potter and the Sorcerer's Stone"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474154022l/3._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1474154022l/3._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/3.Harry_Potter_and_the_Sorcerer_s_Stone'), ('num_pages', '309'), ('format', 'Hardcover'), ('edition_information', 'Library Edition'), ('publisher', 'Scholastic Inc'), ('publication_day', '1'), ('publication_year', '2003'), ('publication_month', '11'), ('average_rating', '4.47'), ('ratings_count', '6876681'), ('description', "Alternate cover edition of ISBN 9780439554930&lt;br /&gt;&lt;br /&gt;Harry Potter's life is miserable. His parents are dead and he's stuck with his heartless relatives, who force him to live in a tiny closet under the stairs. But his fortune changes when he receives a letter that tells him the truth about himself: he's a wizard. A mysterious visitor rescues him from his relatives and takes him to his new home, Hogwarts School of Witchcraft and Wizardry.&lt;br /&gt;&lt;br /&gt;After a lifetime of bottling up his magical powers, Harry finally feels like a normal kid. But even within the Wizarding community, he is special. He is the boy who lived: the only person to have ever survived a killing curse inflicted by the evil Lord Voldemort, who launched a brutal takeover of the Wizarding world, only to vanish after failing to kill Harry.&lt;br /&gt;&lt;br /&gt;Though Harry's first year at Hogwarts is the best of his life, not everything is perfect. There is a dangerous secret object hidden within the castle walls, and Harry believes it's his responsibility to prevent it from falling into evil hands. But doing so will bring him into contact with forces more terrifying than he ever could have imagined.&lt;br /&gt;&lt;br /&gt;Full of sympathetic characters, wildly imaginative situations, and countless exciting details, the first installment in the series assembles an unforgettable magical world and sets the stage for many high-stakes adventures to come."), ('authors', OrderedDict([('author', OrderedDict([('id', '1077326'), ('name', 'J.K. Rowling'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p5/1077326.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596216614p2/1077326.jpg')])), ('link', 'https://www.goodreads.com/author/show/1077326.J_K_Rowling'), ('average_rating', '4.46'), ('ratings_count', '25151657'), ('text_reviews_count', '577132')]))])), ('published', '2003'), ('work', OrderedDict([('id', '4640799'), ('uri', 'kca://work/amzn1.gr.work.v1.TbpxJa2CwiSSz_9W2FruoA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40940121')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1423')])), ('uri', 'kca://book/amzn1.gr.book.v1.itZyR1Fk_Ix0XJXvaEPHLg'), ('title', 'Bridge to Terabithia'), ('title_without_series', 'Bridge to Terabithia'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532478367l/40940121._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532478367l/40940121._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40940121-bridge-to-terabithia'), ('num_pages', '190'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'HarperCollins'), ('publication_day', '6'), ('publication_year', '2009'), ('publication_month', '10'), ('average_rating', '4.01'), ('ratings_count', '436239'), ('description', "Jess Aarons' greatest ambition is to be the fastest runner in his grade. He's been practicing all summer and can't wait to see his classmates' faces when he beats them all. But on the first day of school, a new girl boldly crosses over to the boys' side and outruns everyone.&lt;br /&gt;&lt;br /&gt;That's not a very promising beginning for a friendship, but Jess and Leslie Burke become inseparable. Together they create Terabithia, a magical kingdom in the woods where the two of them reign as king and queen, and their imaginations set the only limits."), ('authors', OrderedDict([('author', OrderedDict([('id', '1949'), ('name', 'Katherine Paterson'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1595481183p5/1949.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1595481183p2/1949.jpg')])), ('link', 'https://www.goodreads.com/author/show/1949.Katherine_Paterson'), ('average_rating', '3.97'), ('ratings_count', '515596'), ('text_reviews_count', '19229')]))])), ('published', '2009'), ('work', OrderedDict([('id', '2237401'), ('uri', 'kca://work/amzn1.gr.work.v1.zzEPgoJCNWRJZ6AuRm8EeQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17158513')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2273')])), ('uri', 'kca://book/amzn1.gr.book.v1.TcadId_zixkpux9JQfySwA'), ('title', 'Captive Prince: Volume Two (Captive Prince, #2)'), ('title_without_series', 'Captive Prince: Volume Two'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356027904l/17158513._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356027904l/17158513._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17158513-captive-prince'), ('num_pages', '216'), ('format', 'ebook'), ('edition_information', None), ('publisher', None), ('publication_day', None), ('publication_year', '2012'), ('publication_month', None), ('average_rating', '4.43'), ('ratings_count', '39325'), ('description', 'With their countries on the brink of war, Damen and his new master, Prince Laurent, must exchange the intrigues of the palace for the sweeping might of the battlefield as they travel to the border to avert a lethal plot.&lt;br /&gt;&lt;br /&gt;Forced to hide his identity, Damen finds himself increasingly drawn to the dangerous, charismatic Laurent. But as the fledgling trust between the two men deepens, the truth of secrets from both their pasts is poised to deal them the crowning death blow . . .'), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '195235'), ('text_reviews_count', '25949')]))])), ('published', '2012'), ('work', OrderedDict([('id', '23581952'), ('uri', 'kca://work/amzn1.gr.work.v1.aY-h5auqNU0sOr_bcd1WSw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '17158532')])), ('isbn', '174348495X'), ('isbn13', '9781743484951'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3183')])), ('uri', 'kca://book/amzn1.gr.book.v1.tzJZCfUkGUT1Wy3DGs6PqA'), ('title', 'Kings Rising (Captive Prince, #3)'), ('title_without_series', 'Kings Rising'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1454160767l/17158532._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1454160767l/17158532._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/17158532-kings-rising'), ('num_pages', '385'), ('format', 'ebook'), ('edition_information', None), ('publisher', 'Penguin Group Australia'), ('publication_day', '2'), ('publication_year', '2016'), ('publication_month', '2'), ('average_rating', '4.46'), ('ratings_count', '33776'), ('description', "&lt;i&gt;Damianos of Akielos has returned&lt;/i&gt;.&lt;br /&gt; &lt;br /&gt;His identity now revealed, Damen must face his master Prince Laurent as Damianos of Akielos, the man Laurent has sworn to kill.&lt;br /&gt; &lt;br /&gt;On the brink of a momentous battle, the future of both their countries hangs in the balance. In the south, Kastor’s forces are massing. In the north, the Regent’s armies are mobilising for war. Damen’s only hope of reclaiming his throne is to fight together with Laurent against their usurpers.&lt;br /&gt; &lt;br /&gt;Forced into an uneasy alliance the two princes journey deep into Akielos, where they face their most dangerous opposition yet. But even if the fragile trust they have built survives the revelation of Damen’s identity—can it stand against the Regent's final, deadly play for the throne?"), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '195235'), ('text_reviews_count', '25949')]))])), ('published', '2016'), ('work', OrderedDict([('id', '23581990'), ('uri', 'kca://work/amzn1.gr.work.v1.-_QRlY1zWL90hb8zqfcwlg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1618')])), ('isbn', '1400032717'), ('isbn13', '9781400032716'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '36537')])), ('uri', 'kca://book/amzn1.gr.book.v1.-HbDY4-Aoh2zmGKIXjEwKg'), ('title', 'The Curious Incident of the Dog in the Night-Time'), ('title_without_series', 'The Curious Incident of the Dog in the Night-Time'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1479863624l/1618._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1479863624l/1618._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1618.The_Curious_Incident_of_the_Dog_in_the_Night_Time'), ('num_pages', '226'), ('format', 'Paperback'), ('edition_information', 'Vintage Contemporaries'), ('publisher', 'Vintage'), ('publication_day', '18'), ('publication_year', '2004'), ('publication_month', '5'), ('average_rating', '3.88'), ('ratings_count', '1172256'), ('description', "Christopher John Francis Boone knows all the countries of the world and their capitals and every prime number up to 7,057. He relates well to animals but has no understanding of human emotions. He cannot stand to be touched. And he detests the color yellow.&lt;br /&gt;&lt;br /&gt;Although gifted with a superbly logical brain, for fifteen-year-old Christopher everyday interactions and admonishments have little meaning. He lives on patterns, rules, and a diagram kept in his pocket. Then one day, a neighbor's dog, Wellington, is killed and his carefully constructive universe is threatened. Christopher sets out to solve the murder in the style of his favourite (logical) detective, Sherlock Holmes. What follows makes for a novel that is funny, poignant and fascinating in its portrayal of a person whose curse and blessing are a mind that perceives the world entirely literally."), ('authors', OrderedDict([('author', OrderedDict([('id', '1050'), ('name', 'Mark Haddon'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1337988298p5/1050.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1337988298p2/1050.jpg')])), ('link', 'https://www.goodreads.com/author/show/1050.Mark_Haddon'), ('average_rating', '3.86'), ('ratings_count', '1235723'), ('text_reviews_count', '51660')]))])), ('published', '2004'), ('work', OrderedDict([('id', '4259809'), ('uri', 'kca://work/amzn1.gr.work.v1.8XQyL2-mXgV1VRh3euWYmw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '7260188')])), ('isbn', '0439023513'), ('isbn13', '9780439023511'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '91823')])), ('uri', 'kca://book/amzn1.gr.book.v1.hFVPFpO-8DyF11Gy1k4d7A'), ('title', 'Mockingjay (The Hunger Games, #3)'), ('title_without_series', 'Mockingjay'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722918l/7260188._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722918l/7260188._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/7260188-mockingjay'), ('num_pages', '390'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '24'), ('publication_year', '2010'), ('publication_month', '8'), ('average_rating', '4.04'), ('ratings_count', '2300381'), ('description', "The final book in the ground-breaking HUNGER GAMES trilogy, this new foiled edition of MOCKINGJAY is available for a limited period of time. Against all odds, Katniss Everdeen has survived the Hunger Games twice. But now that she's made it out of the bloody arena alive, she's still not safe. The Capitol is angry. The Capitol wants revenge. Who do they think should pay for the unrest? Katniss. And what's worse, President Snow has made it clear that no one else is safe either. Not Katniss's family, not her friends, not the people of District 12."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p5/153394.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p2/153394.jpg')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11583768'), ('text_reviews_count', '408035')]))])), ('published', '2010'), ('work', OrderedDict([('id', '8812783'), ('uri', 'kca://work/amzn1.gr.work.v1.4IASwwiLmBwCmDcIe56XuQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6148028')])), ('isbn', '0439023491'), ('isbn13', '9780439023498'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '85732')])), ('uri', 'kca://book/amzn1.gr.book.v1.c5JlFHJrTIJY5yfmJN8b0w'), ('title', 'Catching Fire (The Hunger Games, #2)'), ('title_without_series', 'Catching Fire'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722941l/6148028._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722941l/6148028._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6148028-catching-fire'), ('num_pages', '391'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '1'), ('publication_year', '2009'), ('publication_month', '9'), ('average_rating', '4.29'), ('ratings_count', '2456946'), ('description', "&lt;b&gt;SPARKS ARE IGNITING.&lt;br /&gt;FLAMES ARE SPREADING.&lt;br /&gt;AND THE CAPITAL WANTS REVENGE.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;Against all odds, Katniss Everdeen has survived the Hunger Games. She and fellow District 12 tribute Peeta Mellark are miraculously still alive. Katniss should be relieved, happy even. Yet nothing is the way Katniss wishes it to be. Gale holds her at an icy distance. Peeta has turned his back on her completely. And there are whispers of a rebellion against the Capitol - a rebellion that Katniss and Peeta may have helped create.&lt;br /&gt;&lt;br /&gt;Much to her shock, Katniss has fueled an unrest that she's afraid she cannot stop. And what scares her even more is that she's not entirely convinced she should try. As time draws near for Katniss and Peeta to visit the districts on the Capitol's cruel Victory Tour, the stakes are higher than ever. If they can't prove, without a shadow of a doubt, that they are lost in their love for each other, the consequences will be horrifying. Katniss is about to be tested as never before."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p5/153394.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p2/153394.jpg')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11583768'), ('text_reviews_count', '408035')]))])), ('published', '2009'), ('work', OrderedDict([('id', '6171458'), ('uri', 'kca://work/amzn1.gr.work.v1.2o2efDDMSYr-E3ruRr1VcA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2767052')])), ('isbn', '0439023483'), ('isbn13', '9780439023481'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '153950')])), ('uri', 'kca://book/amzn1.gr.book.v1.YaoKZD8xVx72w5T1ZgR1YQ'), ('title', 'The Hunger Games (The Hunger Games, #1)'), ('title_without_series', 'The Hunger Games'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722975l/2767052._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1586722975l/2767052._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2767052-the-hunger-games'), ('num_pages', '374'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Scholastic Press'), ('publication_day', '14'), ('publication_year', '2008'), ('publication_month', '9'), ('average_rating', '4.33'), ('ratings_count', '6267760'), ('description', "&lt;b&gt;WINNING MEANS FAME AND FORTUNE.&lt;br /&gt;LOSING MEANS CERTAIN DEATH.&lt;br /&gt;THE HUNGER GAMES HAVE BEGUN. . . .&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;In the ruins of a place once known as North America lies the nation of Panem, a shining Capitol surrounded by twelve outlying districts. The Capitol is harsh and cruel and keeps the districts in line by forcing them all to send one boy and once girl between the ages of twelve and eighteen to participate in the annual Hunger Games, a fight to the death on live TV.&lt;br /&gt;&lt;br /&gt;Sixteen-year-old Katniss Everdeen regards it as a death sentence when she steps forward to take her sister's place in the Games. But Katniss has been close to dead before—and survival, for her, is second nature. Without really meaning to, she becomes a contender. But if she is to win, she will have to start making choices that weight survival against humanity and life against love."), ('authors', OrderedDict([('author', OrderedDict([('id', '153394'), ('name', 'Suzanne Collins'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p5/153394.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1596499132p2/153394.jpg')])), ('link', 'https://www.goodreads.com/author/show/153394.Suzanne_Collins'), ('average_rating', '4.26'), ('ratings_count', '11583768'), ('text_reviews_count', '408035')]))])), ('published', '2008'), ('work', OrderedDict([('id', '2792775'), ('uri', 'kca://work/amzn1.gr.work.v1.qDM8aVuWTQKRymQBUS02og')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '5659')])), ('isbn', '0143039091'), ('isbn13', '9780143039099'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3710')])), ('uri', 'kca://book/amzn1.gr.book.v1.Y6Tj1XDUHYcT9fle4yewtg'), ('title', 'The Wind in the Willows'), ('title_without_series', 'The Wind in the Willows'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423183570l/5659._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423183570l/5659._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/5659.The_Wind_in_the_Willows'), ('num_pages', '197'), ('format', 'Paperback'), ('edition_information', 'Penguin Classics'), ('publisher', 'Penguin Books'), ('publication_day', '27'), ('publication_year', '2005'), ('publication_month', '10'), ('average_rating', '3.99'), ('ratings_count', '174738'), ('description', '"There is nothing half so much worth doing as simply messing around in boats."&lt;br /&gt;&lt;br /&gt;When Mole flees his little underground home he discovers new friends and adventures with Raj, Toad and Badger.&lt;br /&gt;&lt;br /&gt;This much-loved story has been carefully retold for young children to enjoy. With beautiful illustrations throughout, it provides the perfect introduction to a classic tale.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3843'), ('name', 'Kenneth Grahame'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201018750p5/3843.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201018750p2/3843.jpg')])), ('link', 'https://www.goodreads.com/author/show/3843.Kenneth_Grahame'), ('average_rating', '3.99'), ('ratings_count', '185986'), ('text_reviews_count', '6837')]))])), ('published', '2005'), ('work', OrderedDict([('id', '1061285'), ('uri', 'kca://work/amzn1.gr.work.v1.yTxsyacrG8lEOhoyMEh2aw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1852')])), ('isbn', '0439227143'), ('isbn13', '9780439227148'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7902')])), ('uri', 'kca://book/amzn1.gr.book.v1.N3Hj-jJMvOmCMWeUygmRPw'), ('title', 'The Call of the Wild'), ('title_without_series', 'The Call of the Wild'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1452291694l/1852._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1452291694l/1852._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1852.The_Call_of_the_Wild'), ('num_pages', '172'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Scholastic'), ('publication_day', '1'), ('publication_year', '2001'), ('publication_month', '1'), ('average_rating', '3.87'), ('ratings_count', '333019'), ('description', "First published in 1903, &lt;i&gt;The Call of the Wild&lt;/i&gt; is regarded as Jack London's masterpiece. Based on London's experiences as a gold prospector in the Canadian wilderness and his ideas about nature and the struggle for existence, &lt;i&gt;The Call of the Wild&lt;/i&gt; is a tale about unbreakable spirit and the fight for survival in the frozen Alaskan Klondike."), ('authors', OrderedDict([('author', OrderedDict([('id', '1240'), ('name', 'Jack London'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1508674808p5/1240.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1508674808p2/1240.jpg')])), ('link', 'https://www.goodreads.com/author/show/1240.Jack_London'), ('average_rating', '3.96'), ('ratings_count', '738753'), ('text_reviews_count', '26503')]))])), ('published', '2001'), ('work', OrderedDict([('id', '3252320'), ('uri', 'kca://work/amzn1.gr.work.v1.nZyZdlJnNCISNRPQkGznZw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '295')])), ('isbn', '0753453800'), ('isbn13', '9780753453803'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7192')])), ('uri', 'kca://book/amzn1.gr.book.v1.NMDBN_fq2yR6xaC4HcPWOw'), ('title', 'Treasure Island'), ('title_without_series', 'Treasure Island'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485248909l/295._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485248909l/295._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/295.Treasure_Island'), ('num_pages', '311'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Kingfisher'), ('publication_day', '15'), ('publication_year', '2001'), ('publication_month', '9'), ('average_rating', '3.83'), ('ratings_count', '393345'), ('description', '"For sheer storytelling delight and pure adventure, &lt;i&gt;Treasure Island&lt;/i&gt; has never been surpassed. From the moment young Jim Hawkins first encounters the sinister Blind Pew at the Admiral Benbow Inn until the climactic battle for treasure on a tropic isle, the novel creates scenes and characters that have fired the imaginations of generations of readers. Written by a superb prose stylist, a master of both action and atmosphere, the story centers upon the conflict between good and evil - but in this case a particularly engaging form of evil. It is the villainy of that most ambiguous rogue Long John Silver that sets the tempo of this tale of treachery, greed, and daring. Designed to forever kindle a dream of high romance and distant horizons, &lt;i&gt;Treasure Island&lt;/i&gt; is, in the words of G. K. Chesterton, \'the realization of an ideal, that which is promised in its provocative and beckoning map; a vision not only of white skeletons but also green palm trees and sapphire seas.\' G. S. Fraser terms it \'an utterly original book\' and goes on to write: \'There will always be a place for stories like &lt;i&gt;Treasure Island&lt;/i&gt; that can keep boys and old men happy.\''), ('authors', OrderedDict([('author', OrderedDict([('id', '854076'), ('name', 'Robert Louis Stevenson'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192746024p5/854076.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192746024p2/854076.jpg')])), ('link', 'https://www.goodreads.com/author/show/854076.Robert_Louis_Stevenson'), ('average_rating', '3.85'), ('ratings_count', '1085852'), ('text_reviews_count', '36055')]))])), ('published', '2001'), ('work', OrderedDict([('id', '3077988'), ('uri', 'kca://work/amzn1.gr.work.v1.jmdkybKCkfrZq5SG8p4pNg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '236093')])), ('isbn', '0140621679'), ('isbn13', '9780140621679'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7676')])), ('uri', 'kca://book/amzn1.gr.book.v1.UivhNgteUMaLX0zsj4Y5Hw'), ('title', 'The Wonderful Wizard of Oz (Oz, #1)'), ('title_without_series', 'The Wonderful Wizard of Oz'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1398003737l/236093._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1398003737l/236093._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/236093.The_Wonderful_Wizard_of_Oz'), ('num_pages', '154'), ('format', 'Paperback'), ('edition_information', 'Penguin Popular Classics'), ('publisher', 'Penguin'), ('publication_day', None), ('publication_year', '1995'), ('publication_month', None), ('average_rating', '3.99'), ('ratings_count', '359526'), ('description', 'When Dorothy and her little dog Toto are caught in a tornado, they and their Kansas farmhouse are suddenly transported to Oz, where Munchkins live, monkeys fly and Wicked Witches rule. Desperate to return home, and with the Wicked Witch of the West on their trail, Dorothy and Toto - together with new friends the Tin Woodsman, Scarecrow and cowardly Lion - embark on a fantastic quest along the Yellow Brick Road in search of the Emerald City. There they hope to meet the legendary, all-powerful Wizard of Oz, who alone may hold the power to grant their every wish.&lt;br /&gt;&lt;br /&gt;Just as captivating as it was a hundred years ago, this is a story that all ages will love.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3242'), ('name', 'L. Frank Baum'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1383720421p5/3242.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1383720421p2/3242.jpg')])), ('link', 'https://www.goodreads.com/author/show/3242.L_Frank_Baum'), ('average_rating', '3.97'), ('ratings_count', '555210'), ('text_reviews_count', '22809')]))])), ('published', '1995'), ('work', OrderedDict([('id', '1993810'), ('uri', 'kca://work/amzn1.gr.work.v1.Brq5W1RwLwTS7yX4kPgQNQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '93')])), ('isbn', '0753454947'), ('isbn13', '9780753454947'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2401')])), ('uri', 'kca://book/amzn1.gr.book.v1.62w6yF6ljGRIHf98OEYAfQ'), ('title', 'Heidi (Heidi, #1-2)'), ('title_without_series', 'Heidi'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/93.Heidi'), ('num_pages', '352'), ('format', 'Paperback'), ('edition_information', 'Kingfisher Classics'), ('publisher', 'Kingfisher'), ('publication_day', '15'), ('publication_year', '2002'), ('publication_month', '11'), ('average_rating', '3.99'), ('ratings_count', '170382'), ('description', 'Little orphan Heidi goes to live high in the Alps with her gruff grandfather and brings happiness to all who know her on the mountain. When Heidi goes to Frankfurt to work in a wealthy household, she dreams of returning to the mountains and meadows, her friend Peter, and her beloved grandfather.'), ('authors', OrderedDict([('author', OrderedDict([('id', '49'), ('name', 'Johanna Spyri'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201029829p5/49.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1201029829p2/49.jpg')])), ('link', 'https://www.goodreads.com/author/show/49.Johanna_Spyri'), ('average_rating', '4.00'), ('ratings_count', '187322'), ('text_reviews_count', '4446')]))])), ('published', '2002'), ('work', OrderedDict([('id', '1738595'), ('uri', 'kca://work/amzn1.gr.work.v1.vupk7zK34JDihBVCwsZlrw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '8127')])), ('isbn', '0451528824'), ('isbn13', '9780451528827'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '15026')])), ('uri', 'kca://book/amzn1.gr.book.v1.srpZjZlpcE9dl03dhQOy8w'), ('title', 'Anne of Green Gables (Anne of Green Gables, #1)'), ('title_without_series', 'Anne of Green Gables'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/8127.Anne_of_Green_Gables'), ('num_pages', '320'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Signet Book'), ('publication_day', '6'), ('publication_year', '2003'), ('publication_month', '5'), ('average_rating', '4.26'), ('ratings_count', '709980'), ('description', "As soon as Anne Shirley arrives at the snug white farmhouse called Green Gables, she is sure she wants to stay forever . . . but will the Cuthberts send her back to to the orphanage? Anne knows she's not what they expected—a skinny girl with fiery red hair and a temper to match. If only she can convince them to let her stay, she'll try very hard not to keep rushing headlong into scrapes and blurting out the first thing that comes to her mind. Anne is not like anyone else, the Cuthberts agree; she is special—a girl with an enormous imagination. This orphan girl dreams of the day when she can call herself Anne of Green Gables."), ('authors', OrderedDict([('author', OrderedDict([('id', '5350'), ('name', 'L.M. Montgomery'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1188896723p5/5350.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1188896723p2/5350.jpg')])), ('link', 'https://www.goodreads.com/author/show/5350.L_M_Montgomery'), ('average_rating', '4.22'), ('ratings_count', '1595196'), ('text_reviews_count', '55935')]))])), ('published', '2003'), ('work', OrderedDict([('id', '3464264'), ('uri', 'kca://work/amzn1.gr.work.v1.s7yrHLy8bDalH9w11O-zTQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1934')])), ('isbn', '0451529308'), ('isbn13', '9780451529305'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '21068')])), ('uri', 'kca://book/amzn1.gr.book.v1.AMKxo9pbFFRBV4qA6jnIYQ'), ('title', 'Little Women'), ('title_without_series', 'Little Women'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1562690475l/1934._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1562690475l/1934._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1934.Little_Women'), ('num_pages', '449'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Signet Classics'), ('publication_day', '6'), ('publication_year', '2004'), ('publication_month', '4'), ('average_rating', '4.08'), ('ratings_count', '1650892'), ('description', 'Generations of readers young and old, male and female, have fallen in love with the March sisters of Louisa May Alcott’s most popular and enduring novel, &lt;i&gt;Little Women&lt;/i&gt;. Here are talented tomboy and author-to-be Jo, tragically frail Beth, beautiful Meg, and romantic, spoiled Amy, united in their devotion to each other and their struggles to survive in New England during the Civil War.&lt;br /&gt;&lt;p&gt;It is no secret that Alcott based &lt;i&gt;Little Women&lt;/i&gt; on her own early life. While her father, the freethinking reformer and abolitionist Bronson Alcott, hobnobbed with such eminent male authors as Emerson, Thoreau, and Hawthorne, Louisa supported herself and her sisters with "woman’s work,” including sewing, doing laundry, and acting as a domestic servant. But she soon discovered she could make more money writing. &lt;i&gt;Little Women&lt;/i&gt; brought her lasting fame and fortune, and far from being the "girl’s book” her publisher requested, it explores such timeless themes as love and death, war and peace, the conflict between personal ambition and family responsibilities, and the clash of cultures between Europe and America.&lt;/p&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '1315'), ('name', 'Louisa May Alcott'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1200326665p5/1315.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1200326665p2/1315.jpg')])), ('link', 'https://www.goodreads.com/author/show/1315.Louisa_May_Alcott'), ('average_rating', '4.06'), ('ratings_count', '1910053'), ('text_reviews_count', '43795')]))])), ('published', '2004'), ('work', OrderedDict([('id', '3244642'), ('uri', 'kca://work/amzn1.gr.work.v1.d2eQgjlqgwEpanKeHkUAgw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '43822024')])), ('isbn', '1481497065'), ('isbn13', '9781481497060'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '5852')])), ('uri', 'kca://book/amzn1.gr.book.v1.7OM3tkgHAmqpnWaIkl3PMA'), ('title', 'The Toll (Arc of a Scythe, #3)'), ('title_without_series', 'The Toll'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558117336l/43822024._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558117336l/43822024._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/43822024-the-toll'), ('num_pages', '625'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon &amp; Schuster Books for Young Readers'), ('publication_day', '5'), ('publication_year', '2019'), ('publication_month', '11'), ('average_rating', '4.27'), ('ratings_count', '37347'), ('description', 'It’s been three years since Rowan and Citra disappeared; since Scythe Goddard came into power; since the Thunderhead closed itself off to everyone but Grayson Tolliver.&lt;br /&gt;&lt;br /&gt;In this pulse-pounding conclusion to &lt;i&gt;New York Times &lt;/i&gt;bestselling author Neal Shusterman’s Arc of a Scythe trilogy, constitutions are tested and old friends are brought back from the dead.'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '686511'), ('text_reviews_count', '89671')]))])), ('published', '2019'), ('work', OrderedDict([('id', '59222476'), ('uri', 'kca://work/amzn1.gr.work.v1.pJ1XvuR9ZysrKirtcMVmFA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '1696832')])), ('isbn', '1405450509'), ('isbn13', '9781405450508'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '16')])), ('uri', 'kca://book/amzn1.gr.book.v1.64kJoRdr3znWUxZmSCO-Pg'), ('title', 'Beers of the World'), ('title_without_series', 'Beers of the World'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/1696832.Beers_of_the_World'), ('num_pages', None), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Parragon Publishing'), ('publication_day', '1'), ('publication_year', '2005'), ('publication_month', '11'), ('average_rating', '3.64'), ('ratings_count', '103'), ('description', None), ('authors', OrderedDict([('author', OrderedDict([('id', '781570'), ('name', 'David Kenning'), ('role', 'Creator'), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/781570.David_Kenning'), ('average_rating', '3.56'), ('ratings_count', '122'), ('text_reviews_count', '21')]))])), ('published', '2005'), ('work', OrderedDict([('id', '1693795'), ('uri', 'kca://work/amzn1.gr.work.v1.CKgueeRMrVBTWuSsun1TyQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '45714170')])), ('isbn', '1406375500'), ('isbn13', '9781406375503'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '299')])), ('uri', 'kca://book/amzn1.gr.book.v1.SJ0DJBotk0KBV2R7Hodmvg'), ('title', 'Burn'), ('title_without_series', 'Burn'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1571075314l/45714170._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1571075314l/45714170._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/45714170-burn'), ('num_pages', '384'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Walker Books'), ('publication_day', '2'), ('publication_year', '2020'), ('publication_month', '6'), ('average_rating', '3.90'), ('ratings_count', '2236'), ('description', "In 1956 Sarah Dewhurst's father shocks her by hiring a dragon to work the farm. The dragon is a smaller blue rather than the traditional larger reds, though even the reds are now scarce. When the blue dragon, Kazimir, unexpectedly saves Sarah and her friend Jason Inagawa from the attentions of the racist police deputy, Kelby, everything changes. Sarah is part of a prophecy and she must escape the clutches of Malcolm, an assassin from a Believer Cell, the dragon-worshiping cult. When Sarah, Malcolm, and Kazimir eventually converge, they are thrown into another universe, where dragons seem never to have existed. Can they save this world and the one they left?"), ('authors', OrderedDict([('author', OrderedDict([('id', '370361'), ('name', 'Patrick Ness'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p5/370361.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p2/370361.jpg')])), ('link', 'https://www.goodreads.com/author/show/370361.Patrick_Ness'), ('average_rating', '4.12'), ('ratings_count', '636355'), ('text_reviews_count', '87548')]))])), ('published', '2020'), ('work', OrderedDict([('id', '70488386'), ('uri', 'kca://work/amzn1.gr.work.v1.aWmQvrbF9XEnGSR-EcfpqA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '31194576')])), ('isbn', '1406377279'), ('isbn13', '9781406377279'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1962')])), ('uri', 'kca://book/amzn1.gr.book.v1.4KQFkkhwyf4ECNZYLNkUBw'), ('title', 'Release'), ('title_without_series', 'Release'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485454954l/31194576._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1485454954l/31194576._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/31194576-release'), ('num_pages', '287'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Walker Books'), ('publication_day', '4'), ('publication_year', '2017'), ('publication_month', '5'), ('average_rating', '3.70'), ('ratings_count', '14170'), ('description', 'It’s Saturday, it’s summer and, although he doesn’t know it yet, everything in Adam Thorn’s life is going to fall apart. Relationships will change, he’ll change, but maybe, just maybe, he’ll find freedom in the release.&lt;br /&gt;&lt;br /&gt;Time is running out though, because way across town a ghost as risen from the lake. Searching, yearning, she leaves a trail of destruction in her wake…'), ('authors', OrderedDict([('author', OrderedDict([('id', '370361'), ('name', 'Patrick Ness'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p5/370361.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1589369436p2/370361.jpg')])), ('link', 'https://www.goodreads.com/author/show/370361.Patrick_Ness'), ('average_rating', '4.12'), ('ratings_count', '636355'), ('text_reviews_count', '87548')]))])), ('published', '2017'), ('work', OrderedDict([('id', '51840657'), ('uri', 'kca://work/amzn1.gr.work.v1.xigxG5wUTMZ4EMpqIofCbg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '33555224')])), ('isbn', '1442472456'), ('isbn13', '9781442472457'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9379')])), ('uri', 'kca://book/amzn1.gr.book.v1.vY1B_oebTKCZxjW7sZRB-Q'), ('title', 'Thunderhead (Arc of a Scythe, #2)'), ('title_without_series', 'Thunderhead'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1505658534l/33555224._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1505658534l/33555224._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/33555224-thunderhead'), ('num_pages', '504'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon &amp; Schuster Books for Young Readers'), ('publication_day', '9'), ('publication_year', '2018'), ('publication_month', '1'), ('average_rating', '4.48'), ('ratings_count', '67905'), ('description', 'Rowan has gone rogue, and has taken it upon himself to put the Scythedom through a trial by fire. Literally. In the year since Winter Conclave, he has gone off-grid, and has been striking out against corrupt scythes—not only in MidMerica, but across the entire continent. He is a dark folk hero now—“Scythe Lucifer”—a vigilante taking down corrupt scythes in flames.&lt;br /&gt;&lt;br /&gt;Citra, now a junior scythe under Scythe Curie, sees the corruption and wants to help change it from the inside out, but is thwarted at every turn, and threatened by the “new order” scythes. Realizing she cannot do this alone—or even with the help of Scythe Curie and Faraday, she does the unthinkable, and risks being “deadish” so she can communicate with the Thunderhead—the only being on earth wise enough to solve the dire problems of a perfect world. But will it help solve those problems, or simply watch as perfection goes into decline?'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '686511'), ('text_reviews_count', '89671')]))])), ('published', '2018'), ('work', OrderedDict([('id', '54332060'), ('uri', 'kca://work/amzn1.gr.work.v1.csIUSRTP1nG0ilANHKdtvw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '28954189')])), ('isbn', '1442472421'), ('isbn13', '9781442472426'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '17271')])), ('uri', 'kca://book/amzn1.gr.book.v1.lW-2WpgCkQiPUhVi7Apjvw'), ('title', 'Scythe (Arc of a Scythe, #1)'), ('title_without_series', 'Scythe'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1456172676l/28954189._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1456172676l/28954189._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/28954189-scythe'), ('num_pages', '435'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Simon Schuster Books for Young Readers'), ('publication_day', '22'), ('publication_year', '2016'), ('publication_month', '11'), ('average_rating', '4.34'), ('ratings_count', '128264'), ('description', '&lt;i&gt;Thou shalt kill.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;A world with no hunger, no disease, no war, no misery. Humanity has conquered all those things, and has even conquered death. Now scythes are the only ones who can end life—and they are commanded to do so, in order to keep the size of the population under control.&lt;br /&gt;&lt;br /&gt;Citra and Rowan are chosen to apprentice to a scythe—a role that neither wants. These teens must master the “art” of taking life, knowing that the consequence of failure could mean losing their own.'), ('authors', OrderedDict([('author', OrderedDict([('id', '19564'), ('name', 'Neal Shusterman'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p5/19564.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1246977170p2/19564.jpg')])), ('link', 'https://www.goodreads.com/author/show/19564.Neal_Shusterman'), ('average_rating', '4.22'), ('ratings_count', '686511'), ('text_reviews_count', '89671')]))])), ('published', '2016'), ('work', OrderedDict([('id', '49179216'), ('uri', 'kca://work/amzn1.gr.work.v1.5n8t82DJpsluB4PsN0tTRA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '16143347')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '39616')])), ('uri', 'kca://book/amzn1.gr.book.v1.K-UvT466iI9PDxkBVNr4wQ'), ('title', 'We Were Liars'), ('title_without_series', 'We Were Liars'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1402749479l/16143347._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1402749479l/16143347._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/16143347-we-were-liars'), ('num_pages', '242'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Delacorte Press'), ('publication_day', '13'), ('publication_year', '2014'), ('publication_month', '5'), ('average_rating', '3.84'), ('ratings_count', '446554'), ('description', 'A beautiful and distinguished family.&lt;br /&gt;A private island.&lt;br /&gt;A brilliant, damaged girl; a passionate, political boy.&lt;br /&gt;A group of four friends—the Liars—whose friendship turns destructive.&lt;br /&gt;A revolution. An accident. A secret.&lt;br /&gt;Lies upon lies.&lt;br /&gt;True love.&lt;br /&gt;The truth.&lt;br /&gt; &lt;br /&gt;&lt;i&gt;We Were Liars&lt;/i&gt; is a modern, sophisticated suspense novel from &lt;i&gt;New York Times&lt;/i&gt; bestselling author, National Book Award finalist, and Printz Award honoree E. Lockhart. &lt;br /&gt;&lt;br /&gt;Read it.&lt;br /&gt;&lt;br /&gt;And if anyone asks you how it ends, just LIE.'), ('authors', OrderedDict([('author', OrderedDict([('id', '173491'), ('name', 'E. Lockhart'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1399077200p5/173491.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1399077200p2/173491.jpg')])), ('link', 'https://www.goodreads.com/author/show/173491.E_Lockhart'), ('average_rating', '3.78'), ('ratings_count', '585842'), ('text_reviews_count', '64631')]))])), ('published', '2014'), ('work', OrderedDict([('id', '21975829'), ('uri', 'kca://work/amzn1.gr.work.v1.SGGFlQ0RQuN1B3XE8ibruQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '29391367')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', '9780994310972'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '76')])), ('uri', 'kca://book/amzn1.gr.book.v1.Jj4YqqkesFUaPlrQUhF88A'), ('title', 'Chapter One: You have the power to change stuff'), ('title_without_series', 'Chapter One: You have the power to change stuff'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1457174638l/29391367._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1457174638l/29391367._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/29391367-chapter-one'), ('num_pages', '254'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'The Messenger Group'), ('publication_day', None), ('publication_year', '2016'), ('publication_month', '2'), ('average_rating', '4.19'), ('ratings_count', '590'), ('description', 'CHAPTER ONE is a story of epic proportions by Thankyou co-founder Daniel Flynn. It’s a bumpy and entertaining ride of gut-wrenching decisions, wild mistakes and daring moves into business, marketing, social enterprise and beyond. Follow the journey of three Australian kids from Melbourne with zero business experience and the shared belief that we all have the power to change stuff.&lt;br /&gt;&lt;br /&gt;Chapter One is more than a book. It’s an invitation, addressed to you. To inspire you to challenge what you know and remind you that crazy ideas can become a reality. It’s also an opportunity to be a part of something big. Something that could change the course of history.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3060790'), ('name', 'Daniel Flynn'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/3060790.Daniel_Flynn'), ('average_rating', '4.19'), ('ratings_count', '594'), ('text_reviews_count', '85')]))])), ('published', '2016'), ('work', OrderedDict([('id', '49645010'), ('uri', 'kca://work/amzn1.gr.work.v1.t_y7EkxOYbIkatJPWXAWXg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40097951')])), ('isbn', '1250301696'), ('isbn13', '9781250301697'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '36562')])), ('uri', 'kca://book/amzn1.gr.book.v1.Vjz3eASF7bmIo5WYoKMsnA'), ('title', 'The Silent Patient'), ('title_without_series', 'The Silent Patient'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582759969l/40097951._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582759969l/40097951._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40097951-the-silent-patient'), ('num_pages', '325'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Celadon Books'), ('publication_day', '5'), ('publication_year', '2019'), ('publication_month', '2'), ('average_rating', '4.09'), ('ratings_count', '440183'), ('description', 'Alicia Berenson’s life is seemingly perfect. A famous painter married to an in-demand fashion photographer, she lives in a grand house with big windows overlooking a park in one of London’s most desirable areas. One evening her husband Gabriel returns home late from a fashion shoot, and Alicia shoots him five times in the face, and then never speaks another word.&lt;br /&gt;&lt;br /&gt;Alicia’s refusal to talk, or give any kind of explanation, turns a domestic tragedy into something far grander, a mystery that captures the public imagination and casts Alicia into notoriety. The price of her art skyrockets, and she, the silent patient, is hidden away from the tabloids and spotlight at the Grove, a secure forensic unit in North London.&lt;br /&gt;&lt;br /&gt;Theo Faber is a criminal psychotherapist who has waited a long time for the opportunity to work with Alicia. His determination to get her to talk and unravel the mystery of why she shot her husband takes him down a twisting path into his own motivations—a search for the truth that threatens to consume him...'), ('authors', OrderedDict([('author', OrderedDict([('id', '17621440'), ('name', 'Alex Michaelides'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1526317750p5/17621440.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1526317750p2/17621440.jpg')])), ('link', 'https://www.goodreads.com/author/show/17621440.Alex_Michaelides'), ('average_rating', '4.09'), ('ratings_count', '441129'), ('text_reviews_count', '45530')]))])), ('published', '2019'), ('work', OrderedDict([('id', '59752778'), ('uri', 'kca://work/amzn1.gr.work.v1.MUfHMLGEE_tCE7JMBSsL1A')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '22628')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '45808')])), ('uri', 'kca://book/amzn1.gr.book.v1.3TyU0wMKQZ7LYyvGh01Eqg'), ('title', 'The Perks of Being a Wallflower'), ('title_without_series', 'The Perks of Being a Wallflower'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1520093244l/22628._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1520093244l/22628._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/22628.The_Perks_of_Being_a_Wallflower'), ('num_pages', '213'), ('format', 'Paperback'), ('edition_information', '1st MTV/Pocket Books trade paperback edition (US/CAN)'), ('publisher', 'MTV Books/Pocket Books'), ('publication_day', None), ('publication_year', '1999'), ('publication_month', '2'), ('average_rating', '4.20'), ('ratings_count', '1228714'), ('description', "standing on the fringes of life...&lt;br /&gt;offers a unique perspective. But there comes a time to see&lt;br /&gt;what it looks like from the dance floor.&lt;br /&gt;&lt;br /&gt;This haunting novel about the dilemma of passivity vs. passion marks the stunning debut of a provocative new voice in contemporary fiction: The Perks of Being A WALLFLOWER&lt;br /&gt;&lt;br /&gt;This is the story of what it's like to grow up in high school. More intimate than a diary, Charlie's letters are singular and unique, hilarious and devastating. We may not know where he lives. We may not know to whom he is writing. All we know is the world he shares. Caught between trying to live his life and trying to run from it puts him on a strange course through uncharted territory. The world of first dates and mixed tapes, family dramas and new friends. The world of sex, drugs, and The Rocky Horror Picture Show, when all one requires is that the perfect song on that perfect drive to feel infinite.&lt;br /&gt;&lt;br /&gt;Through Charlie, Stephen Chbosky has created a deeply affecting coming-of-age story, a powerful novel that will spirit you back to those wild and poignant roller coaster days known as growing up.&lt;br /&gt;&lt;br /&gt;(back cover)"), ('authors', OrderedDict([('author', OrderedDict([('id', '12898'), ('name', 'Stephen Chbosky'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_200x266-d279b33f8eec0f27b7272477f09806be.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/m_50x66-82093808bca726cb3249a493fbd3bd0f.png')])), ('link', 'https://www.goodreads.com/author/show/12898.Stephen_Chbosky'), ('average_rating', '4.19'), ('ratings_count', '1249985'), ('text_reviews_count', '61753')]))])), ('published', '1999'), ('work', OrderedDict([('id', '2236198'), ('uri', 'kca://work/amzn1.gr.work.v1.ssZvkcqaAEbn5_xfTc0TGw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '11870085')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '139431')])), ('uri', 'kca://book/amzn1.gr.book.v1.6rIwidkUTORGkQo3jY4dcg'), ('title', 'The Fault in Our Stars'), ('title_without_series', 'The Fault in Our Stars'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1360206420l/11870085._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1360206420l/11870085._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/11870085-the-fault-in-our-stars'), ('num_pages', '313'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Dutton Books'), ('publication_day', '10'), ('publication_year', '2012'), ('publication_month', '1'), ('average_rating', '4.21'), ('ratings_count', '3472706'), ('description', "Despite the tumor-shrinking medical miracle that has bought her a few years, Hazel has never been anything but terminal, her final chapter inscribed upon diagnosis. But when a gorgeous plot twist named Augustus Waters suddenly appears at Cancer Kid Support Group, Hazel's story is about to be completely rewritten.&lt;br /&gt;&lt;br /&gt;Insightful, bold, irreverent, and raw, The Fault in Our Stars is award-winning author John Green's most ambitious and heartbreaking work yet, brilliantly exploring the funny, thrilling, and tragic business of being alive and in love."), ('authors', OrderedDict([('author', OrderedDict([('id', '1406384'), ('name', 'John Green'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353452301p5/1406384.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353452301p2/1406384.jpg')])), ('link', 'https://www.goodreads.com/author/show/1406384.John_Green'), ('average_rating', '4.04'), ('ratings_count', '6686732'), ('text_reviews_count', '349289')]))])), ('published', '2012'), ('work', OrderedDict([('id', '16827462'), ('uri', 'kca://work/amzn1.gr.work.v1.ZWeA15QphzWjRB87CLg-TA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6900')])), ('isbn', '0751529818'), ('isbn13', '9780751529814'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '21688')])), ('uri', 'kca://book/amzn1.gr.book.v1.HYlfDM7QTPV1OEJGJmRHtw'), ('title', 'Tuesdays with Morrie'), ('title_without_series', 'Tuesdays with Morrie'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423763749l/6900._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1423763749l/6900._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6900.Tuesdays_with_Morrie'), ('num_pages', '210'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Warner'), ('publication_day', None), ('publication_year', '2000'), ('publication_month', None), ('average_rating', '4.11'), ('ratings_count', '766449'), ('description', "Maybe it was a grandparent, or a teacher or a colleague. Someone older, patient and wise, who understood you when you were young and searching, and gave you sound advice to help you make your way through it. For Mitch Albom, that person was Morrie Schwartz, his college professor from nearly twenty years ago.&lt;br /&gt;&lt;br /&gt;Maybe, like Mitch, you lost track of this mentor as you made your way, and the insights faded. Wouldn't you like to see that person again, ask the bigger questions that still haunt you? &lt;br /&gt;&lt;br /&gt;Mitch Albom had that second chance. He rediscovered Morrie in the last months of the older man's life. Knowing he was dying of ALS - or motor neurone disease - Mitch visited Morrie in his study every Tuesday, just as they used to back in college. Their rekindled relationship turned into one final 'class': lessons in how to live."), ('authors', OrderedDict([('author', OrderedDict([('id', '2331'), ('name', 'Mitch Albom'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1368640552p5/2331.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1368640552p2/2331.jpg')])), ('link', 'https://www.goodreads.com/author/show/2331.Mitch_Albom'), ('average_rating', '4.04'), ('ratings_count', '1765971'), ('text_reviews_count', '84350')]))])), ('published', '2000'), ('work', OrderedDict([('id', '1995335'), ('uri', 'kca://work/amzn1.gr.work.v1.zIj_sWs9NizBbBF7FwK_mQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '19063')])), ('isbn', '0375831002'), ('isbn13', '9780375831003'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '89469')])), ('uri', 'kca://book/amzn1.gr.book.v1.A1zfLKejdNPkLkjfE8LN8Q'), ('title', 'The Book Thief'), ('title_without_series', 'The Book Thief'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1522157426l/19063._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1522157426l/19063._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/19063.The_Book_Thief'), ('num_pages', '552'), ('format', 'Hardcover'), ('edition_information', 'First American Edition'), ('publisher', 'Alfred A. Knopf'), ('publication_day', '14'), ('publication_year', '2006'), ('publication_month', '3'), ('average_rating', '4.37'), ('ratings_count', '1795753'), ('description', '&lt;i&gt;Librarian\'s note: An alternate cover edition can be found &lt;a href="https://www.goodreads.com/book/show/41048862.here" title="here" rel="nofollow"&gt;here&lt;/a&gt;&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;It is 1939. Nazi Germany. The country is holding its breath. Death has never been busier, and will be busier still.&lt;br /&gt;&lt;br /&gt;By her brother\'s graveside, Liesel\'s life is changed when she picks up a single object, partially hidden in the snow. It is The Gravedigger\'s Handbook, left behind there by accident, and it is her first act of book thievery. So begins a love affair with books and words, as Liesel, with the help of her accordian-playing foster father, learns to read. Soon she is stealing books from Nazi book-burnings, the mayor\'s wife\'s library, wherever there are books to be found.&lt;br /&gt;&lt;br /&gt;But these are dangerous times. When Liesel\'s foster family hides a Jew in their basement, Liesel\'s world is both opened up, and closed down.&lt;br /&gt;&lt;br /&gt;In superbly crafted writing that burns with intensity, award-winning author Markus Zusak has given us one of the most enduring stories of our time.&lt;br /&gt;&lt;br /&gt;(Note: this title was not published as YA fiction)'), ('authors', OrderedDict([('author', OrderedDict([('id', '11466'), ('name', 'Markus Zusak'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1537240528p5/11466.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1537240528p2/11466.jpg')])), ('link', 'https://www.goodreads.com/author/show/11466.Markus_Zusak'), ('average_rating', '4.34'), ('ratings_count', '1973286'), ('text_reviews_count', '132655')]))])), ('published', '2006'), ('work', OrderedDict([('id', '878368'), ('uri', 'kca://work/amzn1.gr.work.v1.BGVqmVn5CPHsjnZIfHpUUw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '6334')])), ('isbn', '1400078776'), ('isbn13', '9781400078776'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '24096')])), ('uri', 'kca://book/amzn1.gr.book.v1.t3ESMobC-9O2YByR0RqA6g'), ('title', 'Never Let Me Go'), ('title_without_series', 'Never Let Me Go'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353048590l/6334._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1353048590l/6334._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/6334.Never_Let_Me_Go'), ('num_pages', '288'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Vintage Books'), ('publication_day', '31'), ('publication_year', '2010'), ('publication_month', '8'), ('average_rating', '3.82'), ('ratings_count', '460421'), ('description', 'From the Booker Prize-winning author of &lt;i&gt;The Remains of the Day&lt;/i&gt; and &lt;i&gt;When We Were Orphans&lt;/i&gt;, comes an unforgettable edge-of-your-seat mystery that is at once heartbreakingly tender and morally courageous about what it means to be human.&lt;br /&gt;&lt;br /&gt;Hailsham seems like a pleasant English boarding school, far from the influences of the city. Its students are well tended and supported, trained in art and literature, and become just the sort of people the world wants them to be. But, curiously, they are taught nothing of the outside world and are allowed little contact with it.&lt;br /&gt;&lt;br /&gt;Within the grounds of Hailsham, Kathy grows from schoolgirl to young woman, but it’s only when she and her friends Ruth and Tommy leave the safe grounds of the school (as they always knew they would) that they realize the full truth of what Hailsham is.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Never Let Me Go&lt;/i&gt; breaks through the boundaries of the literary novel. It is a gripping mystery, a beautiful love story, and also a scathing critique of human arrogance and a moral examination of how we treat the vulnerable and different in our society. In exploring the themes of memory and the impact of the past, Ishiguro takes on the idea of a possible future to create his most moving and powerful book to date.'), ('authors', OrderedDict([('author', OrderedDict([('id', '4280'), ('name', 'Kazuo Ishiguro'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1424906625p5/4280.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1424906625p2/4280.jpg')])), ('link', 'https://www.goodreads.com/author/show/4280.Kazuo_Ishiguro'), ('average_rating', '3.84'), ('ratings_count', '825706'), ('text_reviews_count', '64155')]))])), ('published', '2010'), ('work', OrderedDict([('id', '1499998'), ('uri', 'kca://work/amzn1.gr.work.v1.Z4gC--jsCarRwWlyoQp-VQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '39335566')])), ('isbn', '0385543875'), ('isbn13', '9780385543873'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '1557')])), ('uri', 'kca://book/amzn1.gr.book.v1.XSmg5W7_uZm9h4X_93gS5g'), ('title', 'The Water Cure'), ('title_without_series', 'The Water Cure'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1521604165l/39335566._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1521604165l/39335566._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/39335566-the-water-cure'), ('num_pages', '288'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Doubleday'), ('publication_day', '8'), ('publication_year', '2019'), ('publication_month', '1'), ('average_rating', '3.26'), ('ratings_count', '17044'), ('description', '&lt;b&gt;&lt;i&gt;The Handmaid’s Tale&lt;/i&gt; meets &lt;i&gt;The Virgin Suicides&lt;/i&gt; in this dystopic feminist revenge fantasy about three sisters on an isolated island, raised to fear men&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;King has tenderly staked out a territory for his wife and three daughters, Grace, Lia, and Sky. He has laid the barbed wire; he has anchored the buoys in the water; he has marked out a clear message: Do not enter. Or viewed from another angle: Not safe to leave. Here women are protected from the chaos and violence of men on the mainland. The cult-like rituals and therapies they endure fortify them from the spreading toxicity of a degrading world.&lt;br /&gt;&lt;br /&gt;But when their father, the only man they’ve ever seen, disappears, they retreat further inward until the day three strange men wash ashore. Over the span of one blistering hot week, a psychological cat-and-mouse game plays out. Sexual tensions and sibling rivalries flare as the sisters confront the amorphous threat the strangers represent. Can they survive the men?&lt;br /&gt;&lt;br /&gt;A haunting, riveting debut about the capacity for violence and the potency of female desire, &lt;i&gt;The Water Cure&lt;/i&gt; both devastates and astonishes as it reflects our own world back at us.'), ('authors', OrderedDict([('author', OrderedDict([('id', '6152025'), ('name', 'Sophie Mackintosh'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1536937022p5/6152025.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1536937022p2/6152025.jpg')])), ('link', 'https://www.goodreads.com/author/show/6152025.Sophie_Mackintosh'), ('average_rating', '3.31'), ('ratings_count', '18865'), ('text_reviews_count', '2718')]))])), ('published', '2019'), ('work', OrderedDict([('id', '56832986'), ('uri', 'kca://work/amzn1.gr.work.v1.Oftp5vHVmbQeEnskpnPsMg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '9305362')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '4231')])), ('uri', 'kca://book/amzn1.gr.book.v1.XRBgHq982k9dupkNGLEqLg'), ('title', 'Captive Prince (Captive Prince, #1)'), ('title_without_series', 'Captive Prince'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356028113l/9305362._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1356028113l/9305362._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/9305362-captive-prince'), ('num_pages', '240'), ('format', 'ebook'), ('edition_information', None), ('publisher', None), ('publication_day', '22'), ('publication_year', '2012'), ('publication_month', '5'), ('average_rating', '3.87'), ('ratings_count', '52731'), ('description', '&lt;b&gt;From global phenomenon C. S. Pacat comes the first in her critically acclaimed trilogy—with a bonus story.&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;Damen is a warrior hero to his people, and the rightful heir to the throne of Akielos. But when his half brother seizes power, Damen is captured, stripped of his identity, and sent to serve the prince of an enemy nation as a pleasure slave.&lt;br /&gt;&lt;br /&gt;Beautiful, manipulative, and deadly, his new master, Prince Laurent, epitomizes the worst of the court at Vere. But in the lethal political web of the Veretian court, nothing is as it seems, and when Damen finds himself caught up in a play for the throne, he must work together with Laurent to survive and save his country.&lt;br /&gt;&lt;br /&gt;For Damen, there is just one rule: never, ever reveal his true identity. Because the one man Damen needs is the one man who has more reason to hate him than anyone else…&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Includes an exclusive extra story!&lt;/b&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '4349837'), ('name', 'C.S. Pacat'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p5/4349837.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1425185129p2/4349837.jpg')])), ('link', 'https://www.goodreads.com/author/show/4349837.C_S_Pacat'), ('average_rating', '4.19'), ('ratings_count', '195235'), ('text_reviews_count', '25949')]))])), ('published', '2012'), ('work', OrderedDict([('id', '14188292'), ('uri', 'kca://work/amzn1.gr.work.v1.0CuNLmY6oZw9oaliTYsfGg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '29283884')])), ('isbn', '0062382802'), ('isbn13', '9780062382801'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '13079')])), ('uri', 'kca://book/amzn1.gr.book.v1.Lo3JQRH4kkQxjMVU6JD9Yg'), ('title', "The Gentleman's Guide to Vice and Virtue (Montague Siblings, #1)"), ('title_without_series', "The Gentleman's Guide to Vice and Virtue"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1492601464l/29283884._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1492601464l/29283884._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/29283884-the-gentleman-s-guide-to-vice-and-virtue'), ('num_pages', '513'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Katherine Tegen Books'), ('publication_day', '27'), ('publication_year', '2017'), ('publication_month', '6'), ('average_rating', '4.11'), ('ratings_count', '85504'), ('description', 'Henry “Monty” Montague was born and bred to be a gentleman, but he was never one to be tamed. The finest boarding schools in England and the constant disapproval of his father haven’t been able to curb any of his roguish passions—not for gambling halls, late nights spent with a bottle of spirits, or waking up in the arms of women or men.&lt;br /&gt;&lt;br /&gt;But as Monty embarks on his Grand Tour of Europe, his quest for a life filled with pleasure and vice is in danger of coming to an end. Not only does his father expect him to take over the family’s estate upon his return, but Monty is also nursing an impossible crush on his best friend and traveling companion, Percy.&lt;br /&gt;&lt;br /&gt;Still it isn’t in Monty’s nature to give up. Even with his younger sister, Felicity, in tow, he vows to make this yearlong escapade one last hedonistic hurrah and flirt with Percy from Paris to Rome. But when one of Monty’s reckless decisions turns their trip abroad into a harrowing manhunt that spans across Europe, it calls into question everything he knows, including his relationship with the boy he adores.'), ('authors', OrderedDict([('author', OrderedDict([('id', '7327341'), ('name', 'Mackenzi Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1512266703p5/7327341.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1512266703p2/7327341.jpg')])), ('link', 'https://www.goodreads.com/author/show/7327341.Mackenzi_Lee'), ('average_rating', '4.10'), ('ratings_count', '132171'), ('text_reviews_count', '25555')]))])), ('published', '2017'), ('work', OrderedDict([('id', '49527118'), ('uri', 'kca://work/amzn1.gr.work.v1.KF8U_R5FRuUIlCVQG4A7pQ')]))])</t>
   </si>
   <si>
     <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '18474149')])), ('isbn', '0500342954'), ('isbn13', '9780500342954'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '2')])), ('uri', 'kca://book/amzn1.gr.book.v1.E1cQ9Bb7M-YjfTINoV66BQ'), ('title', 'The Elements of Modern Architecture: Understanding Contemporary Buildings'), ('title_without_series', 'The Elements of Modern Architecture: Understanding Contemporary Buildings'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1381290149l/18474149._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1381290149l/18474149._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/18474149-the-elements-of-modern-architecture'), ('num_pages', '344'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Thames  Hudson'), ('publication_day', '17'), ('publication_year', '2014'), ('publication_month', '6'), ('average_rating', '4.43'), ('ratings_count', '21'), ('description', 'After a period in which computation-derived architecture—driven by digital design tools, data analysis, and new formal expression—has thrived, students and their teachers have returned to age-old techniques before employing the digital tools that are a part of every architect’s studio. Tired of the perfectly rendered screen image, architects are making presentations that are clearly the work of the hand and the mind, not the computer.&lt;br /&gt;&lt;br /&gt;This ambitious publication, organized chronologically, is aimed at a new generation of architects who take technology for granted, but seek to further understand the principles of what makes a building meaningful and enduring. Each of the fifty works of architecture is presented through detailed consideration of its site, topology, and surroundings; natural light, volumes, and massing; program and circulation; details, fenestration, and ornamentation. Over 2,500 painstakingly hand-drawn images of the buildings of the past seven decades help readers return to the core values of understanding site and creating buildings: looking with the eyes, engaging through direct physical experience, and constructing by hand.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1109791'), ('name', 'Antony Radford'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/1109791.Antony_Radford'), ('average_rating', '4.40'), ('ratings_count', '25'), ('text_reviews_count', '2')]))])), ('published', '2014'), ('work', OrderedDict([('id', '26141386'), ('uri', 'kca://work/amzn1.gr.work.v1.lDKLYqyzLX6tytu5pbDnTg')]))])</t>
   </si>
   <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '28634049')])), ('isbn', '1616892552'), ('isbn13', '9781616892555'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3')])), ('uri', 'kca://book/amzn1.gr.book.v1.X2LWiajTXoUtWYV1S5zXrw'), ('title', 'Manual of Section'), ('title_without_series', 'Manual of Section'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1465687065l/28634049._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1465687065l/28634049._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/28634049-manual-of-section'), ('num_pages', '208'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Princeton Architectural Press'), ('publication_day', '23'), ('publication_year', '2016'), ('publication_month', '8'), ('average_rating', '4.43'), ('ratings_count', '56'), ('description', '&lt;b&gt;"It has been a while since I devoured a book on architecture with as much pleasure. I love a good section and I love this book."—Aaron Betsky, &lt;i&gt;Architect Magazine&lt;/i&gt;&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Award-winning architects Paul Lewis, Marc Tsurumaki, and David J. Lewis\'s essential guide to section.&lt;/b&gt; Section, along with plan and elevation, is one of the most important representational techniques of architectural design. &lt;i&gt;Manual of Section&lt;/i&gt; is the first book to provide a framework to describe and evaluate this fundamental design process in architecture.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Divided into seven categories of section based on extensive archival research:&lt;/b&gt;&lt;br /&gt;• Range is from simple one-story buildings to complex structures&lt;br /&gt;• Features stacked forms, fantastical shapes, internal holes, inclines, sheared planes, nested forms, or combinations of each&lt;br /&gt;• Includes sixty-three intricately detailed cross-section perspective drawings of many of the most significant structures in international architecture from the last one hundred years&lt;br /&gt;&lt;br /&gt;&lt;b&gt;"A must-read for all designers associated with the built environment and should surely be on the library shelves of every architecture, urban design and interior design school...the intricate drawings provided by LTL are sure to inspire all those who have the privilege of cracking the spine of this amazing reference." —&lt;i&gt;Spacing&lt;/i&gt;&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;In addition to the incredible cross-section drawings, the book includes smart and accessible essays on the history and uses of section.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Manual of Section&lt;/i&gt; has become a top architecture book for architecture students and professional architects.'), ('authors', OrderedDict([('author', OrderedDict([('id', '61932'), ('name', 'Paul Lewis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/61932.Paul_Lewis'), ('average_rating', '4.02'), ('ratings_count', '813'), ('text_reviews_count', '77')]))])), ('published', '2016'), ('work', OrderedDict([('id', '48812456'), ('uri', 'kca://work/amzn1.gr.work.v1.2rO6tUoI3SdGAGHVn67IMA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '80660')])), ('isbn', '006112429X'), ('isbn13', '9780061124297'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '11114')])), ('uri', 'kca://book/amzn1.gr.book.v1.XVzibBbNBoaCNgEiJRWt9g'), ('title', 'We Need to Talk About Kevin'), ('title_without_series', 'We Need to Talk About Kevin'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327865017l/80660._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327865017l/80660._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/80660.We_Need_to_Talk_About_Kevin'), ('num_pages', '400'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harper Perennial'), ('publication_day', '3'), ('publication_year', '2006'), ('publication_month', '7'), ('average_rating', '4.05'), ('ratings_count', '156525'), ('description', "&lt;p&gt; The gripping international bestseller about motherhood gone awry.&lt;/p&gt;&lt;p&gt;Eva never really wanted to be a mother - and certainly not the mother of the unlovable boy who murdered seven of his fellow high school students, a cafeteria worker, and a much-adored teacher who tried to befriend him, all two days before his sixteenth birthday. Now, two years later, it is time for her to come to terms with marriage, career, family, parenthood, and Kevin's horrific rampage in a series of startlingly direct correspondences with her estranged husband, Franklin. Uneasy with the sacrifices and social demotion of motherhood from the start, Eva fears that her alarming dislike for her own son may be responsible for driving him so nihilistically off the rails. &lt;/p&gt;&lt;p&gt;&lt;/p&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '45922'), ('name', 'Lionel Shriver'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1332800238p5/45922.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1332800238p2/45922.jpg')])), ('link', 'https://www.goodreads.com/author/show/45922.Lionel_Shriver'), ('average_rating', '3.91'), ('ratings_count', '218569'), ('text_reviews_count', '23118')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3106720'), ('uri', 'kca://work/amzn1.gr.work.v1.xLpjOSFP7LDX8cIvigjctg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '32617610')])), ('isbn', '1473212782'), ('isbn13', '9781473212787'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '742')])), ('uri', 'kca://book/amzn1.gr.book.v1.EoFIbWdTfov5TrDj9-sIsg'), ('title', 'Sea of Rust'), ('title_without_series', 'Sea of Rust'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/32617610-sea-of-rust'), ('num_pages', '365'), ('format', None), ('edition_information', None), ('publisher', None), ('publication_day', None), ('publication_year', None), ('publication_month', None), ('average_rating', '4.08'), ('ratings_count', '7326'), ('description', "One robot's search for meaning in a world where every human is long gone. &lt;br /&gt;&lt;br /&gt;A touching story of a search one robot's search for the answers in a world where every human is dead. &lt;br /&gt;&lt;br /&gt;It is thirty years since the humans lost their war with the artificial intelligences that were once their slaves. Not one human remains. But as the dust settled from our extinction there was no easy peace between the robots that survived. Instead, the two massively powerful artificially intelligent supercomputers that led them to victory now vie for control of the bots that remain, assimilating them into enormous networks called One World Intelligences (OWIs), absorbing their memories and turning them into mere extensions of the whole. Now the remaining freebots wander wastelands that were once warzones, picking the carcasses of the lost for the precious dwindling supply of parts they need to survive. &lt;br /&gt;&lt;br /&gt;BRITTLE started out his life playing nurse to a dying man, purchased in truth instead to look after the man's widow upon his death. But then war came and Brittle was forced to choose between the woman he swore to protect and potential oblivion at the hands of rising anti-AI sentiment. Thirty years later, his choice still haunts him. Now he spends his days in the harshest of the wastelands, known as the Sea of Rust, cannibalizing the walking dead - robots only hours away from total shutdown - looking for parts to trade for those he needs to keep going."), ('authors', OrderedDict([('author', OrderedDict([('id', '3969859'), ('name', 'C. Robert Cargill'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353882150p5/3969859.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353882150p2/3969859.jpg')])), ('link', 'https://www.goodreads.com/author/show/3969859.C_Robert_Cargill'), ('average_rating', '3.90'), ('ratings_count', '14675'), ('text_reviews_count', '2182')]))])), ('published', None), ('work', OrderedDict([('id', '53204799'), ('uri', 'kca://work/amzn1.gr.work.v1.Zx5ELRvYlVOpE4rBne88Yg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38649806')])), ('isbn', '0525534326'), ('isbn13', '9780525534327'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '732')])), ('uri', 'kca://book/amzn1.gr.book.v1.H7ebuEcy5XpuAlKh9eipBA'), ('title', 'Little'), ('title_without_series', 'Little'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1523724459l/38649806._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1523724459l/38649806._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38649806-little'), ('num_pages', '448'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Riverhead Books'), ('publication_day', '23'), ('publication_year', '2018'), ('publication_month', '10'), ('average_rating', '4.00'), ('ratings_count', '5726'), ('description', "The wry, macabre, unforgettable tale of an ambitious orphan in Revolutionary Paris, befriended by royalty and radicals, who transforms herself into the legendary Madame Tussaud.&lt;br /&gt;&lt;br /&gt;In 1761, a tiny, odd-looking girl named Marie is born in a village in Switzerland. After the death of her parents, she is apprenticed to an eccentric wax sculptor and whisked off to the seamy streets of Paris, where they meet a domineering widow and her quiet, pale son. Together, they convert an abandoned monkey house into an exhibition hall for wax heads, and the spectacle becomes a sensation. As word of her artistic talent spreads, Marie is called to Versailles, where she tutors a princess and saves Marie Antoinette in childbirth. But outside the palace walls, Paris is roiling: The revolutionary mob is demanding heads, and... at the wax museum, heads are what they do.&lt;br /&gt;&lt;br /&gt;In the tradition of Gregory Maguire's Wicked and Erin Morgenstern's &lt;i&gt;The Night Circus&lt;/i&gt;, Edward Carey's &lt;i&gt;Little&lt;/i&gt; is a darkly endearing cavalcade of a novel—a story of art, class, determination, and how we hold on to what we love."), ('authors', OrderedDict([('author', OrderedDict([('id', '161399'), ('name', 'Edward Carey'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1388256263p5/161399.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1388256263p2/161399.jpg')])), ('link', 'https://www.goodreads.com/author/show/161399.Edward_Carey'), ('average_rating', '3.89'), ('ratings_count', '11492'), ('text_reviews_count', '1838')]))])), ('published', '2018'), ('work', OrderedDict([('id', '60261099'), ('uri', 'kca://work/amzn1.gr.work.v1.k2B71vWE7GVBP6FRngMwhw')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '9361589')])), ('isbn', '0385534639'), ('isbn13', '9780385534635'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '57644')])), ('uri', 'kca://book/amzn1.gr.book.v1.tPpWGC7kuUxtvkvPBpeniA'), ('title', 'The Night Circus'), ('title_without_series', 'The Night Circus'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1387124618l/9361589._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1387124618l/9361589._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/9361589-the-night-circus'), ('num_pages', '391'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Doubleday'), ('publication_day', '13'), ('publication_year', '2011'), ('publication_month', '9'), ('average_rating', '4.04'), ('ratings_count', '659419'), ('description', 'The circus arrives without warning. No announcements precede it. It is simply there, when yesterday it was not. Within the black-and-white striped canvas tents is an utterly unique experience full of breathtaking amazements. It is called Le Cirque des Rêves, and it is only open at night. &lt;br /&gt;&lt;br /&gt;But behind the scenes, a fierce competition is underway—a duel between two young magicians, Celia and Marco, who have been trained since childhood expressly for this purpose by their mercurial instructors. Unbeknownst to them, this is a game in which only one can be left standing, and the circus is but the stage for a remarkable battle of imagination and will. Despite themselves, however, Celia and Marco tumble headfirst into love—a deep, magical love that makes the lights flicker and the room grow warm whenever they so much as brush hands. &lt;br /&gt;&lt;br /&gt;True love or not, the game must play out, and the fates of everyone involved, from the cast of extraordinary circus performers to the patrons, hang in the balance, suspended as precariously as the daring acrobats overhead. &lt;br /&gt;&lt;br /&gt;Written in rich, seductive prose, this spell-casting novel is a feast for the senses and the heart.'), ('authors', OrderedDict([('author', OrderedDict([('id', '4370565'), ('name', 'Erin Morgenstern'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1552589582p5/4370565.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1552589582p2/4370565.jpg')])), ('link', 'https://www.goodreads.com/author/show/4370565.Erin_Morgenstern'), ('average_rating', '4.02'), ('ratings_count', '731901'), ('text_reviews_count', '87061')]))])), ('published', '2011'), ('work', OrderedDict([('id', '14245059'), ('uri', 'kca://work/amzn1.gr.work.v1.IzoeETdoCBWf_cxRZU_R_Q')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '34051011')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9327')])), ('uri', 'kca://book/amzn1.gr.book.v1.ko9fgGm97_zjs4OlOuIZSw'), ('title', 'Pachinko'), ('title_without_series', 'Pachinko'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1529845599l/34051011._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1529845599l/34051011._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/34051011-pachinko'), ('num_pages', '496'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Grand Central Publishing'), ('publication_day', '7'), ('publication_year', '2017'), ('publication_month', '2'), ('average_rating', '4.27'), ('ratings_count', '188978'), ('description', "In the early 1900s, teenaged Sunja, the adored daughter of a crippled fisherman, falls for a wealthy stranger at the seashore near her home in Korea. He promises her the world, but when she discovers she is pregnant--and that her lover is married--she refuses to be bought. Instead, she accepts an offer of marriage from a gentle, sickly minister passing through on his way to Japan. But her decision to abandon her home, and to reject her son's powerful father, sets off a dramatic saga that will echo down through the generations.&lt;br /&gt;&lt;br /&gt;Richly told and profoundly moving, Pachinko is a story of love, sacrifice, ambition, and loyalty. From bustling street markets to the halls of Japan's finest universities to the pachinko parlors of the criminal underworld, Lee's complex and passionate characters--strong, stubborn women, devoted sisters and sons, fathers shaken by moral crisis--survive and thrive against the indifferent arc of history."), ('authors', OrderedDict([('author', OrderedDict([('id', '378209'), ('name', 'Min Jin Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192651627p5/378209.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192651627p2/378209.jpg')])), ('link', 'https://www.goodreads.com/author/show/378209.Min_Jin_Lee'), ('average_rating', '4.23'), ('ratings_count', '203009'), ('text_reviews_count', '21086')]))])), ('published', '2017'), ('work', OrderedDict([('id', '50384116'), ('uri', 'kca://work/amzn1.gr.work.v1.Kfq1uC_3eoSK1b271iNVKQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '18143977')])), ('isbn', '1476746583'), ('isbn13', '9781476746586'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '65041')])), ('uri', 'kca://book/amzn1.gr.book.v1.0IooOCfVIQPcIMOpfSRpYA'), ('title', 'All the Light We Cannot See'), ('title_without_series', 'All the Light We Cannot See'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1451445646l/18143977._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1451445646l/18143977._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/18143977-all-the-light-we-cannot-see'), ('num_pages', '531'), ('format', 'Hardcover'), ('edition_information', 'First Scribner hardcover edition May 2014'), ('publisher', 'Scribner'), ('publication_day', '6'), ('publication_year', '2014'), ('publication_month', '5'), ('average_rating', '4.33'), ('ratings_count', '982944'), ('description', '&lt;i&gt;An alternate cover for this ISBN can be found &lt;a href="https://www.goodreads.com/book/show/25210408-all-the-light-we-cannot-see" rel="nofollow"&gt;here&lt;/a&gt;&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;From the highly acclaimed, multiple award-winning Anthony Doerr, the stunningly beautiful instant &lt;i&gt;New York Times&lt;/i&gt; bestseller about a blind French girl and a German boy whose paths collide in occupied France as both try to survive the devastation of World War II.&lt;br /&gt;&lt;br /&gt;Marie-Laure lives in Paris near the Museum of Natural History, where her father works. When she is twelve, the Nazis occupy Paris and father and daughter flee to the walled citadel of Saint-Malo, where Marie-Laure’s reclusive great uncle lives in a tall house by the sea. With them they carry what might be the museum’s most valuable and dangerous jewel.&lt;br /&gt;&lt;br /&gt;In a mining town in Germany, Werner Pfennig, an orphan, grows up with his younger sister, enchanted by a crude radio they find that brings them news and stories from places they have never seen or imagined. Werner becomes an expert at building and fixing these crucial new instruments and is enlisted to use his talent to track down the resistance. Deftly interweaving the lives of Marie-Laure and Werner, Doerr illuminates the ways, against all odds, people try to be good to one another.'), ('authors', OrderedDict([('author', OrderedDict([('id', '28186'), ('name', 'Anthony Doerr'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1417812584p5/28186.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1417812584p2/28186.jpg')])), ('link', 'https://www.goodreads.com/author/show/28186.Anthony_Doerr'), ('average_rating', '4.31'), ('ratings_count', '1023129'), ('text_reviews_count', '79477')]))])), ('published', '2014'), ('work', OrderedDict([('id', '25491300'), ('uri', 'kca://work/amzn1.gr.work.v1.RE5swba2G5t7ZuQ6dNCGEQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '45880884')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', '9780648571599'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '165')])), ('uri', 'kca://book/amzn1.gr.book.v1.spE8a2-R6_O3udPVNsG56w'), ('title', 'Weapon (Whisper, #2)'), ('title_without_series', 'Weapon'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558412659l/45880884._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558412659l/45880884._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/45880884-weapon'), ('num_pages', '407'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Pantera Press'), ('publication_day', '4'), ('publication_year', '2019'), ('publication_month', '11'), ('average_rating', '4.36'), ('ratings_count', '1202'), ('description', "The #1 bestselling WHISPER series concludes with WEAPON:&lt;br /&gt;&lt;br /&gt;&lt;i&gt;I already knew he was a psychopath. But now?&lt;br /&gt;He's more dangerous than ever.&lt;br /&gt;And I have less than twenty-four hours to stop him.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;After escaping Lengard and finding sanctuary with the Remnants, Alyssa Scott is desperate to save those she left behind ─ and the rest of the world ─ from the power-hungry scientist, Kendall Vanik. But secrets and lies block her at every turn, and soon Lyss is left questioning everything she has ever believed.&lt;br /&gt;&lt;br /&gt;When long-lost memories begin to surface and the mysteries of her past continue to grow, Lyss battles to retain her hard-won control. Allies become enemies and enemies become allies, leaving her certain about only two things: when it comes to Speakers, nothing is ever as it seems... and the only person she can trust is herself."), ('authors', OrderedDict([('author', OrderedDict([('id', '9857504'), ('name', 'Lynette Noni'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p5/9857504.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p2/9857504.jpg')])), ('link', 'https://www.goodreads.com/author/show/9857504.Lynette_Noni'), ('average_rating', '4.42'), ('ratings_count', '20384'), ('text_reviews_count', '3077')]))])), ('published', '2019'), ('work', OrderedDict([('id', '70706086'), ('uri', 'kca://work/amzn1.gr.work.v1.HcfdpNe0pZXUjdb2-YRgyQ')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '34020950')])), ('isbn', '1525300415'), ('isbn13', '9781525300417'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '506')])), ('uri', 'kca://book/amzn1.gr.book.v1.PNYh92pz7gDLM6qrgJMH6A'), ('title', 'Whisper (Whisper, #1)'), ('title_without_series', 'Whisper'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1504853373l/34020950._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1504853373l/34020950._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/34020950-whisper'), ('num_pages', '320'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'KCP Loft'), ('publication_day', '1'), ('publication_year', '2018'), ('publication_month', '5'), ('average_rating', '4.27'), ('ratings_count', '3881'), ('description', '&lt;i&gt;“Lengard is a secret government facility for extraordinary people,” they told me. &lt;br /&gt;&lt;br /&gt;I believed them. That was my mistake.&lt;br /&gt;&lt;br /&gt;There isn’t anyone else in the world like me.&lt;br /&gt;&lt;br /&gt;I’m different. I’m an anomaly. I’m a monster. &lt;/i&gt;&lt;br /&gt;&lt;br /&gt;For two years, six months, fourteen days, eleven hours and sixteen minutes, Subject Six-Eight-Four — ‘Jane Doe’ — has been locked away and experimented on, without uttering a single word.&lt;br /&gt;&lt;br /&gt;As Jane’s resolve begins to crack under the influence of her new — and unexpectedly kind — evaluator, she uncovers the truth about Lengard’s mysterious ‘program’, discovering that her own secret is at the heart of a sinister plot … and one wrong move, one wrong &lt;i&gt;word&lt;/i&gt;, could change the world.&lt;br /&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '9857504'), ('name', 'Lynette Noni'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p5/9857504.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p2/9857504.jpg')])), ('link', 'https://www.goodreads.com/author/show/9857504.Lynette_Noni'), ('average_rating', '4.42'), ('ratings_count', '20384'), ('text_reviews_count', '3077')]))])), ('published', '2018'), ('work', OrderedDict([('id', '55019335'), ('uri', 'kca://work/amzn1.gr.work.v1.0eRTUABr60Wwho-zRykY5w')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38447')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '49547')])), ('uri', 'kca://book/amzn1.gr.book.v1.QYIb80P3mP0A4pXX0ucI6A'), ('title', "The Handmaid's Tale (The Handmaid's Tale, #1)"), ('title_without_series', "The Handmaid's Tale"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1578028274l/38447._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1578028274l/38447._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38447.The_Handmaid_s_Tale'), ('num_pages', '314'), ('format', 'Paperback'), ('edition_information', '1st Anchor Books edition'), ('publisher', 'Anchor Books'), ('publication_day', None), ('publication_year', '1998'), ('publication_month', '4'), ('average_rating', '4.11'), ('ratings_count', '1409201'), ('description', "Offred is a Handmaid in the Republic of Gilead. She may leave the home of the Commander and his wife once a day to walk to food markets whose signs are now pictures instead of words because women are no longer allowed to read. She must lie on her back once a month and pray that the Commander makes her pregnant, because in an age of declining births, Offred and the other Handmaids are valued only if their ovaries are viable. Offred can remember the years before, when she lived and made love with her husband, Luke; when she played with and protected her daughter; when she had a job, money of her own, and access to knowledge. But all of that is gone now . . . &lt;br /&gt;&lt;br /&gt;Funny, unexpected, horrifying, and altogether convincing, &lt;i&gt;The Handmaid's Tale&lt;/i&gt; is at once scathing satire, dire warning, and tour de force."), ('authors', OrderedDict([('author', OrderedDict([('id', '3472'), ('name', 'Margaret Atwood'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1282859073p5/3472.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1282859073p2/3472.jpg')])), ('link', 'https://www.goodreads.com/author/show/3472.Margaret_Atwood'), ('average_rating', '4.03'), ('ratings_count', '2668037'), ('text_reviews_count', '168844')]))])), ('published', '1998'), ('work', OrderedDict([('id', '1119185'), ('uri', 'kca://work/amzn1.gr.work.v1.C3iSrQ9DOvG8o6BBrFoi4w')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '170448')])), ('isbn', '0451526341'), ('isbn13', '9780451526342'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7565')])), ('uri', 'kca://book/amzn1.gr.book.v1.OPL1L19jvyFEvtyxeIp2CQ'), ('title', 'Animal Farm'), ('title_without_series', 'Animal Farm'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1325861570l/170448._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1325861570l/170448._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/170448.Animal_Farm'), ('num_pages', '141'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Signet Classics'), ('publication_day', None), ('publication_year', '1996'), ('publication_month', '4'), ('average_rating', '3.94'), ('ratings_count', '2662323'), ('description', '&lt;i&gt;Librarian\'s note: There is an Alternate Cover Edition for this edition of this book &lt;a href="https://www.goodreads.com/book/show/13456059-animal-farm" rel="nofollow"&gt;here&lt;/a&gt;.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;A farm is taken over by its overworked, mistreated animals. With flaming idealism and stirring slogans, they set out to create a paradise of progress, justice, and equality. Thus the stage is set for one of the most telling satiric fables ever penned –a razor-edged fairy tale for grown-ups that records the evolution from revolution against tyranny to a totalitarianism just as terrible. &lt;br /&gt;When &lt;i&gt;Animal Farm&lt;/i&gt; was first published, Stalinist Russia was seen as its target. Today it is devastatingly clear that wherever and whenever freedom is attacked, under whatever banner, the cutting clarity and savage comedy of George Orwell’s masterpiece have a meaning and message still ferociously fresh.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3706'), ('name', 'George Orwell'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p5/3706.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p2/3706.jpg')])), ('link', 'https://www.goodreads.com/author/show/3706.George_Orwell'), ('average_rating', '4.07'), ('ratings_count', '6098066'), ('text_reviews_count', '139352')]))])), ('published', '1996'), ('work', OrderedDict([('id', '2207778'), ('uri', 'kca://work/amzn1.gr.work.v1.V_MbIpN8vLdVjldwRz26LA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '36809135')])), ('isbn', '0735219117'), ('isbn13', '9780735219113'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '56795')])), ('uri', 'kca://book/amzn1.gr.book.v1.XegwBbc75MlndG3r2PFrQA'), ('title', 'Where the Crawdads Sing'), ('title_without_series', 'Where the Crawdads Sing'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582135294l/36809135._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582135294l/36809135._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/36809135-where-the-crawdads-sing'), ('num_pages', '384'), ('format', 'ebook'), ('edition_information', None), ('publisher', 'G.P. Putnam’s Sons'), ('publication_day', '14'), ('publication_year', '2018'), ('publication_month', '8'), ('average_rating', '4.48'), ('ratings_count', '836033'), ('description', 'For years, rumors of the “Marsh Girl” have haunted Barkley Cove, a quiet town on the North Carolina coast. So in late 1969, when handsome Chase Andrews is found dead, the locals immediately suspect Kya Clark, the so-called Marsh Girl. But Kya is not what they say. Sensitive and intelligent, she has survived for years alone in the marsh that she calls home, finding friends in the gulls and lessons in the sand. Then the time comes when she yearns to be touched and loved. When two young men from town become intrigued by her wild beauty, Kya opens herself to a new life–until the unthinkable happens.&lt;br /&gt;&lt;br /&gt;Perfect for fans of Barbara Kingsolver and Karen Russell, &lt;i&gt;Where the Crawdads Sing&lt;/i&gt; is at once an exquisite ode to the natural world, a heartbreaking coming-of-age story, and a surprising tale of possible murder. Owens reminds us that we are forever shaped by the children we once were, and that we are all subject to the beautiful and violent secrets that nature keeps.'), ('authors', OrderedDict([('author', OrderedDict([('id', '7043934'), ('name', 'Delia Owens'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1524665831p5/7043934.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1524665831p2/7043934.jpg')])), ('link', 'https://www.goodreads.com/author/show/7043934.Delia_Owens'), ('average_rating', '4.48'), ('ratings_count', '842214'), ('text_reviews_count', '78155')]))])), ('published', '2018'), ('work', OrderedDict([('id', '58589364'), ('uri', 'kca://work/amzn1.gr.work.v1.7--0S3qHZWgptVnUuIyAsg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '4671')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '52995')])), ('uri', 'kca://book/amzn1.gr.book.v1.Rka-Q5n8mdEE6GzuIQRElQ'), ('title', 'The Great Gatsby'), ('title_without_series', 'The Great Gatsby'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1490528560l/4671._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1490528560l/4671._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/4671.The_Great_Gatsby'), ('num_pages', '200'), ('format', 'Paperback'), ('edition_information', 'US / CAN'), ('publisher', 'Scribner'), ('publication_day', None), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '3.92'), ('ratings_count', '3686713'), ('description', 'Alternate Cover Edition ISBN: 0743273567 (ISBN13: &lt;a href="https://www.goodreads.com/book/show/41733839-the-great-gatsby" rel="nofollow"&gt;9780743273565&lt;/a&gt;)&lt;br /&gt;&lt;br /&gt;The Great Gatsby, F. Scott Fitzgerald\'s third book, stands as the supreme achievement of his career. This exemplary novel of the Jazz Age has been acclaimed by generations of readers. The story is of the fabulously wealthy Jay Gatsby and his new love for the beautiful Daisy Buchanan, of lavish parties on Long Island at a time when The New York Times noted "gin was the national drink and sex the national obsession," it is an exquisitely crafted tale of America in the 1920s.&lt;br /&gt;&lt;br /&gt;The Great Gatsby is one of the great classics of twentieth-century literature.&lt;br /&gt;(back cover)'), ('authors', OrderedDict([('author', OrderedDict([('id', '3190'), ('name', 'F. Scott Fitzgerald'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517864008p5/3190.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517864008p2/3190.jpg')])), ('link', 'https://www.goodreads.com/author/show/3190.F_Scott_Fitzgerald'), ('average_rating', '3.91'), ('ratings_count', '4051325'), ('text_reviews_count', '87853')]))])), ('published', '2004'), ('work', OrderedDict([('id', '245494'), ('uri', 'kca://work/amzn1.gr.work.v1.56BQMsZ2-7G__6NkMx9vWg')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40961427')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9062')])), ('uri', 'kca://book/amzn1.gr.book.v1.zhUOQmSWRGKlQ7eRG3QkRw'), ('title', '1984'), ('title_without_series', '1984'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532714506l/40961427._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532714506l/40961427._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40961427-1984'), ('num_pages', '237'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Houghton Mifflin Harcourt'), ('publication_day', '3'), ('publication_year', '2013'), ('publication_month', '9'), ('average_rating', '4.18'), ('ratings_count', '3036407'), ('description', "Among the seminal texts of the 20th century, &lt;i&gt;Nineteen Eighty-Four&lt;/i&gt; is a rare work that grows more haunting as its futuristic purgatory becomes more real. Published in 1949, the book offers political satirist George Orwell's nightmarish vision of a totalitarian, bureaucratic world and one poor stiff's attempt to find individuality. The brilliance of the novel is Orwell's prescience of modern life—the ubiquity of television, the distortion of the language—and his ability to construct such a thorough version of hell. Required reading for students since it was published, it ranks among the most terrifying novels ever written."), ('authors', OrderedDict([('author', OrderedDict([('id', '3706'), ('name', 'George Orwell'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p5/3706.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p2/3706.jpg')])), ('link', 'https://www.goodreads.com/author/show/3706.George_Orwell'), ('average_rating', '4.07'), ('ratings_count', '6098066'), ('text_reviews_count', '139352')]))])), ('published', '2013'), ('work', OrderedDict([('id', '153313'), ('uri', 'kca://work/amzn1.gr.work.v1.SgJQSc4-cyFNY1JLB6R9mA')]))])</t>
-  </si>
-  <si>
-    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2657')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '70920')])), ('uri', 'kca://book/amzn1.gr.book.v1.n0CD0ECMpxCldCqzG72KSQ'), ('title', 'To Kill a Mockingbird'), ('title_without_series', 'To Kill a Mockingbird'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1553383690l/2657._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1553383690l/2657._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2657.To_Kill_a_Mockingbird'), ('num_pages', '324'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harper Perennial Modern Classics'), ('publication_day', '23'), ('publication_year', '2006'), ('publication_month', '5'), ('average_rating', '4.28'), ('ratings_count', '4388278'), ('description', 'The unforgettable novel of a childhood in a sleepy Southern town and the crisis of conscience that rocked it, To Kill A Mockingbird became both an instant bestseller and a critical success when it was first published in 1960. It went on to win the Pulitzer Prize in 1961 and was later made into an Academy Award-winning film, also a classic.&lt;br /&gt;&lt;br /&gt;Compassionate, dramatic, and deeply moving, To Kill A Mockingbird takes readers to the roots of human behavior - to innocence and experience, kindness and cruelty, love and hatred, humor and pathos. Now with over 18 million copies in print and translated into forty languages, this regional story by a young Alabama woman claims universal appeal. Harper Lee always considered her book to be a simple love story. Today it is regarded as a masterpiece of American literature.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1825'), ('name', 'Harper Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1593873322p5/1825.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1593873322p2/1825.jpg')])), ('link', 'https://www.goodreads.com/author/show/1825.Harper_Lee'), ('average_rating', '4.23'), ('ratings_count', '4629544'), ('text_reviews_count', '119332')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3275794'), ('uri', 'kca://work/amzn1.gr.work.v1.bBuiCknnVtCo2qKc86WVjw')]))])</t>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '28634049')])), ('isbn', '1616892552'), ('isbn13', '9781616892555'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '3')])), ('uri', 'kca://book/amzn1.gr.book.v1.X2LWiajTXoUtWYV1S5zXrw'), ('title', 'Manual of Section'), ('title_without_series', 'Manual of Section'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1465687065l/28634049._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1465687065l/28634049._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/28634049-manual-of-section'), ('num_pages', '208'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Princeton Architectural Press'), ('publication_day', '23'), ('publication_year', '2016'), ('publication_month', '8'), ('average_rating', '4.43'), ('ratings_count', '56'), ('description', '&lt;b&gt;"It has been a while since I devoured a book on architecture with as much pleasure. I love a good section and I love this book."—Aaron Betsky, &lt;i&gt;Architect Magazine&lt;/i&gt;&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Award-winning architects Paul Lewis, Marc Tsurumaki, and David J. Lewis\'s essential guide to section.&lt;/b&gt; Section, along with plan and elevation, is one of the most important representational techniques of architectural design. &lt;i&gt;Manual of Section&lt;/i&gt; is the first book to provide a framework to describe and evaluate this fundamental design process in architecture.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Divided into seven categories of section based on extensive archival research:&lt;/b&gt;&lt;br /&gt;• Range is from simple one-story buildings to complex structures&lt;br /&gt;• Features stacked forms, fantastical shapes, internal holes, inclines, sheared planes, nested forms, or combinations of each&lt;br /&gt;• Includes sixty-three intricately detailed cross-section perspective drawings of many of the most significant structures in international architecture from the last one hundred years&lt;br /&gt;&lt;br /&gt;&lt;b&gt;"A must-read for all designers associated with the built environment and should surely be on the library shelves of every architecture, urban design and interior design school...the intricate drawings provided by LTL are sure to inspire all those who have the privilege of cracking the spine of this amazing reference." —&lt;i&gt;Spacing&lt;/i&gt;&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;In addition to the incredible cross-section drawings, the book includes smart and accessible essays on the history and uses of section.&lt;br /&gt;&lt;br /&gt;&lt;i&gt;Manual of Section&lt;/i&gt; has become a top architecture book for architecture students and professional architects.'), ('authors', OrderedDict([('author', OrderedDict([('id', '61932'), ('name', 'Paul Lewis'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_200x266-e183445fd1a1b5cc7075bb1cf7043306.png')])), ('small_image_url', OrderedDict([('@nophoto', 'true'), ('#text', 'https://s.gr-assets.com/assets/nophoto/user/u_50x66-632230dc9882b4352d753eedf9396530.png')])), ('link', 'https://www.goodreads.com/author/show/61932.Paul_Lewis'), ('average_rating', '4.02'), ('ratings_count', '823'), ('text_reviews_count', '78')]))])), ('published', '2016'), ('work', OrderedDict([('id', '48812456'), ('uri', 'kca://work/amzn1.gr.work.v1.2rO6tUoI3SdGAGHVn67IMA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '80660')])), ('isbn', '006112429X'), ('isbn13', '9780061124297'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '11141')])), ('uri', 'kca://book/amzn1.gr.book.v1.XVzibBbNBoaCNgEiJRWt9g'), ('title', 'We Need to Talk About Kevin'), ('title_without_series', 'We Need to Talk About Kevin'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327865017l/80660._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1327865017l/80660._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/80660.We_Need_to_Talk_About_Kevin'), ('num_pages', '400'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harper Perennial'), ('publication_day', '3'), ('publication_year', '2006'), ('publication_month', '7'), ('average_rating', '4.05'), ('ratings_count', '158092'), ('description', "&lt;p&gt; The gripping international bestseller about motherhood gone awry.&lt;/p&gt;&lt;p&gt;Eva never really wanted to be a mother - and certainly not the mother of the unlovable boy who murdered seven of his fellow high school students, a cafeteria worker, and a much-adored teacher who tried to befriend him, all two days before his sixteenth birthday. Now, two years later, it is time for her to come to terms with marriage, career, family, parenthood, and Kevin's horrific rampage in a series of startlingly direct correspondences with her estranged husband, Franklin. Uneasy with the sacrifices and social demotion of motherhood from the start, Eva fears that her alarming dislike for her own son may be responsible for driving him so nihilistically off the rails. &lt;/p&gt;&lt;p&gt;&lt;/p&gt;"), ('authors', OrderedDict([('author', OrderedDict([('id', '45922'), ('name', 'Lionel Shriver'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1332800238p5/45922.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1332800238p2/45922.jpg')])), ('link', 'https://www.goodreads.com/author/show/45922.Lionel_Shriver'), ('average_rating', '3.91'), ('ratings_count', '220627'), ('text_reviews_count', '23232')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3106720'), ('uri', 'kca://work/amzn1.gr.work.v1.xLpjOSFP7LDX8cIvigjctg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '32617610')])), ('isbn', '1473212782'), ('isbn13', '9781473212787'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '752')])), ('uri', 'kca://book/amzn1.gr.book.v1.EoFIbWdTfov5TrDj9-sIsg'), ('title', 'Sea of Rust'), ('title_without_series', 'Sea of Rust'), ('image_url', 'https://s.gr-assets.com/assets/nophoto/book/111x148-bcc042a9c91a29c1d680899eff700a03.png'), ('small_image_url', 'https://s.gr-assets.com/assets/nophoto/book/50x75-a91bf249278a81aabab721ef782c4a74.png'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/32617610-sea-of-rust'), ('num_pages', '365'), ('format', None), ('edition_information', None), ('publisher', None), ('publication_day', None), ('publication_year', None), ('publication_month', None), ('average_rating', '4.08'), ('ratings_count', '7386'), ('description', "One robot's search for meaning in a world where every human is long gone. &lt;br /&gt;&lt;br /&gt;A touching story of a search one robot's search for the answers in a world where every human is dead. &lt;br /&gt;&lt;br /&gt;It is thirty years since the humans lost their war with the artificial intelligences that were once their slaves. Not one human remains. But as the dust settled from our extinction there was no easy peace between the robots that survived. Instead, the two massively powerful artificially intelligent supercomputers that led them to victory now vie for control of the bots that remain, assimilating them into enormous networks called One World Intelligences (OWIs), absorbing their memories and turning them into mere extensions of the whole. Now the remaining freebots wander wastelands that were once warzones, picking the carcasses of the lost for the precious dwindling supply of parts they need to survive. &lt;br /&gt;&lt;br /&gt;BRITTLE started out his life playing nurse to a dying man, purchased in truth instead to look after the man's widow upon his death. But then war came and Brittle was forced to choose between the woman he swore to protect and potential oblivion at the hands of rising anti-AI sentiment. Thirty years later, his choice still haunts him. Now he spends his days in the harshest of the wastelands, known as the Sea of Rust, cannibalizing the walking dead - robots only hours away from total shutdown - looking for parts to trade for those he needs to keep going."), ('authors', OrderedDict([('author', OrderedDict([('id', '3969859'), ('name', 'C. Robert Cargill'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353882150p5/3969859.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1353882150p2/3969859.jpg')])), ('link', 'https://www.goodreads.com/author/show/3969859.C_Robert_Cargill'), ('average_rating', '3.90'), ('ratings_count', '14762'), ('text_reviews_count', '2197')]))])), ('published', None), ('work', OrderedDict([('id', '53204799'), ('uri', 'kca://work/amzn1.gr.work.v1.Zx5ELRvYlVOpE4rBne88Yg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38649806')])), ('isbn', '0525534326'), ('isbn13', '9780525534327'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '747')])), ('uri', 'kca://book/amzn1.gr.book.v1.H7ebuEcy5XpuAlKh9eipBA'), ('title', 'Little'), ('title_without_series', 'Little'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1523724459l/38649806._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1523724459l/38649806._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38649806-little'), ('num_pages', '448'), ('format', 'Hardcover'), ('edition_information', None), ('publisher', 'Riverhead Books'), ('publication_day', '23'), ('publication_year', '2018'), ('publication_month', '10'), ('average_rating', '4.00'), ('ratings_count', '5829'), ('description', "The wry, macabre, unforgettable tale of an ambitious orphan in Revolutionary Paris, befriended by royalty and radicals, who transforms herself into the legendary Madame Tussaud.&lt;br /&gt;&lt;br /&gt;In 1761, a tiny, odd-looking girl named Marie is born in a village in Switzerland. After the death of her parents, she is apprenticed to an eccentric wax sculptor and whisked off to the seamy streets of Paris, where they meet a domineering widow and her quiet, pale son. Together, they convert an abandoned monkey house into an exhibition hall for wax heads, and the spectacle becomes a sensation. As word of her artistic talent spreads, Marie is called to Versailles, where she tutors a princess and saves Marie Antoinette in childbirth. But outside the palace walls, Paris is roiling: The revolutionary mob is demanding heads, and... at the wax museum, heads are what they do.&lt;br /&gt;&lt;br /&gt;In the tradition of Gregory Maguire's Wicked and Erin Morgenstern's &lt;i&gt;The Night Circus&lt;/i&gt;, Edward Carey's &lt;i&gt;Little&lt;/i&gt; is a darkly endearing cavalcade of a novel—a story of art, class, determination, and how we hold on to what we love."), ('authors', OrderedDict([('author', OrderedDict([('id', '161399'), ('name', 'Edward Carey'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1388256263p5/161399.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1388256263p2/161399.jpg')])), ('link', 'https://www.goodreads.com/author/show/161399.Edward_Carey'), ('average_rating', '3.89'), ('ratings_count', '11636'), ('text_reviews_count', '1861')]))])), ('published', '2018'), ('work', OrderedDict([('id', '60261099'), ('uri', 'kca://work/amzn1.gr.work.v1.k2B71vWE7GVBP6FRngMwhw')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '9361589')])), ('isbn', '0385534639'), ('isbn13', '9780385534635'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '57951')])), ('uri', 'kca://book/amzn1.gr.book.v1.tPpWGC7kuUxtvkvPBpeniA'), ('title', 'The Night Circus'), ('title_without_series', 'The Night Circus'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1387124618l/9361589._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1387124618l/9361589._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/9361589-the-night-circus'), ('num_pages', '391'), ('format', 'Hardcover'), ('edition_information', 'First Edition'), ('publisher', 'Doubleday'), ('publication_day', '13'), ('publication_year', '2011'), ('publication_month', '9'), ('average_rating', '4.04'), ('ratings_count', '664398'), ('description', 'The circus arrives without warning. No announcements precede it. It is simply there, when yesterday it was not. Within the black-and-white striped canvas tents is an utterly unique experience full of breathtaking amazements. It is called Le Cirque des Rêves, and it is only open at night. &lt;br /&gt;&lt;br /&gt;But behind the scenes, a fierce competition is underway—a duel between two young magicians, Celia and Marco, who have been trained since childhood expressly for this purpose by their mercurial instructors. Unbeknownst to them, this is a game in which only one can be left standing, and the circus is but the stage for a remarkable battle of imagination and will. Despite themselves, however, Celia and Marco tumble headfirst into love—a deep, magical love that makes the lights flicker and the room grow warm whenever they so much as brush hands. &lt;br /&gt;&lt;br /&gt;True love or not, the game must play out, and the fates of everyone involved, from the cast of extraordinary circus performers to the patrons, hang in the balance, suspended as precariously as the daring acrobats overhead. &lt;br /&gt;&lt;br /&gt;Written in rich, seductive prose, this spell-casting novel is a feast for the senses and the heart.'), ('authors', OrderedDict([('author', OrderedDict([('id', '4370565'), ('name', 'Erin Morgenstern'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1552589582p5/4370565.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1552589582p2/4370565.jpg')])), ('link', 'https://www.goodreads.com/author/show/4370565.Erin_Morgenstern'), ('average_rating', '4.02'), ('ratings_count', '740497'), ('text_reviews_count', '88166')]))])), ('published', '2011'), ('work', OrderedDict([('id', '14245059'), ('uri', 'kca://work/amzn1.gr.work.v1.IzoeETdoCBWf_cxRZU_R_Q')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '34051011')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9570')])), ('uri', 'kca://book/amzn1.gr.book.v1.ko9fgGm97_zjs4OlOuIZSw'), ('title', 'Pachinko'), ('title_without_series', 'Pachinko'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1529845599l/34051011._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1529845599l/34051011._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/34051011-pachinko'), ('num_pages', '496'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Grand Central Publishing'), ('publication_day', '7'), ('publication_year', '2017'), ('publication_month', '2'), ('average_rating', '4.27'), ('ratings_count', '192983'), ('description', "In the early 1900s, teenaged Sunja, the adored daughter of a crippled fisherman, falls for a wealthy stranger at the seashore near her home in Korea. He promises her the world, but when she discovers she is pregnant--and that her lover is married--she refuses to be bought. Instead, she accepts an offer of marriage from a gentle, sickly minister passing through on his way to Japan. But her decision to abandon her home, and to reject her son's powerful father, sets off a dramatic saga that will echo down through the generations.&lt;br /&gt;&lt;br /&gt;Richly told and profoundly moving, Pachinko is a story of love, sacrifice, ambition, and loyalty. From bustling street markets to the halls of Japan's finest universities to the pachinko parlors of the criminal underworld, Lee's complex and passionate characters--strong, stubborn women, devoted sisters and sons, fathers shaken by moral crisis--survive and thrive against the indifferent arc of history."), ('authors', OrderedDict([('author', OrderedDict([('id', '378209'), ('name', 'Min Jin Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192651627p5/378209.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1192651627p2/378209.jpg')])), ('link', 'https://www.goodreads.com/author/show/378209.Min_Jin_Lee'), ('average_rating', '4.23'), ('ratings_count', '207248'), ('text_reviews_count', '21453')]))])), ('published', '2017'), ('work', OrderedDict([('id', '50384116'), ('uri', 'kca://work/amzn1.gr.work.v1.Kfq1uC_3eoSK1b271iNVKQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '18143977')])), ('isbn', '1476746583'), ('isbn13', '9781476746586'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '65336')])), ('uri', 'kca://book/amzn1.gr.book.v1.0IooOCfVIQPcIMOpfSRpYA'), ('title', 'All the Light We Cannot See'), ('title_without_series', 'All the Light We Cannot See'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1451445646l/18143977._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1451445646l/18143977._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/18143977-all-the-light-we-cannot-see'), ('num_pages', '531'), ('format', 'Hardcover'), ('edition_information', 'First Scribner hardcover edition May 2014'), ('publisher', 'Scribner'), ('publication_day', '6'), ('publication_year', '2014'), ('publication_month', '5'), ('average_rating', '4.33'), ('ratings_count', '992300'), ('description', '&lt;i&gt;An alternate cover for this ISBN can be found &lt;a href="https://www.goodreads.com/book/show/25210408-all-the-light-we-cannot-see" rel="nofollow"&gt;here&lt;/a&gt;&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;From the highly acclaimed, multiple award-winning Anthony Doerr, the stunningly beautiful instant &lt;i&gt;New York Times&lt;/i&gt; bestseller about a blind French girl and a German boy whose paths collide in occupied France as both try to survive the devastation of World War II.&lt;br /&gt;&lt;br /&gt;Marie-Laure lives in Paris near the Museum of Natural History, where her father works. When she is twelve, the Nazis occupy Paris and father and daughter flee to the walled citadel of Saint-Malo, where Marie-Laure’s reclusive great uncle lives in a tall house by the sea. With them they carry what might be the museum’s most valuable and dangerous jewel.&lt;br /&gt;&lt;br /&gt;In a mining town in Germany, Werner Pfennig, an orphan, grows up with his younger sister, enchanted by a crude radio they find that brings them news and stories from places they have never seen or imagined. Werner becomes an expert at building and fixing these crucial new instruments and is enlisted to use his talent to track down the resistance. Deftly interweaving the lives of Marie-Laure and Werner, Doerr illuminates the ways, against all odds, people try to be good to one another.'), ('authors', OrderedDict([('author', OrderedDict([('id', '28186'), ('name', 'Anthony Doerr'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1417812584p5/28186.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1417812584p2/28186.jpg')])), ('link', 'https://www.goodreads.com/author/show/28186.Anthony_Doerr'), ('average_rating', '4.31'), ('ratings_count', '1032893'), ('text_reviews_count', '79891')]))])), ('published', '2014'), ('work', OrderedDict([('id', '25491300'), ('uri', 'kca://work/amzn1.gr.work.v1.RE5swba2G5t7ZuQ6dNCGEQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '45880884')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', '9780648571599'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '169')])), ('uri', 'kca://book/amzn1.gr.book.v1.spE8a2-R6_O3udPVNsG56w'), ('title', 'Weapon (Whisper, #2)'), ('title_without_series', 'Weapon'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558412659l/45880884._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1558412659l/45880884._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/45880884-weapon'), ('num_pages', '407'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Pantera Press'), ('publication_day', '4'), ('publication_year', '2019'), ('publication_month', '11'), ('average_rating', '4.35'), ('ratings_count', '1255'), ('description', "The #1 bestselling WHISPER series concludes with WEAPON:&lt;br /&gt;&lt;br /&gt;&lt;i&gt;I already knew he was a psychopath. But now?&lt;br /&gt;He's more dangerous than ever.&lt;br /&gt;And I have less than twenty-four hours to stop him.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;After escaping Lengard and finding sanctuary with the Remnants, Alyssa Scott is desperate to save those she left behind ─ and the rest of the world ─ from the power-hungry scientist, Kendall Vanik. But secrets and lies block her at every turn, and soon Lyss is left questioning everything she has ever believed.&lt;br /&gt;&lt;br /&gt;When long-lost memories begin to surface and the mysteries of her past continue to grow, Lyss battles to retain her hard-won control. Allies become enemies and enemies become allies, leaving her certain about only two things: when it comes to Speakers, nothing is ever as it seems... and the only person she can trust is herself."), ('authors', OrderedDict([('author', OrderedDict([('id', '9857504'), ('name', 'Lynette Noni'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p5/9857504.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p2/9857504.jpg')])), ('link', 'https://www.goodreads.com/author/show/9857504.Lynette_Noni'), ('average_rating', '4.43'), ('ratings_count', '20816'), ('text_reviews_count', '3127')]))])), ('published', '2019'), ('work', OrderedDict([('id', '70706086'), ('uri', 'kca://work/amzn1.gr.work.v1.HcfdpNe0pZXUjdb2-YRgyQ')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '34020950')])), ('isbn', '1525300415'), ('isbn13', '9781525300417'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '510')])), ('uri', 'kca://book/amzn1.gr.book.v1.PNYh92pz7gDLM6qrgJMH6A'), ('title', 'Whisper (Whisper, #1)'), ('title_without_series', 'Whisper'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1504853373l/34020950._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1504853373l/34020950._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/34020950-whisper'), ('num_pages', '320'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'KCP Loft'), ('publication_day', '1'), ('publication_year', '2018'), ('publication_month', '5'), ('average_rating', '4.27'), ('ratings_count', '3949'), ('description', '&lt;i&gt;“Lengard is a secret government facility for extraordinary people,” they told me. &lt;br /&gt;&lt;br /&gt;I believed them. That was my mistake.&lt;br /&gt;&lt;br /&gt;There isn’t anyone else in the world like me.&lt;br /&gt;&lt;br /&gt;I’m different. I’m an anomaly. I’m a monster. &lt;/i&gt;&lt;br /&gt;&lt;br /&gt;For two years, six months, fourteen days, eleven hours and sixteen minutes, Subject Six-Eight-Four — ‘Jane Doe’ — has been locked away and experimented on, without uttering a single word.&lt;br /&gt;&lt;br /&gt;As Jane’s resolve begins to crack under the influence of her new — and unexpectedly kind — evaluator, she uncovers the truth about Lengard’s mysterious ‘program’, discovering that her own secret is at the heart of a sinister plot … and one wrong move, one wrong &lt;i&gt;word&lt;/i&gt;, could change the world.&lt;br /&gt;'), ('authors', OrderedDict([('author', OrderedDict([('id', '9857504'), ('name', 'Lynette Noni'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p5/9857504.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1540204020p2/9857504.jpg')])), ('link', 'https://www.goodreads.com/author/show/9857504.Lynette_Noni'), ('average_rating', '4.43'), ('ratings_count', '20816'), ('text_reviews_count', '3127')]))])), ('published', '2018'), ('work', OrderedDict([('id', '55019335'), ('uri', 'kca://work/amzn1.gr.work.v1.0eRTUABr60Wwho-zRykY5w')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '38447')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '49848')])), ('uri', 'kca://book/amzn1.gr.book.v1.QYIb80P3mP0A4pXX0ucI6A'), ('title', "The Handmaid's Tale (The Handmaid's Tale, #1)"), ('title_without_series', "The Handmaid's Tale"), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1578028274l/38447._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1578028274l/38447._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/38447.The_Handmaid_s_Tale'), ('num_pages', '314'), ('format', 'Paperback'), ('edition_information', '1st Anchor Books edition'), ('publisher', 'Anchor Books'), ('publication_day', None), ('publication_year', '1998'), ('publication_month', '4'), ('average_rating', '4.11'), ('ratings_count', '1420566'), ('description', "Offred is a Handmaid in the Republic of Gilead. She may leave the home of the Commander and his wife once a day to walk to food markets whose signs are now pictures instead of words because women are no longer allowed to read. She must lie on her back once a month and pray that the Commander makes her pregnant, because in an age of declining births, Offred and the other Handmaids are valued only if their ovaries are viable. Offred can remember the years before, when she lived and made love with her husband, Luke; when she played with and protected her daughter; when she had a job, money of her own, and access to knowledge. But all of that is gone now . . . &lt;br /&gt;&lt;br /&gt;Funny, unexpected, horrifying, and altogether convincing, &lt;i&gt;The Handmaid's Tale&lt;/i&gt; is at once scathing satire, dire warning, and tour de force."), ('authors', OrderedDict([('author', OrderedDict([('id', '3472'), ('name', 'Margaret Atwood'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1282859073p5/3472.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1282859073p2/3472.jpg')])), ('link', 'https://www.goodreads.com/author/show/3472.Margaret_Atwood'), ('average_rating', '4.03'), ('ratings_count', '2692179'), ('text_reviews_count', '170205')]))])), ('published', '1998'), ('work', OrderedDict([('id', '1119185'), ('uri', 'kca://work/amzn1.gr.work.v1.C3iSrQ9DOvG8o6BBrFoi4w')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '170448')])), ('isbn', '0451526341'), ('isbn13', '9780451526342'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '7820')])), ('uri', 'kca://book/amzn1.gr.book.v1.OPL1L19jvyFEvtyxeIp2CQ'), ('title', 'Animal Farm'), ('title_without_series', 'Animal Farm'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1325861570l/170448._SY160_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1325861570l/170448._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/170448.Animal_Farm'), ('num_pages', '141'), ('format', 'Mass Market Paperback'), ('edition_information', None), ('publisher', 'Signet Classics'), ('publication_day', None), ('publication_year', '1996'), ('publication_month', '4'), ('average_rating', '3.94'), ('ratings_count', '2679434'), ('description', '&lt;i&gt;Librarian\'s note: There is an Alternate Cover Edition for this edition of this book &lt;a href="https://www.goodreads.com/book/show/13456059-animal-farm" rel="nofollow"&gt;here&lt;/a&gt;.&lt;/i&gt;&lt;br /&gt;&lt;br /&gt;A farm is taken over by its overworked, mistreated animals. With flaming idealism and stirring slogans, they set out to create a paradise of progress, justice, and equality. Thus the stage is set for one of the most telling satiric fables ever penned –a razor-edged fairy tale for grown-ups that records the evolution from revolution against tyranny to a totalitarianism just as terrible. &lt;br /&gt;When &lt;i&gt;Animal Farm&lt;/i&gt; was first published, Stalinist Russia was seen as its target. Today it is devastatingly clear that wherever and whenever freedom is attacked, under whatever banner, the cutting clarity and savage comedy of George Orwell’s masterpiece have a meaning and message still ferociously fresh.'), ('authors', OrderedDict([('author', OrderedDict([('id', '3706'), ('name', 'George Orwell'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p5/3706.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p2/3706.jpg')])), ('link', 'https://www.goodreads.com/author/show/3706.George_Orwell'), ('average_rating', '4.08'), ('ratings_count', '6149627'), ('text_reviews_count', '140651')]))])), ('published', '1996'), ('work', OrderedDict([('id', '2207778'), ('uri', 'kca://work/amzn1.gr.work.v1.V_MbIpN8vLdVjldwRz26LA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '36809135')])), ('isbn', '0735219117'), ('isbn13', '9780735219113'), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '58552')])), ('uri', 'kca://book/amzn1.gr.book.v1.XegwBbc75MlndG3r2PFrQA'), ('title', 'Where the Crawdads Sing'), ('title_without_series', 'Where the Crawdads Sing'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582135294l/36809135._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1582135294l/36809135._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/36809135-where-the-crawdads-sing'), ('num_pages', '384'), ('format', 'ebook'), ('edition_information', None), ('publisher', 'G.P. Putnam’s Sons'), ('publication_day', '14'), ('publication_year', '2018'), ('publication_month', '8'), ('average_rating', '4.48'), ('ratings_count', '868575'), ('description', 'For years, rumors of the “Marsh Girl” have haunted Barkley Cove, a quiet town on the North Carolina coast. So in late 1969, when handsome Chase Andrews is found dead, the locals immediately suspect Kya Clark, the so-called Marsh Girl. But Kya is not what they say. Sensitive and intelligent, she has survived for years alone in the marsh that she calls home, finding friends in the gulls and lessons in the sand. Then the time comes when she yearns to be touched and loved. When two young men from town become intrigued by her wild beauty, Kya opens herself to a new life–until the unthinkable happens.&lt;br /&gt;&lt;br /&gt;Perfect for fans of Barbara Kingsolver and Karen Russell, &lt;i&gt;Where the Crawdads Sing&lt;/i&gt; is at once an exquisite ode to the natural world, a heartbreaking coming-of-age story, and a surprising tale of possible murder. Owens reminds us that we are forever shaped by the children we once were, and that we are all subject to the beautiful and violent secrets that nature keeps.'), ('authors', OrderedDict([('author', OrderedDict([('id', '7043934'), ('name', 'Delia Owens'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1524665831p5/7043934.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1524665831p2/7043934.jpg')])), ('link', 'https://www.goodreads.com/author/show/7043934.Delia_Owens'), ('average_rating', '4.48'), ('ratings_count', '874824'), ('text_reviews_count', '80567')]))])), ('published', '2018'), ('work', OrderedDict([('id', '58589364'), ('uri', 'kca://work/amzn1.gr.work.v1.7--0S3qHZWgptVnUuIyAsg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '4671')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '53251')])), ('uri', 'kca://book/amzn1.gr.book.v1.Rka-Q5n8mdEE6GzuIQRElQ'), ('title', 'The Great Gatsby'), ('title_without_series', 'The Great Gatsby'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1490528560l/4671._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1490528560l/4671._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/4671.The_Great_Gatsby'), ('num_pages', '200'), ('format', 'Paperback'), ('edition_information', 'US / CAN'), ('publisher', 'Scribner'), ('publication_day', None), ('publication_year', '2004'), ('publication_month', '9'), ('average_rating', '3.92'), ('ratings_count', '3707091'), ('description', 'Alternate Cover Edition ISBN: 0743273567 (ISBN13: &lt;a href="https://www.goodreads.com/book/show/41733839-the-great-gatsby" rel="nofollow"&gt;9780743273565&lt;/a&gt;)&lt;br /&gt;&lt;br /&gt;The Great Gatsby, F. Scott Fitzgerald\'s third book, stands as the supreme achievement of his career. This exemplary novel of the Jazz Age has been acclaimed by generations of readers. The story is of the fabulously wealthy Jay Gatsby and his new love for the beautiful Daisy Buchanan, of lavish parties on Long Island at a time when The New York Times noted "gin was the national drink and sex the national obsession," it is an exquisitely crafted tale of America in the 1920s.&lt;br /&gt;&lt;br /&gt;The Great Gatsby is one of the great classics of twentieth-century literature.&lt;br /&gt;(back cover)'), ('authors', OrderedDict([('author', OrderedDict([('id', '3190'), ('name', 'F. Scott Fitzgerald'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517864008p5/3190.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1517864008p2/3190.jpg')])), ('link', 'https://www.goodreads.com/author/show/3190.F_Scott_Fitzgerald'), ('average_rating', '3.91'), ('ratings_count', '4073890'), ('text_reviews_count', '88402')]))])), ('published', '2004'), ('work', OrderedDict([('id', '245494'), ('uri', 'kca://work/amzn1.gr.work.v1.56BQMsZ2-7G__6NkMx9vWg')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '40961427')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '9478')])), ('uri', 'kca://book/amzn1.gr.book.v1.zhUOQmSWRGKlQ7eRG3QkRw'), ('title', '1984'), ('title_without_series', '1984'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532714506l/40961427._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1532714506l/40961427._SX50_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/40961427-1984'), ('num_pages', '237'), ('format', 'Kindle Edition'), ('edition_information', None), ('publisher', 'Houghton Mifflin Harcourt'), ('publication_day', '3'), ('publication_year', '2013'), ('publication_month', '9'), ('average_rating', '4.18'), ('ratings_count', '3059685'), ('description', "Among the seminal texts of the 20th century, &lt;i&gt;Nineteen Eighty-Four&lt;/i&gt; is a rare work that grows more haunting as its futuristic purgatory becomes more real. Published in 1949, the book offers political satirist George Orwell's nightmarish vision of a totalitarian, bureaucratic world and one poor stiff's attempt to find individuality. The brilliance of the novel is Orwell's prescience of modern life—the ubiquity of television, the distortion of the language—and his ability to construct such a thorough version of hell. Required reading for students since it was published, it ranks among the most terrifying novels ever written."), ('authors', OrderedDict([('author', OrderedDict([('id', '3706'), ('name', 'George Orwell'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p5/3706.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1588856560p2/3706.jpg')])), ('link', 'https://www.goodreads.com/author/show/3706.George_Orwell'), ('average_rating', '4.08'), ('ratings_count', '6149627'), ('text_reviews_count', '140651')]))])), ('published', '2013'), ('work', OrderedDict([('id', '153313'), ('uri', 'kca://work/amzn1.gr.work.v1.SgJQSc4-cyFNY1JLB6R9mA')]))])</t>
+  </si>
+  <si>
+    <t>OrderedDict([('id', OrderedDict([('@type', 'integer'), ('#text', '2657')])), ('isbn', OrderedDict([('@nil', 'true')])), ('isbn13', OrderedDict([('@nil', 'true')])), ('text_reviews_count', OrderedDict([('@type', 'integer'), ('#text', '71181')])), ('uri', 'kca://book/amzn1.gr.book.v1.n0CD0ECMpxCldCqzG72KSQ'), ('title', 'To Kill a Mockingbird'), ('title_without_series', 'To Kill a Mockingbird'), ('image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1553383690l/2657._SX98_.jpg'), ('small_image_url', 'https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1553383690l/2657._SY75_.jpg'), ('large_image_url', None), ('link', 'https://www.goodreads.com/book/show/2657.To_Kill_a_Mockingbird'), ('num_pages', '324'), ('format', 'Paperback'), ('edition_information', None), ('publisher', 'Harper Perennial Modern Classics'), ('publication_day', '23'), ('publication_year', '2006'), ('publication_month', '5'), ('average_rating', '4.28'), ('ratings_count', '4410322'), ('description', 'The unforgettable novel of a childhood in a sleepy Southern town and the crisis of conscience that rocked it, To Kill A Mockingbird became both an instant bestseller and a critical success when it was first published in 1960. It went on to win the Pulitzer Prize in 1961 and was later made into an Academy Award-winning film, also a classic.&lt;br /&gt;&lt;br /&gt;Compassionate, dramatic, and deeply moving, To Kill A Mockingbird takes readers to the roots of human behavior - to innocence and experience, kindness and cruelty, love and hatred, humor and pathos. Now with over 18 million copies in print and translated into forty languages, this regional story by a young Alabama woman claims universal appeal. Harper Lee always considered her book to be a simple love story. Today it is regarded as a masterpiece of American literature.'), ('authors', OrderedDict([('author', OrderedDict([('id', '1825'), ('name', 'Harper Lee'), ('role', None), ('image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1593873322p5/1825.jpg')])), ('small_image_url', OrderedDict([('@nophoto', 'false'), ('#text', 'https://images.gr-assets.com/authors/1593873322p2/1825.jpg')])), ('link', 'https://www.goodreads.com/author/show/1825.Harper_Lee'), ('average_rating', '4.23'), ('ratings_count', '4653285'), ('text_reviews_count', '119829')]))])), ('published', '2006'), ('work', OrderedDict([('id', '3275794'), ('uri', 'kca://work/amzn1.gr.work.v1.bBuiCknnVtCo2qKc86WVjw')]))])</t>
   </si>
   <si>
     <t>3</t>
@@ -2476,7 +2476,7 @@
     <t>Walker Books</t>
   </si>
   <si>
-    <t>Simon  Schuster Books for Young Readers</t>
+    <t>Simon Schuster Books for Young Readers</t>
   </si>
   <si>
     <t>Delacorte Press</t>
@@ -3248,10 +3248,10 @@
         <v>326</v>
       </c>
       <c r="N2" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O2" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P2" t="s">
         <v>238</v>
@@ -3310,10 +3310,10 @@
         <v>239</v>
       </c>
       <c r="N3" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O3" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P3" t="s">
         <v>239</v>
@@ -3372,10 +3372,10 @@
         <v>327</v>
       </c>
       <c r="N4" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O4" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P4" t="s">
         <v>240</v>
@@ -3434,10 +3434,10 @@
         <v>328</v>
       </c>
       <c r="N5" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O5" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P5" t="s">
         <v>241</v>
@@ -3496,10 +3496,10 @@
         <v>329</v>
       </c>
       <c r="N6" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O6" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P6" t="s">
         <v>242</v>
@@ -3558,10 +3558,10 @@
         <v>330</v>
       </c>
       <c r="N7" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O7" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P7" t="s">
         <v>243</v>
@@ -3688,10 +3688,10 @@
         <v>331</v>
       </c>
       <c r="N9" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O9" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P9" t="s">
         <v>244</v>
@@ -3750,10 +3750,10 @@
         <v>332</v>
       </c>
       <c r="N10" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O10" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P10" t="s">
         <v>245</v>
@@ -3812,10 +3812,10 @@
         <v>333</v>
       </c>
       <c r="N11" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O11" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P11" t="s">
         <v>246</v>
@@ -3874,10 +3874,10 @@
         <v>334</v>
       </c>
       <c r="N12" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O12" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P12" t="s">
         <v>247</v>
@@ -3936,10 +3936,10 @@
         <v>335</v>
       </c>
       <c r="N13" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O13" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P13" t="s">
         <v>248</v>
@@ -3998,10 +3998,10 @@
         <v>336</v>
       </c>
       <c r="N14" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O14" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P14" t="s">
         <v>249</v>
@@ -4060,10 +4060,10 @@
         <v>337</v>
       </c>
       <c r="N15" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O15" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P15" t="s">
         <v>250</v>
@@ -4122,10 +4122,10 @@
         <v>338</v>
       </c>
       <c r="N16" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O16" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P16" t="s">
         <v>251</v>
@@ -4184,10 +4184,10 @@
         <v>339</v>
       </c>
       <c r="N17" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O17" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P17" t="s">
         <v>252</v>
@@ -4246,10 +4246,10 @@
         <v>340</v>
       </c>
       <c r="N18" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O18" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P18" t="s">
         <v>253</v>
@@ -4308,10 +4308,10 @@
         <v>341</v>
       </c>
       <c r="N19" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O19" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P19" t="s">
         <v>254</v>
@@ -4370,10 +4370,10 @@
         <v>342</v>
       </c>
       <c r="N20" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O20" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P20" t="s">
         <v>255</v>
@@ -4432,10 +4432,10 @@
         <v>343</v>
       </c>
       <c r="N21" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O21" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P21" t="s">
         <v>256</v>
@@ -4494,10 +4494,10 @@
         <v>344</v>
       </c>
       <c r="N22" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O22" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P22" t="s">
         <v>257</v>
@@ -4556,10 +4556,10 @@
         <v>258</v>
       </c>
       <c r="N23" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O23" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P23" t="s">
         <v>258</v>
@@ -4618,10 +4618,10 @@
         <v>345</v>
       </c>
       <c r="N24" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O24" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P24" t="s">
         <v>259</v>
@@ -4680,10 +4680,10 @@
         <v>260</v>
       </c>
       <c r="N25" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O25" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P25" t="s">
         <v>260</v>
@@ -4742,10 +4742,10 @@
         <v>261</v>
       </c>
       <c r="N26" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O26" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P26" t="s">
         <v>261</v>
@@ -4804,10 +4804,10 @@
         <v>346</v>
       </c>
       <c r="N27" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O27" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P27" t="s">
         <v>262</v>
@@ -4866,10 +4866,10 @@
         <v>347</v>
       </c>
       <c r="N28" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O28" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P28" t="s">
         <v>263</v>
@@ -4928,10 +4928,10 @@
         <v>264</v>
       </c>
       <c r="N29" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O29" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P29" t="s">
         <v>264</v>
@@ -4990,10 +4990,10 @@
         <v>348</v>
       </c>
       <c r="N30" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O30" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P30" t="s">
         <v>265</v>
@@ -5052,10 +5052,10 @@
         <v>349</v>
       </c>
       <c r="N31" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O31" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P31" t="s">
         <v>266</v>
@@ -5114,10 +5114,10 @@
         <v>350</v>
       </c>
       <c r="N32" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O32" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P32" t="s">
         <v>267</v>
@@ -5176,10 +5176,10 @@
         <v>351</v>
       </c>
       <c r="N33" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O33" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P33" t="s">
         <v>268</v>
@@ -5238,10 +5238,10 @@
         <v>352</v>
       </c>
       <c r="N34" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O34" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P34" t="s">
         <v>269</v>
@@ -5300,10 +5300,10 @@
         <v>353</v>
       </c>
       <c r="N35" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O35" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P35" t="s">
         <v>270</v>
@@ -5362,10 +5362,10 @@
         <v>354</v>
       </c>
       <c r="N36" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O36" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P36" t="s">
         <v>271</v>
@@ -5424,10 +5424,10 @@
         <v>355</v>
       </c>
       <c r="N37" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O37" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P37" t="s">
         <v>272</v>
@@ -5486,10 +5486,10 @@
         <v>356</v>
       </c>
       <c r="N38" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O38" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P38" t="s">
         <v>273</v>
@@ -5548,10 +5548,10 @@
         <v>357</v>
       </c>
       <c r="N39" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O39" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P39" t="s">
         <v>274</v>
@@ -5610,10 +5610,10 @@
         <v>358</v>
       </c>
       <c r="N40" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O40" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P40" t="s">
         <v>275</v>
@@ -5672,10 +5672,10 @@
         <v>359</v>
       </c>
       <c r="N41" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O41" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P41" t="s">
         <v>276</v>
@@ -5734,10 +5734,10 @@
         <v>360</v>
       </c>
       <c r="N42" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O42" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P42" t="s">
         <v>277</v>
@@ -5796,10 +5796,10 @@
         <v>361</v>
       </c>
       <c r="N43" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O43" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P43" t="s">
         <v>278</v>
@@ -5858,10 +5858,10 @@
         <v>362</v>
       </c>
       <c r="N44" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O44" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P44" t="s">
         <v>279</v>
@@ -5920,10 +5920,10 @@
         <v>280</v>
       </c>
       <c r="N45" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O45" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P45" t="s">
         <v>280</v>
@@ -5982,10 +5982,10 @@
         <v>363</v>
       </c>
       <c r="N46" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O46" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P46" t="s">
         <v>281</v>
@@ -6041,10 +6041,10 @@
         <v>364</v>
       </c>
       <c r="N47" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O47" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P47" t="s">
         <v>282</v>
@@ -6103,10 +6103,10 @@
         <v>283</v>
       </c>
       <c r="N48" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O48" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P48" t="s">
         <v>283</v>
@@ -6165,10 +6165,10 @@
         <v>365</v>
       </c>
       <c r="N49" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O49" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P49" t="s">
         <v>284</v>
@@ -6227,10 +6227,10 @@
         <v>366</v>
       </c>
       <c r="N50" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O50" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P50" t="s">
         <v>285</v>
@@ -6289,10 +6289,10 @@
         <v>367</v>
       </c>
       <c r="N51" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O51" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P51" t="s">
         <v>286</v>
@@ -6351,10 +6351,10 @@
         <v>287</v>
       </c>
       <c r="N52" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O52" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P52" t="s">
         <v>287</v>
@@ -6413,10 +6413,10 @@
         <v>288</v>
       </c>
       <c r="N53" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O53" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P53" t="s">
         <v>288</v>
@@ -6475,10 +6475,10 @@
         <v>289</v>
       </c>
       <c r="N54" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O54" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P54" t="s">
         <v>289</v>
@@ -6537,10 +6537,10 @@
         <v>290</v>
       </c>
       <c r="N55" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O55" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P55" t="s">
         <v>290</v>
@@ -6599,10 +6599,10 @@
         <v>368</v>
       </c>
       <c r="N56" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O56" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P56" t="s">
         <v>291</v>
@@ -6661,10 +6661,10 @@
         <v>369</v>
       </c>
       <c r="N57" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O57" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P57" t="s">
         <v>292</v>
@@ -6723,10 +6723,10 @@
         <v>370</v>
       </c>
       <c r="N58" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O58" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P58" t="s">
         <v>293</v>
@@ -6853,10 +6853,10 @@
         <v>372</v>
       </c>
       <c r="N60" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O60" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P60" t="s">
         <v>295</v>
@@ -7459,10 +7459,10 @@
         <v>375</v>
       </c>
       <c r="N69" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O69" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P69" t="s">
         <v>303</v>
@@ -7521,10 +7521,10 @@
         <v>376</v>
       </c>
       <c r="N70" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O70" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P70" t="s">
         <v>304</v>
@@ -7651,10 +7651,10 @@
         <v>378</v>
       </c>
       <c r="N72" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O72" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P72" t="s">
         <v>306</v>
@@ -7713,10 +7713,10 @@
         <v>379</v>
       </c>
       <c r="N73" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O73" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P73" t="s">
         <v>307</v>
@@ -7908,10 +7908,10 @@
         <v>380</v>
       </c>
       <c r="N76" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O76" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P76" t="s">
         <v>310</v>
@@ -7970,10 +7970,10 @@
         <v>381</v>
       </c>
       <c r="N77" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O77" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P77" t="s">
         <v>311</v>
@@ -8032,10 +8032,10 @@
         <v>382</v>
       </c>
       <c r="N78" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O78" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P78" t="s">
         <v>312</v>
@@ -8094,10 +8094,10 @@
         <v>383</v>
       </c>
       <c r="N79" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O79" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P79" t="s">
         <v>313</v>
@@ -8150,10 +8150,10 @@
         <v>384</v>
       </c>
       <c r="N80" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O80" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P80" t="s">
         <v>314</v>
@@ -8280,10 +8280,10 @@
         <v>385</v>
       </c>
       <c r="N82" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O82" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P82" t="s">
         <v>316</v>
@@ -8342,10 +8342,10 @@
         <v>386</v>
       </c>
       <c r="N83" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O83" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P83" t="s">
         <v>317</v>
@@ -8472,10 +8472,10 @@
         <v>387</v>
       </c>
       <c r="N85" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O85" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P85" t="s">
         <v>319</v>
@@ -8534,10 +8534,10 @@
         <v>388</v>
       </c>
       <c r="N86" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O86" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P86" t="s">
         <v>320</v>
@@ -8596,10 +8596,10 @@
         <v>321</v>
       </c>
       <c r="N87" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O87" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P87" t="s">
         <v>321</v>
@@ -8726,10 +8726,10 @@
         <v>389</v>
       </c>
       <c r="N89" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O89" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P89" t="s">
         <v>323</v>
@@ -8788,10 +8788,10 @@
         <v>390</v>
       </c>
       <c r="N90" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O90" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P90" t="s">
         <v>324</v>
@@ -8850,10 +8850,10 @@
         <v>391</v>
       </c>
       <c r="N91" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="O91" s="3">
-        <v>43922</v>
+        <v>25569</v>
       </c>
       <c r="P91" t="s">
         <v>325</v>

</xml_diff>